<commit_message>
introduce initial data to be continued
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Defninition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Defninition.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafalkalita/dev/moj/ccd-api-test-automation-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/HMCTS/DEVLAB/WS/STS_HMCTS/CCD/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67ED300F-7ABE-5744-A736-A6DFCA7FAC34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238CCE87-AAF0-154E-927A-55B44C3C0806}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37300" yWindow="100" windowWidth="35220" windowHeight="18280" firstSheet="5" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4800" yWindow="-21140" windowWidth="38400" windowHeight="21140" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5432" uniqueCount="936">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5477" uniqueCount="942">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -2944,6 +2944,24 @@
   </si>
   <si>
     <t>Policy Case Assigned Role</t>
+  </si>
+  <si>
+    <t>DefaultValue</t>
+  </si>
+  <si>
+    <t>organisationForCaseRole1</t>
+  </si>
+  <si>
+    <t>organisationForCaseRole2</t>
+  </si>
+  <si>
+    <t>organisationForCaseRole3</t>
+  </si>
+  <si>
+    <t>setOrganisationsForCaseRoles</t>
+  </si>
+  <si>
+    <t>someOrganisation</t>
   </si>
 </sst>
 </file>
@@ -3351,7 +3369,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3416,6 +3434,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -3603,7 +3627,7 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="413">
+  <cellXfs count="419">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -4657,6 +4681,24 @@
     <xf numFmtId="1" fontId="48" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -4674,7 +4716,48 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Normal 2 3" xfId="13" xr:uid="{983C50BB-8B6C-1941-95CA-614B186AEA1E}"/>
   </cellStyles>
-  <dxfs count="302">
+  <dxfs count="303">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
@@ -11618,372 +11701,373 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1F077F35-774C-E743-83C7-6E310AAD8337}" name="Table5" displayName="Table5" ref="A3:E4" totalsRowShown="0" headerRowDxfId="301" dataDxfId="299" headerRowBorderDxfId="300" tableBorderDxfId="298" totalsRowBorderDxfId="297">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1F077F35-774C-E743-83C7-6E310AAD8337}" name="Table5" displayName="Table5" ref="A3:E4" totalsRowShown="0" headerRowDxfId="302" dataDxfId="300" headerRowBorderDxfId="301" tableBorderDxfId="299" totalsRowBorderDxfId="298">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{46ECD1A9-127E-3F45-96EF-07D1A76637A0}" name="LiveFrom" dataDxfId="296"/>
-    <tableColumn id="2" xr3:uid="{13DE718E-2141-6449-B408-2893D5F825EE}" name="LiveTo" dataDxfId="295"/>
-    <tableColumn id="3" xr3:uid="{2B218C4E-E8AE-9640-AF62-1EB51790A676}" name="ID" dataDxfId="294"/>
-    <tableColumn id="4" xr3:uid="{3EF730D3-305C-8E4D-ADBC-A778C1C17A83}" name="Name" dataDxfId="293"/>
-    <tableColumn id="5" xr3:uid="{EB212619-E76B-834D-9639-6E70EF2B808C}" name="Description" dataDxfId="292"/>
+    <tableColumn id="1" xr3:uid="{46ECD1A9-127E-3F45-96EF-07D1A76637A0}" name="LiveFrom" dataDxfId="297"/>
+    <tableColumn id="2" xr3:uid="{13DE718E-2141-6449-B408-2893D5F825EE}" name="LiveTo" dataDxfId="296"/>
+    <tableColumn id="3" xr3:uid="{2B218C4E-E8AE-9640-AF62-1EB51790A676}" name="ID" dataDxfId="295"/>
+    <tableColumn id="4" xr3:uid="{3EF730D3-305C-8E4D-ADBC-A778C1C17A83}" name="Name" dataDxfId="294"/>
+    <tableColumn id="5" xr3:uid="{EB212619-E76B-834D-9639-6E70EF2B808C}" name="Description" dataDxfId="293"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4CFBCA8A-9EC2-9242-9BDE-961374475E58}" name="Table9" displayName="Table9" ref="A3:H27" totalsRowShown="0" headerRowDxfId="170" dataDxfId="168" headerRowBorderDxfId="169" tableBorderDxfId="167" totalsRowBorderDxfId="166">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4CFBCA8A-9EC2-9242-9BDE-961374475E58}" name="Table9" displayName="Table9" ref="A3:H27" totalsRowShown="0" headerRowDxfId="171" dataDxfId="169" headerRowBorderDxfId="170" tableBorderDxfId="168" totalsRowBorderDxfId="167">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{3A9C2213-3C87-B242-A50F-DAA873031CFD}" name="LiveFrom" dataDxfId="165"/>
-    <tableColumn id="2" xr3:uid="{4438559D-2DCB-194A-BFAA-A68A1596F0EA}" name="LiveTo" dataDxfId="164"/>
-    <tableColumn id="3" xr3:uid="{20BC5FF0-EE97-BA41-80E0-333D8430A55D}" name="CaseTypeID" dataDxfId="163"/>
-    <tableColumn id="4" xr3:uid="{660AAD23-D344-7148-A6CD-579BFC3B0553}" name="ID" dataDxfId="162"/>
-    <tableColumn id="5" xr3:uid="{0D9AC729-9189-6841-A6A5-90D572AE955C}" name="Name" dataDxfId="161"/>
-    <tableColumn id="6" xr3:uid="{FFD16467-336A-A547-B4D7-4F82B645BDFB}" name="Description" dataDxfId="160"/>
-    <tableColumn id="7" xr3:uid="{00DD245F-92BF-574F-AF05-7500BA8A31B1}" name="DisplayOrder" dataDxfId="159"/>
-    <tableColumn id="8" xr3:uid="{51D53217-2A1C-DA4C-BB84-EF7FA0AEE74E}" name="TitleDisplay" dataDxfId="158"/>
+    <tableColumn id="1" xr3:uid="{3A9C2213-3C87-B242-A50F-DAA873031CFD}" name="LiveFrom" dataDxfId="166"/>
+    <tableColumn id="2" xr3:uid="{4438559D-2DCB-194A-BFAA-A68A1596F0EA}" name="LiveTo" dataDxfId="165"/>
+    <tableColumn id="3" xr3:uid="{20BC5FF0-EE97-BA41-80E0-333D8430A55D}" name="CaseTypeID" dataDxfId="164"/>
+    <tableColumn id="4" xr3:uid="{660AAD23-D344-7148-A6CD-579BFC3B0553}" name="ID" dataDxfId="163"/>
+    <tableColumn id="5" xr3:uid="{0D9AC729-9189-6841-A6A5-90D572AE955C}" name="Name" dataDxfId="162"/>
+    <tableColumn id="6" xr3:uid="{FFD16467-336A-A547-B4D7-4F82B645BDFB}" name="Description" dataDxfId="161"/>
+    <tableColumn id="7" xr3:uid="{00DD245F-92BF-574F-AF05-7500BA8A31B1}" name="DisplayOrder" dataDxfId="160"/>
+    <tableColumn id="8" xr3:uid="{51D53217-2A1C-DA4C-BB84-EF7FA0AEE74E}" name="TitleDisplay" dataDxfId="159"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E477A732-1DEE-F046-8ECD-8D2F086ABA9E}" name="Table10" displayName="Table10" ref="A3:T38" totalsRowShown="0" headerRowDxfId="157" dataDxfId="155" headerRowBorderDxfId="156" tableBorderDxfId="154" totalsRowBorderDxfId="153">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E477A732-1DEE-F046-8ECD-8D2F086ABA9E}" name="Table10" displayName="Table10" ref="A3:T38" totalsRowShown="0" headerRowDxfId="158" dataDxfId="156" headerRowBorderDxfId="157" tableBorderDxfId="155" totalsRowBorderDxfId="154">
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{A9949271-C952-5B4E-BDD4-4AFFF2D8614D}" name="LiveFrom" dataDxfId="152"/>
-    <tableColumn id="2" xr3:uid="{D137D6E5-6C3F-A546-91A2-6E5E88E5BD8A}" name="LiveTo" dataDxfId="151"/>
-    <tableColumn id="3" xr3:uid="{3485553F-1201-FF40-807A-E908084BDCE3}" name="CaseTypeID" dataDxfId="150"/>
-    <tableColumn id="4" xr3:uid="{C3A27859-CA49-9344-834B-BF2BE2280BB4}" name="ID" dataDxfId="149"/>
-    <tableColumn id="5" xr3:uid="{72817C12-B46E-604D-AABA-E2DA5A7F4255}" name="Name" dataDxfId="148"/>
-    <tableColumn id="6" xr3:uid="{06145D1D-7832-CA4E-980E-F24369297133}" name="Description" dataDxfId="147"/>
-    <tableColumn id="7" xr3:uid="{C1DFBC7C-115D-3149-9402-7DEBAC2F59B0}" name="DisplayOrder" dataDxfId="146"/>
-    <tableColumn id="8" xr3:uid="{05E21023-6279-404D-8752-82C93B7DD0FC}" name="PreConditionState(s)" dataDxfId="145"/>
-    <tableColumn id="9" xr3:uid="{57F8432A-B070-BC4C-9AF1-0A4A5ECB36E6}" name="PostConditionState" dataDxfId="144"/>
-    <tableColumn id="10" xr3:uid="{21E5C290-DF7D-984C-AD84-C1D3B8F4424F}" name="CallBackURLAboutToStartEvent" dataDxfId="143" dataCellStyle="Hyperlink"/>
-    <tableColumn id="11" xr3:uid="{2C9FCA41-AF28-F544-8544-3684A2AD897E}" name="RetriesTimeoutAboutToStartEvent" dataDxfId="142"/>
-    <tableColumn id="12" xr3:uid="{D0331CD4-2EE6-504E-8F08-4697D43974EE}" name="CallBackURLAboutToSubmitEvent" dataDxfId="141"/>
-    <tableColumn id="13" xr3:uid="{B34611C8-3477-894C-92ED-CDE1252E012A}" name="RetriesTimeoutURLAboutToSubmitEvent" dataDxfId="140"/>
-    <tableColumn id="14" xr3:uid="{A562B2B1-BF10-184B-B111-9D18B99B33C6}" name="CallBackURLSubmittedEvent" dataDxfId="139"/>
-    <tableColumn id="15" xr3:uid="{D5665814-36D0-5248-A5BE-E38060DE9D83}" name="RetriesTimeoutURLSubmittedEvent" dataDxfId="138"/>
-    <tableColumn id="16" xr3:uid="{9616BB75-22E6-F24C-B873-522862AC1B37}" name="SecurityClassification" dataDxfId="137"/>
-    <tableColumn id="17" xr3:uid="{382FE088-0BCD-084F-9D03-25A08E5400C5}" name="ShowSummary" dataDxfId="136"/>
-    <tableColumn id="18" xr3:uid="{D488E70D-0F94-1F4D-96D4-756627B23921}" name="ShowEventNotes" dataDxfId="135"/>
-    <tableColumn id="19" xr3:uid="{E634F39B-A849-4841-8801-2AF4F6A4CB4E}" name="CanSaveDraft" dataDxfId="134"/>
-    <tableColumn id="20" xr3:uid="{AC1595BB-697C-6344-8AF3-1672794828BA}" name="EndButtonLabel" dataDxfId="133"/>
+    <tableColumn id="1" xr3:uid="{A9949271-C952-5B4E-BDD4-4AFFF2D8614D}" name="LiveFrom" dataDxfId="153"/>
+    <tableColumn id="2" xr3:uid="{D137D6E5-6C3F-A546-91A2-6E5E88E5BD8A}" name="LiveTo" dataDxfId="152"/>
+    <tableColumn id="3" xr3:uid="{3485553F-1201-FF40-807A-E908084BDCE3}" name="CaseTypeID" dataDxfId="151"/>
+    <tableColumn id="4" xr3:uid="{C3A27859-CA49-9344-834B-BF2BE2280BB4}" name="ID" dataDxfId="150"/>
+    <tableColumn id="5" xr3:uid="{72817C12-B46E-604D-AABA-E2DA5A7F4255}" name="Name" dataDxfId="149"/>
+    <tableColumn id="6" xr3:uid="{06145D1D-7832-CA4E-980E-F24369297133}" name="Description" dataDxfId="148"/>
+    <tableColumn id="7" xr3:uid="{C1DFBC7C-115D-3149-9402-7DEBAC2F59B0}" name="DisplayOrder" dataDxfId="147"/>
+    <tableColumn id="8" xr3:uid="{05E21023-6279-404D-8752-82C93B7DD0FC}" name="PreConditionState(s)" dataDxfId="146"/>
+    <tableColumn id="9" xr3:uid="{57F8432A-B070-BC4C-9AF1-0A4A5ECB36E6}" name="PostConditionState" dataDxfId="145"/>
+    <tableColumn id="10" xr3:uid="{21E5C290-DF7D-984C-AD84-C1D3B8F4424F}" name="CallBackURLAboutToStartEvent" dataDxfId="144" dataCellStyle="Hyperlink"/>
+    <tableColumn id="11" xr3:uid="{2C9FCA41-AF28-F544-8544-3684A2AD897E}" name="RetriesTimeoutAboutToStartEvent" dataDxfId="143"/>
+    <tableColumn id="12" xr3:uid="{D0331CD4-2EE6-504E-8F08-4697D43974EE}" name="CallBackURLAboutToSubmitEvent" dataDxfId="142"/>
+    <tableColumn id="13" xr3:uid="{B34611C8-3477-894C-92ED-CDE1252E012A}" name="RetriesTimeoutURLAboutToSubmitEvent" dataDxfId="141"/>
+    <tableColumn id="14" xr3:uid="{A562B2B1-BF10-184B-B111-9D18B99B33C6}" name="CallBackURLSubmittedEvent" dataDxfId="140"/>
+    <tableColumn id="15" xr3:uid="{D5665814-36D0-5248-A5BE-E38060DE9D83}" name="RetriesTimeoutURLSubmittedEvent" dataDxfId="139"/>
+    <tableColumn id="16" xr3:uid="{9616BB75-22E6-F24C-B873-522862AC1B37}" name="SecurityClassification" dataDxfId="138"/>
+    <tableColumn id="17" xr3:uid="{382FE088-0BCD-084F-9D03-25A08E5400C5}" name="ShowSummary" dataDxfId="137"/>
+    <tableColumn id="18" xr3:uid="{D488E70D-0F94-1F4D-96D4-756627B23921}" name="ShowEventNotes" dataDxfId="136"/>
+    <tableColumn id="19" xr3:uid="{E634F39B-A849-4841-8801-2AF4F6A4CB4E}" name="CanSaveDraft" dataDxfId="135"/>
+    <tableColumn id="20" xr3:uid="{AC1595BB-697C-6344-8AF3-1672794828BA}" name="EndButtonLabel" dataDxfId="134"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{3FE29A4D-B6F7-B846-B37F-DE13E60B0795}" name="Table11" displayName="Table11" ref="A3:Q152" totalsRowShown="0" headerRowDxfId="132" dataDxfId="130" headerRowBorderDxfId="131" tableBorderDxfId="129" totalsRowBorderDxfId="128">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{3FE29A4D-B6F7-B846-B37F-DE13E60B0795}" name="Table11" displayName="Table11" ref="A3:Q152" totalsRowShown="0" headerRowDxfId="133" dataDxfId="131" headerRowBorderDxfId="132" tableBorderDxfId="130" totalsRowBorderDxfId="129">
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{09247200-910B-D14F-B26E-C50BECE0CCDE}" name="LiveFrom" dataDxfId="127"/>
-    <tableColumn id="2" xr3:uid="{D786058E-A950-5447-A9D7-81AFC8311866}" name="LiveTo" dataDxfId="126"/>
-    <tableColumn id="3" xr3:uid="{AED0E002-7D37-FB41-AD15-A0C135BF7DB3}" name="CaseTypeID" dataDxfId="125"/>
-    <tableColumn id="4" xr3:uid="{C474B0B2-C3DD-C64D-9F85-849C309F4E8F}" name="CaseEventID" dataDxfId="124"/>
-    <tableColumn id="5" xr3:uid="{E022EAF9-1C59-A049-B2D0-18417D29991E}" name="CaseFieldID" dataDxfId="123"/>
-    <tableColumn id="6" xr3:uid="{BA15E598-8D72-9D46-AB77-B605C7E29638}" name="PageFieldDisplayOrder" dataDxfId="122"/>
-    <tableColumn id="7" xr3:uid="{29A321E2-396E-8048-9500-1781CBB8AF23}" name="DisplayContext" dataDxfId="121"/>
-    <tableColumn id="8" xr3:uid="{500AE31D-F96A-9B4B-A577-919C9F7EB527}" name="PageID" dataDxfId="120"/>
-    <tableColumn id="9" xr3:uid="{77251A7B-4C0C-C44D-98D1-9673C5AAF038}" name="PageLabel" dataDxfId="119"/>
-    <tableColumn id="10" xr3:uid="{C3731FA3-2CB9-F448-B34D-5174A743CFC8}" name="PageDisplayOrder" dataDxfId="118"/>
-    <tableColumn id="11" xr3:uid="{087C997E-1430-BA4E-BE31-C1E6F8A09FC4}" name="PageColumnNumber" dataDxfId="117"/>
-    <tableColumn id="12" xr3:uid="{5F8D1DCD-BFA6-5D41-9085-4E8392AFBA5C}" name="FieldShowCondition" dataDxfId="116"/>
-    <tableColumn id="13" xr3:uid="{60ABBC14-F21E-7149-B13C-78981EAAC5AD}" name="PageShowCondition" dataDxfId="115"/>
-    <tableColumn id="14" xr3:uid="{92F3BFA3-CAC9-2C47-B4B5-E5193838BFBF}" name="DisplayContextParameter" dataDxfId="114"/>
-    <tableColumn id="15" xr3:uid="{6E7E82A2-72B3-1E4A-BB83-8C87B685E5AC}" name="ShowSummaryChangeOption" dataDxfId="113"/>
-    <tableColumn id="16" xr3:uid="{11418AC4-C205-D945-A936-1A37779FB35F}" name="ShowSummaryContentOption" dataDxfId="112"/>
-    <tableColumn id="17" xr3:uid="{CB58B471-584C-5B49-865D-C3B523596273}" name="CallBackURLMidEvent" dataDxfId="111"/>
+    <tableColumn id="1" xr3:uid="{09247200-910B-D14F-B26E-C50BECE0CCDE}" name="LiveFrom" dataDxfId="128"/>
+    <tableColumn id="2" xr3:uid="{D786058E-A950-5447-A9D7-81AFC8311866}" name="LiveTo" dataDxfId="127"/>
+    <tableColumn id="3" xr3:uid="{AED0E002-7D37-FB41-AD15-A0C135BF7DB3}" name="CaseTypeID" dataDxfId="126"/>
+    <tableColumn id="4" xr3:uid="{C474B0B2-C3DD-C64D-9F85-849C309F4E8F}" name="CaseEventID" dataDxfId="125"/>
+    <tableColumn id="5" xr3:uid="{E022EAF9-1C59-A049-B2D0-18417D29991E}" name="CaseFieldID" dataDxfId="124"/>
+    <tableColumn id="6" xr3:uid="{BA15E598-8D72-9D46-AB77-B605C7E29638}" name="PageFieldDisplayOrder" dataDxfId="123"/>
+    <tableColumn id="7" xr3:uid="{29A321E2-396E-8048-9500-1781CBB8AF23}" name="DisplayContext" dataDxfId="122"/>
+    <tableColumn id="8" xr3:uid="{500AE31D-F96A-9B4B-A577-919C9F7EB527}" name="PageID" dataDxfId="121"/>
+    <tableColumn id="9" xr3:uid="{77251A7B-4C0C-C44D-98D1-9673C5AAF038}" name="PageLabel" dataDxfId="120"/>
+    <tableColumn id="10" xr3:uid="{C3731FA3-2CB9-F448-B34D-5174A743CFC8}" name="PageDisplayOrder" dataDxfId="119"/>
+    <tableColumn id="11" xr3:uid="{087C997E-1430-BA4E-BE31-C1E6F8A09FC4}" name="PageColumnNumber" dataDxfId="118"/>
+    <tableColumn id="12" xr3:uid="{5F8D1DCD-BFA6-5D41-9085-4E8392AFBA5C}" name="FieldShowCondition" dataDxfId="117"/>
+    <tableColumn id="13" xr3:uid="{60ABBC14-F21E-7149-B13C-78981EAAC5AD}" name="PageShowCondition" dataDxfId="116"/>
+    <tableColumn id="14" xr3:uid="{92F3BFA3-CAC9-2C47-B4B5-E5193838BFBF}" name="DisplayContextParameter" dataDxfId="115"/>
+    <tableColumn id="15" xr3:uid="{6E7E82A2-72B3-1E4A-BB83-8C87B685E5AC}" name="ShowSummaryChangeOption" dataDxfId="114"/>
+    <tableColumn id="16" xr3:uid="{11418AC4-C205-D945-A936-1A37779FB35F}" name="ShowSummaryContentOption" dataDxfId="113"/>
+    <tableColumn id="17" xr3:uid="{CB58B471-584C-5B49-865D-C3B523596273}" name="CallBackURLMidEvent" dataDxfId="112"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C0942DB8-64D6-184E-8B7E-425FFE75053F}" name="Table12" displayName="Table12" ref="A3:H46" totalsRowShown="0" headerRowDxfId="110" dataDxfId="108" headerRowBorderDxfId="109" tableBorderDxfId="107" totalsRowBorderDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C0942DB8-64D6-184E-8B7E-425FFE75053F}" name="Table12" displayName="Table12" ref="A3:H46" totalsRowShown="0" headerRowDxfId="111" dataDxfId="109" headerRowBorderDxfId="110" tableBorderDxfId="108" totalsRowBorderDxfId="107">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{D94535AC-AF6B-A346-9394-2AEC1726FFC2}" name="LiveFrom" dataDxfId="105"/>
-    <tableColumn id="2" xr3:uid="{C1E40171-ED97-924B-9092-45E6DCB4FBD8}" name="LiveTo" dataDxfId="104"/>
-    <tableColumn id="3" xr3:uid="{22DC41E1-CD9E-1242-8CBA-BC0A19E00355}" name="CaseTypeID" dataDxfId="103"/>
-    <tableColumn id="4" xr3:uid="{84C83114-BBD1-C244-AF58-8DD790788A0E}" name="CaseFieldID" dataDxfId="102"/>
-    <tableColumn id="5" xr3:uid="{0346AC0F-F0E3-154A-9634-D0AA66CA21FD}" name="ListElementCode" dataDxfId="101"/>
-    <tableColumn id="6" xr3:uid="{E6AADCBC-8243-9F41-B0DB-0BE53FC0C362}" name="Label" dataDxfId="100"/>
-    <tableColumn id="7" xr3:uid="{FCF69EEE-2E56-444B-86FC-7F66B3D6AC95}" name="DisplayOrder" dataDxfId="99"/>
-    <tableColumn id="8" xr3:uid="{35DCFF60-D0A8-B54E-82C5-A30ED8395060}" name="DisplayContextParameter" dataDxfId="98"/>
+    <tableColumn id="1" xr3:uid="{D94535AC-AF6B-A346-9394-2AEC1726FFC2}" name="LiveFrom" dataDxfId="106"/>
+    <tableColumn id="2" xr3:uid="{C1E40171-ED97-924B-9092-45E6DCB4FBD8}" name="LiveTo" dataDxfId="105"/>
+    <tableColumn id="3" xr3:uid="{22DC41E1-CD9E-1242-8CBA-BC0A19E00355}" name="CaseTypeID" dataDxfId="104"/>
+    <tableColumn id="4" xr3:uid="{84C83114-BBD1-C244-AF58-8DD790788A0E}" name="CaseFieldID" dataDxfId="103"/>
+    <tableColumn id="5" xr3:uid="{0346AC0F-F0E3-154A-9634-D0AA66CA21FD}" name="ListElementCode" dataDxfId="102"/>
+    <tableColumn id="6" xr3:uid="{E6AADCBC-8243-9F41-B0DB-0BE53FC0C362}" name="Label" dataDxfId="101"/>
+    <tableColumn id="7" xr3:uid="{FCF69EEE-2E56-444B-86FC-7F66B3D6AC95}" name="DisplayOrder" dataDxfId="100"/>
+    <tableColumn id="8" xr3:uid="{35DCFF60-D0A8-B54E-82C5-A30ED8395060}" name="DisplayContextParameter" dataDxfId="99"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E7EE5CF4-F848-A444-80DE-82691AE949C0}" name="Table14" displayName="Table14" ref="A3:G35" totalsRowShown="0" headerRowDxfId="97" dataDxfId="95" headerRowBorderDxfId="96" tableBorderDxfId="94" totalsRowBorderDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E7EE5CF4-F848-A444-80DE-82691AE949C0}" name="Table14" displayName="Table14" ref="A3:G35" totalsRowShown="0" headerRowDxfId="98" dataDxfId="96" headerRowBorderDxfId="97" tableBorderDxfId="95" totalsRowBorderDxfId="94">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3A97DD00-8341-8A41-A062-99688A018570}" name="LiveFrom" dataDxfId="92"/>
-    <tableColumn id="2" xr3:uid="{7F24098A-B78A-4D49-BA3A-C64496932992}" name="LiveTo" dataDxfId="91"/>
-    <tableColumn id="3" xr3:uid="{4CECB00E-A59E-564E-9219-37AD7AAD6CA5}" name="CaseTypeID" dataDxfId="90"/>
-    <tableColumn id="4" xr3:uid="{32CEDFFA-35E9-B14E-89B8-F141DF840E42}" name="CaseFieldID" dataDxfId="89"/>
-    <tableColumn id="5" xr3:uid="{8A24F22E-1F45-F74A-B5FB-62E38937CC1B}" name="Label" dataDxfId="88"/>
-    <tableColumn id="6" xr3:uid="{73036E3A-A2DE-6345-B66E-F08F294B3920}" name="ListElementCode" dataDxfId="87"/>
-    <tableColumn id="7" xr3:uid="{0835D7A8-697B-CC41-AD8F-1A04E56A255E}" name="DisplayOrder" dataDxfId="86"/>
+    <tableColumn id="1" xr3:uid="{3A97DD00-8341-8A41-A062-99688A018570}" name="LiveFrom" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{7F24098A-B78A-4D49-BA3A-C64496932992}" name="LiveTo" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{4CECB00E-A59E-564E-9219-37AD7AAD6CA5}" name="CaseTypeID" dataDxfId="91"/>
+    <tableColumn id="4" xr3:uid="{32CEDFFA-35E9-B14E-89B8-F141DF840E42}" name="CaseFieldID" dataDxfId="90"/>
+    <tableColumn id="5" xr3:uid="{8A24F22E-1F45-F74A-B5FB-62E38937CC1B}" name="Label" dataDxfId="89"/>
+    <tableColumn id="6" xr3:uid="{73036E3A-A2DE-6345-B66E-F08F294B3920}" name="ListElementCode" dataDxfId="88"/>
+    <tableColumn id="7" xr3:uid="{0835D7A8-697B-CC41-AD8F-1A04E56A255E}" name="DisplayOrder" dataDxfId="87"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{23DB5BED-2DD5-DE42-8EA2-592AC1696272}" name="Table15" displayName="Table15" ref="A3:H52" totalsRowShown="0" headerRowDxfId="85" dataDxfId="83" headerRowBorderDxfId="84" tableBorderDxfId="82" totalsRowBorderDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{23DB5BED-2DD5-DE42-8EA2-592AC1696272}" name="Table15" displayName="Table15" ref="A3:H52" totalsRowShown="0" headerRowDxfId="86" dataDxfId="84" headerRowBorderDxfId="85" tableBorderDxfId="83" totalsRowBorderDxfId="82">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{4FCEDBE0-A9B0-0441-86AD-C7E7E6374F81}" name="LiveFrom" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{56793764-D9BF-1745-BA2A-131F10197717}" name="LiveTo" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{7B736E9A-236E-E84D-AB00-D5119AE8FDF4}" name="CaseTypeID" dataDxfId="78"/>
-    <tableColumn id="4" xr3:uid="{B2C20176-DB0A-0249-981A-083B6720F21B}" name="CaseFieldID" dataDxfId="77"/>
-    <tableColumn id="5" xr3:uid="{CA39F3C7-9B7B-1540-8FA6-8FE5E75DB625}" name="ListElementCode" dataDxfId="76"/>
-    <tableColumn id="6" xr3:uid="{B86E7729-2A08-3346-89EB-D64286E6CEED}" name="Label" dataDxfId="75"/>
-    <tableColumn id="7" xr3:uid="{E92211C5-8284-6246-B2E2-BC654D7297A5}" name="DisplayOrder" dataDxfId="74"/>
-    <tableColumn id="8" xr3:uid="{23A34836-8CA8-D941-A339-02B719A12676}" name="DisplayContextParameter" dataDxfId="73"/>
+    <tableColumn id="1" xr3:uid="{4FCEDBE0-A9B0-0441-86AD-C7E7E6374F81}" name="LiveFrom" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{56793764-D9BF-1745-BA2A-131F10197717}" name="LiveTo" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{7B736E9A-236E-E84D-AB00-D5119AE8FDF4}" name="CaseTypeID" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{B2C20176-DB0A-0249-981A-083B6720F21B}" name="CaseFieldID" dataDxfId="78"/>
+    <tableColumn id="5" xr3:uid="{CA39F3C7-9B7B-1540-8FA6-8FE5E75DB625}" name="ListElementCode" dataDxfId="77"/>
+    <tableColumn id="6" xr3:uid="{B86E7729-2A08-3346-89EB-D64286E6CEED}" name="Label" dataDxfId="76"/>
+    <tableColumn id="7" xr3:uid="{E92211C5-8284-6246-B2E2-BC654D7297A5}" name="DisplayOrder" dataDxfId="75"/>
+    <tableColumn id="8" xr3:uid="{23A34836-8CA8-D941-A339-02B719A12676}" name="DisplayContextParameter" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{0CA40DD8-8152-3D46-8168-0AE0B6974BE8}" name="Table16" displayName="Table16" ref="A3:I52" totalsRowShown="0" headerRowDxfId="72" dataDxfId="70" headerRowBorderDxfId="71" tableBorderDxfId="69" totalsRowBorderDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{0CA40DD8-8152-3D46-8168-0AE0B6974BE8}" name="Table16" displayName="Table16" ref="A3:I52" totalsRowShown="0" headerRowDxfId="73" dataDxfId="71" headerRowBorderDxfId="72" tableBorderDxfId="70" totalsRowBorderDxfId="69">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{89FB5309-B489-D04A-A245-5D0966E24720}" name="LiveFrom" dataDxfId="67"/>
-    <tableColumn id="2" xr3:uid="{0FF183E8-34AA-1E40-9440-3AF75B9978C6}" name="LiveTo" dataDxfId="66"/>
-    <tableColumn id="3" xr3:uid="{3390D839-8BB1-154A-AE30-84D075D9116D}" name="CaseTypeID" dataDxfId="65"/>
-    <tableColumn id="4" xr3:uid="{35990B77-262E-AE45-8172-61C1076B15BA}" name="CaseFieldID" dataDxfId="64"/>
-    <tableColumn id="7" xr3:uid="{70CF7FE5-8C40-2744-A7FE-26E60C76A62F}" name="ListElementCode" dataDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{BB41D60A-EC82-9941-A7B0-EF6AA438629F}" name="Label" dataDxfId="62"/>
-    <tableColumn id="6" xr3:uid="{031B36DA-C870-5745-A2EF-349414540475}" name="DisplayOrder" dataDxfId="61"/>
-    <tableColumn id="8" xr3:uid="{D282B24B-D0FD-DA44-9FC3-F20196FBA42D}" name="ResultsOrdering" dataDxfId="60"/>
-    <tableColumn id="9" xr3:uid="{7023267C-7AEA-EA4A-B007-2A8D3955A354}" name="DisplayContextParameter" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{89FB5309-B489-D04A-A245-5D0966E24720}" name="LiveFrom" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{0FF183E8-34AA-1E40-9440-3AF75B9978C6}" name="LiveTo" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{3390D839-8BB1-154A-AE30-84D075D9116D}" name="CaseTypeID" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{35990B77-262E-AE45-8172-61C1076B15BA}" name="CaseFieldID" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{70CF7FE5-8C40-2744-A7FE-26E60C76A62F}" name="ListElementCode" dataDxfId="64"/>
+    <tableColumn id="5" xr3:uid="{BB41D60A-EC82-9941-A7B0-EF6AA438629F}" name="Label" dataDxfId="63"/>
+    <tableColumn id="6" xr3:uid="{031B36DA-C870-5745-A2EF-349414540475}" name="DisplayOrder" dataDxfId="62"/>
+    <tableColumn id="8" xr3:uid="{D282B24B-D0FD-DA44-9FC3-F20196FBA42D}" name="ResultsOrdering" dataDxfId="61"/>
+    <tableColumn id="9" xr3:uid="{7023267C-7AEA-EA4A-B007-2A8D3955A354}" name="DisplayContextParameter" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{68D1BADF-97D2-B54C-B71F-46D015D9E181}" name="Table17" displayName="Table17" ref="A3:F5" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55" totalsRowBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{68D1BADF-97D2-B54C-B71F-46D015D9E181}" name="Table17" displayName="Table17" ref="A3:F5" totalsRowShown="0" headerRowDxfId="59" dataDxfId="57" headerRowBorderDxfId="58" tableBorderDxfId="56" totalsRowBorderDxfId="55">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7E998E97-505C-684E-9311-941AC17D5757}" name="LiveFrom" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{374279D4-23E7-9049-A9CB-C1788CC30194}" name="LiveTo" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{ADDEDA3F-CF2C-6D47-BC79-E1E4F6B6FF9B}" name="UserIDAMId" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{5D5CFFD9-D505-374F-8608-56EFBB6781C4}" name="WorkBasketDefaultJurisdiction" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{B2DEADF8-CB97-CD4B-9539-A848AD58DF04}" name="WorkBasketDefaultCaseType" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{CCAA7475-CF17-FD4A-B27C-B26DE0267EB6}" name="WorkBasketDefaultState" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{7E998E97-505C-684E-9311-941AC17D5757}" name="LiveFrom" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{374279D4-23E7-9049-A9CB-C1788CC30194}" name="LiveTo" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{ADDEDA3F-CF2C-6D47-BC79-E1E4F6B6FF9B}" name="UserIDAMId" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{5D5CFFD9-D505-374F-8608-56EFBB6781C4}" name="WorkBasketDefaultJurisdiction" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{B2DEADF8-CB97-CD4B-9539-A848AD58DF04}" name="WorkBasketDefaultCaseType" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{CCAA7475-CF17-FD4A-B27C-B26DE0267EB6}" name="WorkBasketDefaultState" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E19" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E19" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D7EDF212-81C7-1F49-98C0-8F28E87DCE6C}" name="LiveFrom" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{36550BF7-0E65-0D45-9932-4D227DD7D5DE}" name="LiveTo" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{D8A5019D-CCD7-0844-A9A5-378A259F60E5}" name="CaseTypeID" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{592355E2-FBF9-0947-A50E-1100535FD79E}" name="UserRole" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{B020D27C-2BA7-4145-B517-CECBAD029F6A}" name="CRUD" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{D7EDF212-81C7-1F49-98C0-8F28E87DCE6C}" name="LiveFrom" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{36550BF7-0E65-0D45-9932-4D227DD7D5DE}" name="LiveTo" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{D8A5019D-CCD7-0844-A9A5-378A259F60E5}" name="CaseTypeID" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{592355E2-FBF9-0947-A50E-1100535FD79E}" name="UserRole" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{B020D27C-2BA7-4145-B517-CECBAD029F6A}" name="CRUD" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F126" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F126" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{72C60802-2E7D-F542-8A1C-F0E147FA4DCE}" name="LiveFrom" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{FC67D30A-2836-1743-B4FA-D61DEE5FAF0A}" name="LiveTo" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{DE9841E4-2385-6944-AC9E-2418EBE9C323}" name="CaseTypeID" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{129D8AD7-2252-2343-A6AC-C828E01663E8}" name="CaseFieldID" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{313DEE97-0F1D-EB44-AAA1-862E98AA51C6}" name="UserRole" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{ED6F0D67-5349-4C4E-8FFC-F133A2D34661}" name="CRUD" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{72C60802-2E7D-F542-8A1C-F0E147FA4DCE}" name="LiveFrom" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{FC67D30A-2836-1743-B4FA-D61DEE5FAF0A}" name="LiveTo" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{DE9841E4-2385-6944-AC9E-2418EBE9C323}" name="CaseTypeID" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{129D8AD7-2252-2343-A6AC-C828E01663E8}" name="CaseFieldID" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{313DEE97-0F1D-EB44-AAA1-862E98AA51C6}" name="UserRole" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{ED6F0D67-5349-4C4E-8FFC-F133A2D34661}" name="CRUD" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C2696846-A994-B14A-A929-B58A056832F8}" name="Table4" displayName="Table4" ref="A3:D4" totalsRowShown="0" headerRowDxfId="291" dataDxfId="289" headerRowBorderDxfId="290" tableBorderDxfId="288" totalsRowBorderDxfId="287">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C2696846-A994-B14A-A929-B58A056832F8}" name="Table4" displayName="Table4" ref="A3:D4" totalsRowShown="0" headerRowDxfId="292" dataDxfId="290" headerRowBorderDxfId="291" tableBorderDxfId="289" totalsRowBorderDxfId="288">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DAC385B5-3CA7-F54F-ABF5-8A0FB9739A81}" name="BannerEnabled" dataDxfId="286"/>
-    <tableColumn id="2" xr3:uid="{5063DD1E-29B3-9240-B104-B878A78A961D}" name="BannerDescription" dataDxfId="285"/>
-    <tableColumn id="3" xr3:uid="{1802650A-8968-8C49-94DD-3A508725B56E}" name="BannerUrlText" dataDxfId="284"/>
-    <tableColumn id="4" xr3:uid="{C2492B8E-6768-C945-9E6B-68B481B89F36}" name="BannerUrl" dataDxfId="283" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{DAC385B5-3CA7-F54F-ABF5-8A0FB9739A81}" name="BannerEnabled" dataDxfId="287"/>
+    <tableColumn id="2" xr3:uid="{5063DD1E-29B3-9240-B104-B878A78A961D}" name="BannerDescription" dataDxfId="286"/>
+    <tableColumn id="3" xr3:uid="{1802650A-8968-8C49-94DD-3A508725B56E}" name="BannerUrlText" dataDxfId="285"/>
+    <tableColumn id="4" xr3:uid="{C2492B8E-6768-C945-9E6B-68B481B89F36}" name="BannerUrl" dataDxfId="284" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{F689229C-DA57-CE47-9FAB-39CC9062D12E}" name="Table20" displayName="Table20" ref="A3:D7" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{F689229C-DA57-CE47-9FAB-39CC9062D12E}" name="Table20" displayName="Table20" ref="A3:D7" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{108C9CDA-76BA-EE4D-8549-5BED5EA603A6}" name="CaseTypeID" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{4C2ED72C-37EE-A14B-9BFE-577416753198}" name="ID" dataDxfId="22" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{A13E9F3C-9866-6844-97A2-CECF13410611}" name="Name" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{5010B2BB-616D-A946-8844-A944EB690018}" name="Description" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{108C9CDA-76BA-EE4D-8549-5BED5EA603A6}" name="CaseTypeID" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{4C2ED72C-37EE-A14B-9BFE-577416753198}" name="ID" dataDxfId="23" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{A13E9F3C-9866-6844-97A2-CECF13410611}" name="Name" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{5010B2BB-616D-A946-8844-A944EB690018}" name="Description" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F44" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F44" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{EE9F57B3-787C-C642-A2B0-1CB2CD584A64}" name="CaseTypeID" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{A6633300-114A-5846-B7B7-C57244A39F58}" name="CaseEventID" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{229CDFFE-02D8-6042-9F1C-B67EA1F30C09}" name="UserRole" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{872585F6-B038-2149-8440-E4F3A404C8A9}" name="CRUD" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{EE9F57B3-787C-C642-A2B0-1CB2CD584A64}" name="CaseTypeID" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{A6633300-114A-5846-B7B7-C57244A39F58}" name="CaseEventID" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{229CDFFE-02D8-6042-9F1C-B67EA1F30C09}" name="UserRole" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{872585F6-B038-2149-8440-E4F3A404C8A9}" name="CRUD" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F32" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F32" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{F6F18BFB-2335-8D4F-9DC5-89FC7FD3B64B}" name="CaseTypeID" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{EB11A8E2-8EA8-0B46-B3B3-103461A3AF54}" name="CaseStateID" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{1C1D63D9-6997-9E47-9725-BB01CA7FD1F3}" name="UserRole" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{82473FFF-1C61-B242-A091-BA139462FACF}" name="CRUD" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{F6F18BFB-2335-8D4F-9DC5-89FC7FD3B64B}" name="CaseTypeID" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{EB11A8E2-8EA8-0B46-B3B3-103461A3AF54}" name="CaseStateID" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{1C1D63D9-6997-9E47-9725-BB01CA7FD1F3}" name="UserRole" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{82473FFF-1C61-B242-A091-BA139462FACF}" name="CRUD" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40D0FC50-9439-5741-A23D-29ACBB37469B}" name="Table3" displayName="Table3" ref="A3:I17" totalsRowShown="0" headerRowDxfId="282" dataDxfId="280" headerRowBorderDxfId="281" tableBorderDxfId="279" totalsRowBorderDxfId="278">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40D0FC50-9439-5741-A23D-29ACBB37469B}" name="Table3" displayName="Table3" ref="A3:I17" totalsRowShown="0" headerRowDxfId="283" dataDxfId="281" headerRowBorderDxfId="282" tableBorderDxfId="280" totalsRowBorderDxfId="279">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D407453C-8672-E84F-A1D8-F563E678DC8E}" name="LiveFrom" dataDxfId="277"/>
-    <tableColumn id="2" xr3:uid="{14122774-0C33-6C4D-A9AB-91FA15DB8A2C}" name="LiveTo" dataDxfId="276"/>
-    <tableColumn id="3" xr3:uid="{CB71BBA2-34F1-C545-B80D-4FB0AC6ACAFF}" name="ID" dataDxfId="275"/>
-    <tableColumn id="4" xr3:uid="{2CFC219C-166E-B343-97B5-1158954E0D8F}" name="Name" dataDxfId="274"/>
-    <tableColumn id="5" xr3:uid="{5592454F-E93D-5A44-B0EC-7DBD0663FC3A}" name="Description" dataDxfId="273"/>
-    <tableColumn id="6" xr3:uid="{0DB64C3F-680C-9C46-96C5-C0C984291BE2}" name="JurisdictionID" dataDxfId="272"/>
-    <tableColumn id="7" xr3:uid="{3EF72FC4-7B2C-7D46-8B03-99FBCADE4E25}" name="PrintableDocumentsUrl" dataDxfId="271"/>
-    <tableColumn id="8" xr3:uid="{35352FF6-3E6C-7440-9592-B69B66487A2F}" name="RetriesTimeoutURLPrintEvent" dataDxfId="270"/>
-    <tableColumn id="9" xr3:uid="{1ACB6DB4-FECA-7B47-9847-0243E309AD6A}" name="SecurityClassification" dataDxfId="269"/>
+    <tableColumn id="1" xr3:uid="{D407453C-8672-E84F-A1D8-F563E678DC8E}" name="LiveFrom" dataDxfId="278"/>
+    <tableColumn id="2" xr3:uid="{14122774-0C33-6C4D-A9AB-91FA15DB8A2C}" name="LiveTo" dataDxfId="277"/>
+    <tableColumn id="3" xr3:uid="{CB71BBA2-34F1-C545-B80D-4FB0AC6ACAFF}" name="ID" dataDxfId="276"/>
+    <tableColumn id="4" xr3:uid="{2CFC219C-166E-B343-97B5-1158954E0D8F}" name="Name" dataDxfId="275"/>
+    <tableColumn id="5" xr3:uid="{5592454F-E93D-5A44-B0EC-7DBD0663FC3A}" name="Description" dataDxfId="274"/>
+    <tableColumn id="6" xr3:uid="{0DB64C3F-680C-9C46-96C5-C0C984291BE2}" name="JurisdictionID" dataDxfId="273"/>
+    <tableColumn id="7" xr3:uid="{3EF72FC4-7B2C-7D46-8B03-99FBCADE4E25}" name="PrintableDocumentsUrl" dataDxfId="272"/>
+    <tableColumn id="8" xr3:uid="{35352FF6-3E6C-7440-9592-B69B66487A2F}" name="RetriesTimeoutURLPrintEvent" dataDxfId="271"/>
+    <tableColumn id="9" xr3:uid="{1ACB6DB4-FECA-7B47-9847-0243E309AD6A}" name="SecurityClassification" dataDxfId="270"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7853914-D748-214F-AB78-CCB4D9972099}" name="Table1" displayName="Table1" ref="A3:M126" totalsRowShown="0" headerRowDxfId="268" dataDxfId="266" headerRowBorderDxfId="267" tableBorderDxfId="265" totalsRowBorderDxfId="264">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7853914-D748-214F-AB78-CCB4D9972099}" name="Table1" displayName="Table1" ref="A3:M126" totalsRowShown="0" headerRowDxfId="269" dataDxfId="267" headerRowBorderDxfId="268" tableBorderDxfId="266" totalsRowBorderDxfId="265">
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{E6FCE3E8-E7C3-7C45-8832-C5E6EBCF5AD5}" name="LiveFrom" dataDxfId="263"/>
-    <tableColumn id="2" xr3:uid="{CCAF30FC-5E10-F84C-B526-0674ECA9972F}" name="LiveTo" dataDxfId="262"/>
-    <tableColumn id="3" xr3:uid="{9C767F7C-E4A3-E840-9D9C-30A8E9D03DE5}" name="CaseTypeID" dataDxfId="261"/>
-    <tableColumn id="4" xr3:uid="{0094B065-3327-9942-8F35-B92CB893A599}" name="ID" dataDxfId="260"/>
-    <tableColumn id="5" xr3:uid="{4CDE5603-12E3-DC45-91B4-D3F9BD04951B}" name="Label" dataDxfId="259"/>
-    <tableColumn id="6" xr3:uid="{5191E0DF-A515-CB40-9BD8-A0244E4F8C57}" name="HintText" dataDxfId="258"/>
-    <tableColumn id="7" xr3:uid="{00561C5B-D5D1-DC47-8E78-49D3C85569ED}" name="FieldType" dataDxfId="257"/>
-    <tableColumn id="13" xr3:uid="{41692C06-7AD8-F04A-B809-308DF1149252}" name="CategoryID" dataDxfId="256"/>
-    <tableColumn id="8" xr3:uid="{10BF8A09-644E-FB4A-8572-93D527306174}" name="FieldTypeParameter" dataDxfId="255"/>
-    <tableColumn id="9" xr3:uid="{DBABBB37-2DCF-2241-AEE6-1F2042FDD321}" name="RegularExpression" dataDxfId="254"/>
-    <tableColumn id="10" xr3:uid="{04F14DFC-0A0D-ED4E-B6FF-D294F3DF9079}" name="SecurityClassification" dataDxfId="253"/>
-    <tableColumn id="11" xr3:uid="{715917FF-FEBF-B843-A600-2D124CAB48A3}" name="Min" dataDxfId="252"/>
-    <tableColumn id="12" xr3:uid="{5FE67360-F088-F14B-A346-DE81B164ECE4}" name="Max" dataDxfId="251"/>
+    <tableColumn id="1" xr3:uid="{E6FCE3E8-E7C3-7C45-8832-C5E6EBCF5AD5}" name="LiveFrom" dataDxfId="264"/>
+    <tableColumn id="2" xr3:uid="{CCAF30FC-5E10-F84C-B526-0674ECA9972F}" name="LiveTo" dataDxfId="263"/>
+    <tableColumn id="3" xr3:uid="{9C767F7C-E4A3-E840-9D9C-30A8E9D03DE5}" name="CaseTypeID" dataDxfId="262"/>
+    <tableColumn id="4" xr3:uid="{0094B065-3327-9942-8F35-B92CB893A599}" name="ID" dataDxfId="261"/>
+    <tableColumn id="5" xr3:uid="{4CDE5603-12E3-DC45-91B4-D3F9BD04951B}" name="Label" dataDxfId="260"/>
+    <tableColumn id="6" xr3:uid="{5191E0DF-A515-CB40-9BD8-A0244E4F8C57}" name="HintText" dataDxfId="259"/>
+    <tableColumn id="7" xr3:uid="{00561C5B-D5D1-DC47-8E78-49D3C85569ED}" name="FieldType" dataDxfId="258"/>
+    <tableColumn id="13" xr3:uid="{41692C06-7AD8-F04A-B809-308DF1149252}" name="CategoryID" dataDxfId="257"/>
+    <tableColumn id="8" xr3:uid="{10BF8A09-644E-FB4A-8572-93D527306174}" name="FieldTypeParameter" dataDxfId="256"/>
+    <tableColumn id="9" xr3:uid="{DBABBB37-2DCF-2241-AEE6-1F2042FDD321}" name="RegularExpression" dataDxfId="255"/>
+    <tableColumn id="10" xr3:uid="{04F14DFC-0A0D-ED4E-B6FF-D294F3DF9079}" name="SecurityClassification" dataDxfId="254"/>
+    <tableColumn id="11" xr3:uid="{715917FF-FEBF-B843-A600-2D124CAB48A3}" name="Min" dataDxfId="253"/>
+    <tableColumn id="12" xr3:uid="{5FE67360-F088-F14B-A346-DE81B164ECE4}" name="Max" dataDxfId="252"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74540BC8-D704-5047-98FB-694A477BC83D}" name="Table2" displayName="Table2" ref="A3:R76" totalsRowShown="0" headerRowDxfId="250" dataDxfId="248" headerRowBorderDxfId="249" tableBorderDxfId="247" totalsRowBorderDxfId="246">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74540BC8-D704-5047-98FB-694A477BC83D}" name="Table2" displayName="Table2" ref="A3:R76" totalsRowShown="0" headerRowDxfId="251" dataDxfId="249" headerRowBorderDxfId="250" tableBorderDxfId="248" totalsRowBorderDxfId="247">
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{069BCF45-09C7-1D4D-9D96-EA818F065192}" name="LiveFrom" dataDxfId="245"/>
-    <tableColumn id="2" xr3:uid="{3201B607-7572-A641-B166-02ABBDA29C68}" name="LiveTo" dataDxfId="244"/>
-    <tableColumn id="3" xr3:uid="{BF418433-54F7-784B-88CA-F18E9603844B}" name="ID" dataDxfId="243"/>
-    <tableColumn id="4" xr3:uid="{9C8DE998-5550-0640-B6C2-CB5427FC3A63}" name="ListElementCode" dataDxfId="242"/>
-    <tableColumn id="5" xr3:uid="{D21D6A37-98CD-4E4A-BCE8-9A25879A6E2D}" name="FieldType" dataDxfId="241"/>
-    <tableColumn id="14" xr3:uid="{0CA72D38-CCA8-E348-8398-3563015AFFB0}" name="CategoryID" dataDxfId="240"/>
-    <tableColumn id="6" xr3:uid="{4BAE99B3-6B76-CF47-810C-6E284FAC7C45}" name="FieldTypeParameter" dataDxfId="239"/>
-    <tableColumn id="7" xr3:uid="{4E74D643-6B67-0D46-9AB2-7DF2E1703511}" name="ElementLabel" dataDxfId="238"/>
-    <tableColumn id="8" xr3:uid="{C675650F-2935-D647-A61E-517A892F4378}" name="FieldShowCondition" dataDxfId="237"/>
-    <tableColumn id="9" xr3:uid="{EA69CEA6-E76B-D949-9578-347B7A74E10D}" name="RegularExpression" dataDxfId="236"/>
-    <tableColumn id="10" xr3:uid="{D3A49B2C-58F9-B842-9608-581A999364E4}" name="HintText" dataDxfId="235"/>
-    <tableColumn id="11" xr3:uid="{CC47353C-D501-AA41-8CF6-3B49859BA97A}" name="SecurityClassification" dataDxfId="234"/>
-    <tableColumn id="12" xr3:uid="{6EBA010E-76A9-2946-B1FA-052FBF58B238}" name="Min" dataDxfId="233"/>
-    <tableColumn id="13" xr3:uid="{60640AE7-10CC-AB4C-B4E8-13C947D3CC74}" name="Max" dataDxfId="232"/>
-    <tableColumn id="15" xr3:uid="{C2DEBC92-657F-8B48-AEF6-35F078A0DDF4}" name="DisplayContextParameter" dataDxfId="231"/>
-    <tableColumn id="16" xr3:uid="{1D93B227-456B-3E42-85B4-0F278B7523D8}" name="Column2" dataDxfId="230"/>
-    <tableColumn id="17" xr3:uid="{F79DC235-9922-6D4E-9889-C653A521E8AE}" name="Column3" dataDxfId="229"/>
-    <tableColumn id="18" xr3:uid="{F1215911-B6F6-C345-9EC6-179495CC62C1}" name="Column4" dataDxfId="228"/>
+    <tableColumn id="1" xr3:uid="{069BCF45-09C7-1D4D-9D96-EA818F065192}" name="LiveFrom" dataDxfId="246"/>
+    <tableColumn id="2" xr3:uid="{3201B607-7572-A641-B166-02ABBDA29C68}" name="LiveTo" dataDxfId="245"/>
+    <tableColumn id="3" xr3:uid="{BF418433-54F7-784B-88CA-F18E9603844B}" name="ID" dataDxfId="244"/>
+    <tableColumn id="4" xr3:uid="{9C8DE998-5550-0640-B6C2-CB5427FC3A63}" name="ListElementCode" dataDxfId="243"/>
+    <tableColumn id="5" xr3:uid="{D21D6A37-98CD-4E4A-BCE8-9A25879A6E2D}" name="FieldType" dataDxfId="242"/>
+    <tableColumn id="14" xr3:uid="{0CA72D38-CCA8-E348-8398-3563015AFFB0}" name="CategoryID" dataDxfId="241"/>
+    <tableColumn id="6" xr3:uid="{4BAE99B3-6B76-CF47-810C-6E284FAC7C45}" name="FieldTypeParameter" dataDxfId="240"/>
+    <tableColumn id="7" xr3:uid="{4E74D643-6B67-0D46-9AB2-7DF2E1703511}" name="ElementLabel" dataDxfId="239"/>
+    <tableColumn id="8" xr3:uid="{C675650F-2935-D647-A61E-517A892F4378}" name="FieldShowCondition" dataDxfId="238"/>
+    <tableColumn id="9" xr3:uid="{EA69CEA6-E76B-D949-9578-347B7A74E10D}" name="RegularExpression" dataDxfId="237"/>
+    <tableColumn id="10" xr3:uid="{D3A49B2C-58F9-B842-9608-581A999364E4}" name="HintText" dataDxfId="236"/>
+    <tableColumn id="11" xr3:uid="{CC47353C-D501-AA41-8CF6-3B49859BA97A}" name="SecurityClassification" dataDxfId="235"/>
+    <tableColumn id="12" xr3:uid="{6EBA010E-76A9-2946-B1FA-052FBF58B238}" name="Min" dataDxfId="234"/>
+    <tableColumn id="13" xr3:uid="{60640AE7-10CC-AB4C-B4E8-13C947D3CC74}" name="Max" dataDxfId="233"/>
+    <tableColumn id="15" xr3:uid="{C2DEBC92-657F-8B48-AEF6-35F078A0DDF4}" name="DisplayContextParameter" dataDxfId="232"/>
+    <tableColumn id="16" xr3:uid="{1D93B227-456B-3E42-85B4-0F278B7523D8}" name="Column2" dataDxfId="231"/>
+    <tableColumn id="17" xr3:uid="{F79DC235-9922-6D4E-9889-C653A521E8AE}" name="Column3" dataDxfId="230"/>
+    <tableColumn id="18" xr3:uid="{F1215911-B6F6-C345-9EC6-179495CC62C1}" name="Column4" dataDxfId="229"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7776E297-B7F9-FE43-8EE1-4BFB68FF9F3F}" name="Table6" displayName="Table6" ref="A3:G41" totalsRowShown="0" headerRowDxfId="227" dataDxfId="225" headerRowBorderDxfId="226" tableBorderDxfId="224" totalsRowBorderDxfId="223" headerRowCellStyle="Normal 2 3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7776E297-B7F9-FE43-8EE1-4BFB68FF9F3F}" name="Table6" displayName="Table6" ref="A3:G41" totalsRowShown="0" headerRowDxfId="228" dataDxfId="226" headerRowBorderDxfId="227" tableBorderDxfId="225" totalsRowBorderDxfId="224" headerRowCellStyle="Normal 2 3">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{10086A25-442C-7449-826A-B35FDEA13C5A}" name="LiveFrom" dataDxfId="222"/>
-    <tableColumn id="2" xr3:uid="{FB00A34E-44D3-2D4F-B5A8-96DA629491A0}" name="LiveTo" dataDxfId="221"/>
-    <tableColumn id="3" xr3:uid="{57331FEC-6C64-FF4E-AA60-883707FE9499}" name="CaseTypeID" dataDxfId="220"/>
-    <tableColumn id="4" xr3:uid="{88000BEA-50CE-2F4B-AD0C-7BEACAD282A9}" name="CaseFieldID" dataDxfId="219"/>
-    <tableColumn id="5" xr3:uid="{221E5BAD-472B-5347-A0E1-E4EB0C802640}" name="ListElementCode" dataDxfId="218"/>
-    <tableColumn id="6" xr3:uid="{B9EB3CC1-0BFB-F14D-AC9C-52AE589CD01A}" name="UserRole" dataDxfId="217"/>
-    <tableColumn id="7" xr3:uid="{777EED2E-8C44-2049-B5F3-F79010FCB8B9}" name="CRUD" dataDxfId="216"/>
+    <tableColumn id="1" xr3:uid="{10086A25-442C-7449-826A-B35FDEA13C5A}" name="LiveFrom" dataDxfId="223"/>
+    <tableColumn id="2" xr3:uid="{FB00A34E-44D3-2D4F-B5A8-96DA629491A0}" name="LiveTo" dataDxfId="222"/>
+    <tableColumn id="3" xr3:uid="{57331FEC-6C64-FF4E-AA60-883707FE9499}" name="CaseTypeID" dataDxfId="221"/>
+    <tableColumn id="4" xr3:uid="{88000BEA-50CE-2F4B-AD0C-7BEACAD282A9}" name="CaseFieldID" dataDxfId="220"/>
+    <tableColumn id="5" xr3:uid="{221E5BAD-472B-5347-A0E1-E4EB0C802640}" name="ListElementCode" dataDxfId="219"/>
+    <tableColumn id="6" xr3:uid="{B9EB3CC1-0BFB-F14D-AC9C-52AE589CD01A}" name="UserRole" dataDxfId="218"/>
+    <tableColumn id="7" xr3:uid="{777EED2E-8C44-2049-B5F3-F79010FCB8B9}" name="CRUD" dataDxfId="217"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{3217A593-E48A-BB42-A2D0-9D3131CA3F9C}" name="Table23" displayName="Table23" ref="A3:K42" totalsRowShown="0" headerRowDxfId="215" dataDxfId="213" headerRowBorderDxfId="214" tableBorderDxfId="212" totalsRowBorderDxfId="211">
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{CDA5C744-4A48-0C44-9DDE-72388C860C99}" name="LiveFrom" dataDxfId="210"/>
-    <tableColumn id="2" xr3:uid="{8A3CAE25-78FA-AC45-B741-FC9B0207A6D2}" name="LiveTo" dataDxfId="209"/>
-    <tableColumn id="3" xr3:uid="{E48B42B4-FF8F-E247-B69B-452FB019B56A}" name="ID" dataDxfId="208"/>
-    <tableColumn id="4" xr3:uid="{10CD4350-B2F2-C548-B931-D6CE2C4B3E79}" name="CaseEventID" dataDxfId="207"/>
-    <tableColumn id="5" xr3:uid="{E3E6155A-EA92-DF46-8888-ED7D749B974B}" name="CaseFieldId" dataDxfId="206"/>
-    <tableColumn id="6" xr3:uid="{09371456-1EA3-1E4E-A5BB-2B5AA70A6515}" name="ListElementCode" dataDxfId="205"/>
-    <tableColumn id="7" xr3:uid="{4BB7C15A-9707-A84E-B400-8458D3F72D15}" name="EventElementLabel" dataDxfId="204"/>
-    <tableColumn id="8" xr3:uid="{CFDCFEAC-052F-4E4F-97AB-3DD41D189409}" name="EventHintText" dataDxfId="203"/>
-    <tableColumn id="9" xr3:uid="{27B7471F-FF90-7A47-8A9D-E9D960A6E136}" name="FieldDisplayOrder" dataDxfId="202"/>
-    <tableColumn id="10" xr3:uid="{E2F9B116-7625-3446-AC24-38AEC7DDE066}" name="DisplayContext" dataDxfId="201"/>
-    <tableColumn id="11" xr3:uid="{33B43FDA-A050-7949-85A2-D71C872415D1}" name="FieldShowCondition" dataDxfId="200"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{3217A593-E48A-BB42-A2D0-9D3131CA3F9C}" name="Table23" displayName="Table23" ref="A3:L56" totalsRowShown="0" headerRowDxfId="216" dataDxfId="214" headerRowBorderDxfId="215" tableBorderDxfId="213" totalsRowBorderDxfId="212">
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{CDA5C744-4A48-0C44-9DDE-72388C860C99}" name="LiveFrom" dataDxfId="211"/>
+    <tableColumn id="2" xr3:uid="{8A3CAE25-78FA-AC45-B741-FC9B0207A6D2}" name="LiveTo" dataDxfId="210"/>
+    <tableColumn id="3" xr3:uid="{E48B42B4-FF8F-E247-B69B-452FB019B56A}" name="ID" dataDxfId="209"/>
+    <tableColumn id="4" xr3:uid="{10CD4350-B2F2-C548-B931-D6CE2C4B3E79}" name="CaseEventID" dataDxfId="208"/>
+    <tableColumn id="5" xr3:uid="{E3E6155A-EA92-DF46-8888-ED7D749B974B}" name="CaseFieldId" dataDxfId="207"/>
+    <tableColumn id="6" xr3:uid="{09371456-1EA3-1E4E-A5BB-2B5AA70A6515}" name="ListElementCode" dataDxfId="206"/>
+    <tableColumn id="12" xr3:uid="{4E9EBE21-1E8A-8F42-8DBF-15D634A7D163}" name="DefaultValue" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{4BB7C15A-9707-A84E-B400-8458D3F72D15}" name="EventElementLabel" dataDxfId="205"/>
+    <tableColumn id="8" xr3:uid="{CFDCFEAC-052F-4E4F-97AB-3DD41D189409}" name="EventHintText" dataDxfId="204"/>
+    <tableColumn id="9" xr3:uid="{27B7471F-FF90-7A47-8A9D-E9D960A6E136}" name="FieldDisplayOrder" dataDxfId="203"/>
+    <tableColumn id="10" xr3:uid="{E2F9B116-7625-3446-AC24-38AEC7DDE066}" name="DisplayContext" dataDxfId="202"/>
+    <tableColumn id="11" xr3:uid="{33B43FDA-A050-7949-85A2-D71C872415D1}" name="FieldShowCondition" dataDxfId="201"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{261F291B-49E9-7A47-AB56-BF364E30DB6B}" name="Table7" displayName="Table7" ref="A3:G24" totalsRowShown="0" headerRowDxfId="199" dataDxfId="197" headerRowBorderDxfId="198" tableBorderDxfId="196" totalsRowBorderDxfId="195">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{261F291B-49E9-7A47-AB56-BF364E30DB6B}" name="Table7" displayName="Table7" ref="A3:G24" totalsRowShown="0" headerRowDxfId="200" dataDxfId="198" headerRowBorderDxfId="199" tableBorderDxfId="197" totalsRowBorderDxfId="196">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{0FE98DA5-8D77-8146-ABB3-BB35B0A6C8A0}" name="LiveFrom" dataDxfId="194"/>
-    <tableColumn id="2" xr3:uid="{40479094-15A4-7F47-89AA-CC3E78D030E7}" name="LiveTo" dataDxfId="193"/>
-    <tableColumn id="3" xr3:uid="{FC1F3A20-DA92-A542-8712-9F23DC888392}" name="ID" dataDxfId="192"/>
-    <tableColumn id="4" xr3:uid="{88A6995E-37E7-2D43-A83A-FB28F631182B}" name="ListElementCode" dataDxfId="191"/>
-    <tableColumn id="5" xr3:uid="{70D3C9B9-96C2-F543-AAC5-6A771FC842FB}" name="ListElement" dataDxfId="190"/>
-    <tableColumn id="8" xr3:uid="{59643B70-8EC4-EA40-A49D-8B57B783888C}" name="CategoryID" dataDxfId="189"/>
-    <tableColumn id="6" xr3:uid="{60021BAA-94DF-114C-B62A-D5D7CFD8AC66}" name="DisplayOrder" dataDxfId="188"/>
+    <tableColumn id="1" xr3:uid="{0FE98DA5-8D77-8146-ABB3-BB35B0A6C8A0}" name="LiveFrom" dataDxfId="195"/>
+    <tableColumn id="2" xr3:uid="{40479094-15A4-7F47-89AA-CC3E78D030E7}" name="LiveTo" dataDxfId="194"/>
+    <tableColumn id="3" xr3:uid="{FC1F3A20-DA92-A542-8712-9F23DC888392}" name="ID" dataDxfId="193"/>
+    <tableColumn id="4" xr3:uid="{88A6995E-37E7-2D43-A83A-FB28F631182B}" name="ListElementCode" dataDxfId="192"/>
+    <tableColumn id="5" xr3:uid="{70D3C9B9-96C2-F543-AAC5-6A771FC842FB}" name="ListElement" dataDxfId="191"/>
+    <tableColumn id="8" xr3:uid="{59643B70-8EC4-EA40-A49D-8B57B783888C}" name="CategoryID" dataDxfId="190"/>
+    <tableColumn id="6" xr3:uid="{60021BAA-94DF-114C-B62A-D5D7CFD8AC66}" name="DisplayOrder" dataDxfId="189"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B2671E45-89F4-0848-8638-A186A962D516}" name="Table8" displayName="Table8" ref="A3:L65" totalsRowShown="0" headerRowDxfId="187" dataDxfId="185" headerRowBorderDxfId="186" tableBorderDxfId="184" totalsRowBorderDxfId="183">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B2671E45-89F4-0848-8638-A186A962D516}" name="Table8" displayName="Table8" ref="A3:L65" totalsRowShown="0" headerRowDxfId="188" dataDxfId="186" headerRowBorderDxfId="187" tableBorderDxfId="185" totalsRowBorderDxfId="184">
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{0A3DAEEE-2CC5-0044-A886-149AE812BFAA}" name="LiveFrom" dataDxfId="182"/>
-    <tableColumn id="2" xr3:uid="{0034116A-2F06-744E-96DE-13C53D21D193}" name="LiveTo" dataDxfId="181"/>
-    <tableColumn id="3" xr3:uid="{4E6FF688-3BC6-B34A-92F8-7285F5956CC6}" name="CaseTypeID" dataDxfId="180"/>
-    <tableColumn id="4" xr3:uid="{09102647-DA84-5E49-88D5-212E4C82F684}" name="Channel" dataDxfId="179"/>
-    <tableColumn id="5" xr3:uid="{5162BADF-56AB-0642-B0E0-D4BFAB4F3A56}" name="TabID" dataDxfId="178"/>
-    <tableColumn id="6" xr3:uid="{0BF66D3F-8E5E-FD48-ADD9-C749E508C46F}" name="TabLabel" dataDxfId="177"/>
-    <tableColumn id="7" xr3:uid="{69F4B009-8625-BC4D-9C35-6ADA6C44F63C}" name="TabDisplayOrder" dataDxfId="176"/>
-    <tableColumn id="8" xr3:uid="{F3B4D28F-14B6-0B4F-B9D7-E418EC66FF7D}" name="CaseFieldID" dataDxfId="175"/>
-    <tableColumn id="9" xr3:uid="{D7540CEE-0139-244D-B0F6-61FB3BAFAB2E}" name="TabFieldDisplayOrder" dataDxfId="174"/>
-    <tableColumn id="10" xr3:uid="{F03848C6-8BF9-C045-BE97-D5A5B7B6AF7E}" name="FieldShowCondition" dataDxfId="173"/>
-    <tableColumn id="11" xr3:uid="{351643CD-F5C2-594D-B984-2BD6A557A2A6}" name="TabShowCondition" dataDxfId="172"/>
-    <tableColumn id="12" xr3:uid="{E5813993-7410-BE44-87B6-E432B935A456}" name="DisplayContextParameter" dataDxfId="171"/>
+    <tableColumn id="1" xr3:uid="{0A3DAEEE-2CC5-0044-A886-149AE812BFAA}" name="LiveFrom" dataDxfId="183"/>
+    <tableColumn id="2" xr3:uid="{0034116A-2F06-744E-96DE-13C53D21D193}" name="LiveTo" dataDxfId="182"/>
+    <tableColumn id="3" xr3:uid="{4E6FF688-3BC6-B34A-92F8-7285F5956CC6}" name="CaseTypeID" dataDxfId="181"/>
+    <tableColumn id="4" xr3:uid="{09102647-DA84-5E49-88D5-212E4C82F684}" name="Channel" dataDxfId="180"/>
+    <tableColumn id="5" xr3:uid="{5162BADF-56AB-0642-B0E0-D4BFAB4F3A56}" name="TabID" dataDxfId="179"/>
+    <tableColumn id="6" xr3:uid="{0BF66D3F-8E5E-FD48-ADD9-C749E508C46F}" name="TabLabel" dataDxfId="178"/>
+    <tableColumn id="7" xr3:uid="{69F4B009-8625-BC4D-9C35-6ADA6C44F63C}" name="TabDisplayOrder" dataDxfId="177"/>
+    <tableColumn id="8" xr3:uid="{F3B4D28F-14B6-0B4F-B9D7-E418EC66FF7D}" name="CaseFieldID" dataDxfId="176"/>
+    <tableColumn id="9" xr3:uid="{D7540CEE-0139-244D-B0F6-61FB3BAFAB2E}" name="TabFieldDisplayOrder" dataDxfId="175"/>
+    <tableColumn id="10" xr3:uid="{F03848C6-8BF9-C045-BE97-D5A5B7B6AF7E}" name="FieldShowCondition" dataDxfId="174"/>
+    <tableColumn id="11" xr3:uid="{351643CD-F5C2-594D-B984-2BD6A557A2A6}" name="TabShowCondition" dataDxfId="173"/>
+    <tableColumn id="12" xr3:uid="{E5813993-7410-BE44-87B6-E432B935A456}" name="DisplayContextParameter" dataDxfId="172"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -17635,8 +17719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q162"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A17" zoomScale="88" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33:D33"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="88" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -24788,7 +24872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
@@ -30705,7 +30789,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -32256,7 +32340,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F4" sqref="F4:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -32947,8 +33031,8 @@
   <dimension ref="A1:IO126"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
+      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -38700,7 +38784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R76"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A17" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A35" workbookViewId="0">
       <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
@@ -42128,10 +42212,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -42139,18 +42223,19 @@
     <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
     <col min="6" max="6" width="57.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" customWidth="1"/>
-    <col min="11" max="11" width="88.5" customWidth="1"/>
-    <col min="12" max="16384" width="11.5" style="19"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="88.5" customWidth="1"/>
+    <col min="13" max="16384" width="11.5" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.15">
       <c r="A1" s="242" t="s">
         <v>355</v>
       </c>
@@ -42167,19 +42252,20 @@
       <c r="F1" s="245" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="243" t="s">
+      <c r="G1" s="245"/>
+      <c r="H1" s="243" t="s">
         <v>356</v>
       </c>
-      <c r="H1" s="243" t="s">
+      <c r="I1" s="243" t="s">
         <v>357</v>
       </c>
-      <c r="I1" s="243" t="s">
+      <c r="J1" s="243" t="s">
         <v>358</v>
       </c>
-      <c r="J1" s="95"/>
-      <c r="K1" s="243"/>
-    </row>
-    <row r="2" spans="1:11" ht="122" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K1" s="95"/>
+      <c r="L1" s="243"/>
+    </row>
+    <row r="2" spans="1:12" ht="122" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="246"/>
       <c r="B2" s="246"/>
       <c r="C2" s="247" t="s">
@@ -42194,23 +42280,24 @@
       <c r="F2" s="246" t="s">
         <v>359</v>
       </c>
-      <c r="G2" s="246" t="s">
+      <c r="G2" s="246"/>
+      <c r="H2" s="246" t="s">
         <v>362</v>
       </c>
-      <c r="H2" s="246" t="s">
+      <c r="I2" s="246" t="s">
         <v>363</v>
       </c>
-      <c r="I2" s="248" t="s">
+      <c r="J2" s="248" t="s">
         <v>364</v>
       </c>
-      <c r="J2" s="248" t="s">
+      <c r="K2" s="248" t="s">
         <v>365</v>
       </c>
-      <c r="K2" s="249" t="s">
+      <c r="L2" s="249" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="254" t="s">
         <v>9</v>
       </c>
@@ -42230,22 +42317,25 @@
         <v>225</v>
       </c>
       <c r="G3" s="255" t="s">
+        <v>936</v>
+      </c>
+      <c r="H3" s="255" t="s">
         <v>369</v>
       </c>
-      <c r="H3" s="255" t="s">
+      <c r="I3" s="255" t="s">
         <v>370</v>
       </c>
-      <c r="I3" s="255" t="s">
+      <c r="J3" s="255" t="s">
         <v>371</v>
       </c>
-      <c r="J3" s="255" t="s">
+      <c r="K3" s="255" t="s">
         <v>372</v>
       </c>
-      <c r="K3" s="256" t="s">
+      <c r="L3" s="256" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="250">
         <v>43101</v>
       </c>
@@ -42262,17 +42352,18 @@
       <c r="F4" s="132" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="95"/>
+      <c r="G4" s="132"/>
       <c r="H4" s="95"/>
-      <c r="I4" s="95">
+      <c r="I4" s="95"/>
+      <c r="J4" s="95">
         <v>1</v>
       </c>
-      <c r="J4" s="132" t="s">
+      <c r="K4" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K4" s="78"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L4" s="78"/>
+    </row>
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="250">
         <v>43101</v>
       </c>
@@ -42289,17 +42380,18 @@
       <c r="F5" s="132" t="s">
         <v>311</v>
       </c>
-      <c r="G5" s="95"/>
+      <c r="G5" s="132"/>
       <c r="H5" s="95"/>
-      <c r="I5" s="95">
+      <c r="I5" s="95"/>
+      <c r="J5" s="95">
         <v>2</v>
       </c>
-      <c r="J5" s="132" t="s">
+      <c r="K5" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K5" s="78"/>
-    </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L5" s="78"/>
+    </row>
+    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="250">
         <v>43101</v>
       </c>
@@ -42316,17 +42408,18 @@
       <c r="F6" s="81" t="s">
         <v>315</v>
       </c>
-      <c r="G6" s="95"/>
+      <c r="G6" s="81"/>
       <c r="H6" s="95"/>
-      <c r="I6" s="95">
+      <c r="I6" s="95"/>
+      <c r="J6" s="95">
         <v>3</v>
       </c>
-      <c r="J6" s="132" t="s">
+      <c r="K6" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K6" s="78"/>
-    </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L6" s="78"/>
+    </row>
+    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="250">
         <v>43101</v>
       </c>
@@ -42343,17 +42436,18 @@
       <c r="F7" s="132" t="s">
         <v>341</v>
       </c>
-      <c r="G7" s="95"/>
+      <c r="G7" s="132"/>
       <c r="H7" s="95"/>
-      <c r="I7" s="95">
+      <c r="I7" s="95"/>
+      <c r="J7" s="95">
         <v>1</v>
       </c>
-      <c r="J7" s="132" t="s">
+      <c r="K7" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K7" s="78"/>
-    </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L7" s="78"/>
+    </row>
+    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="250">
         <v>43101</v>
       </c>
@@ -42370,17 +42464,18 @@
       <c r="F8" s="132" t="s">
         <v>344</v>
       </c>
-      <c r="G8" s="95"/>
+      <c r="G8" s="132"/>
       <c r="H8" s="95"/>
-      <c r="I8" s="95">
+      <c r="I8" s="95"/>
+      <c r="J8" s="95">
         <v>2</v>
       </c>
-      <c r="J8" s="132" t="s">
+      <c r="K8" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K8" s="78"/>
-    </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L8" s="78"/>
+    </row>
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="250">
         <v>43101</v>
       </c>
@@ -42399,15 +42494,16 @@
       </c>
       <c r="G9" s="95"/>
       <c r="H9" s="95"/>
-      <c r="I9" s="95">
+      <c r="I9" s="95"/>
+      <c r="J9" s="95">
         <v>2</v>
       </c>
-      <c r="J9" s="132" t="s">
+      <c r="K9" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K9" s="78"/>
-    </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L9" s="78"/>
+    </row>
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="250">
         <v>43101</v>
       </c>
@@ -42426,15 +42522,16 @@
       </c>
       <c r="G10" s="95"/>
       <c r="H10" s="95"/>
-      <c r="I10" s="95">
+      <c r="I10" s="95"/>
+      <c r="J10" s="95">
         <v>3</v>
       </c>
-      <c r="J10" s="132" t="s">
+      <c r="K10" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K10" s="78"/>
-    </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L10" s="78"/>
+    </row>
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="251">
         <v>43101</v>
       </c>
@@ -42453,15 +42550,16 @@
       </c>
       <c r="G11" s="98"/>
       <c r="H11" s="98"/>
-      <c r="I11" s="98">
+      <c r="I11" s="98"/>
+      <c r="J11" s="98">
         <v>5</v>
       </c>
-      <c r="J11" s="98" t="s">
+      <c r="K11" s="98" t="s">
         <v>375</v>
       </c>
-      <c r="K11" s="77"/>
-    </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L11" s="77"/>
+    </row>
+    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="251">
         <v>43101</v>
       </c>
@@ -42480,15 +42578,16 @@
       </c>
       <c r="G12" s="98"/>
       <c r="H12" s="98"/>
-      <c r="I12" s="98">
+      <c r="I12" s="98"/>
+      <c r="J12" s="98">
         <v>6</v>
       </c>
-      <c r="J12" s="132" t="s">
+      <c r="K12" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K12" s="77"/>
-    </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L12" s="77"/>
+    </row>
+    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="250">
         <v>43101</v>
       </c>
@@ -42505,17 +42604,18 @@
       <c r="F13" s="132" t="s">
         <v>342</v>
       </c>
-      <c r="G13" s="95"/>
+      <c r="G13" s="132"/>
       <c r="H13" s="95"/>
       <c r="I13" s="95"/>
-      <c r="J13" s="132" t="s">
+      <c r="J13" s="95"/>
+      <c r="K13" s="132" t="s">
         <v>375</v>
       </c>
-      <c r="K13" s="231" t="s">
+      <c r="L13" s="231" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="250">
         <v>43101</v>
       </c>
@@ -42532,19 +42632,20 @@
       <c r="F14" s="132" t="s">
         <v>377</v>
       </c>
-      <c r="G14" s="95"/>
+      <c r="G14" s="132"/>
       <c r="H14" s="95"/>
-      <c r="I14" s="95">
+      <c r="I14" s="95"/>
+      <c r="J14" s="95">
         <v>7</v>
       </c>
-      <c r="J14" s="132" t="s">
+      <c r="K14" s="132" t="s">
         <v>375</v>
       </c>
-      <c r="K14" s="231" t="s">
+      <c r="L14" s="231" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="250">
         <v>43101</v>
       </c>
@@ -42561,21 +42662,22 @@
       <c r="F15" s="132" t="s">
         <v>379</v>
       </c>
-      <c r="G15" s="132" t="s">
+      <c r="G15" s="132"/>
+      <c r="H15" s="132" t="s">
         <v>380</v>
       </c>
-      <c r="H15" s="132" t="s">
+      <c r="I15" s="132" t="s">
         <v>381</v>
       </c>
-      <c r="I15" s="95">
+      <c r="J15" s="95">
         <v>4</v>
       </c>
-      <c r="J15" s="132" t="s">
+      <c r="K15" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K15" s="231"/>
-    </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L15" s="231"/>
+    </row>
+    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="250">
         <v>43101</v>
       </c>
@@ -42592,17 +42694,18 @@
       <c r="F16" s="132" t="s">
         <v>382</v>
       </c>
-      <c r="G16" s="95"/>
+      <c r="G16" s="132"/>
       <c r="H16" s="95"/>
-      <c r="I16" s="95">
+      <c r="I16" s="95"/>
+      <c r="J16" s="95">
         <v>6</v>
       </c>
-      <c r="J16" s="132" t="s">
+      <c r="K16" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K16" s="78"/>
-    </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L16" s="78"/>
+    </row>
+    <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="250">
         <v>43101</v>
       </c>
@@ -42619,17 +42722,18 @@
       <c r="F17" s="132" t="s">
         <v>772</v>
       </c>
-      <c r="G17" s="95"/>
+      <c r="G17" s="132"/>
       <c r="H17" s="95"/>
-      <c r="I17" s="95">
+      <c r="I17" s="95"/>
+      <c r="J17" s="95">
         <v>6</v>
       </c>
-      <c r="J17" s="132" t="s">
+      <c r="K17" s="132" t="s">
         <v>375</v>
       </c>
-      <c r="K17" s="78"/>
-    </row>
-    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L17" s="78"/>
+    </row>
+    <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="250">
         <v>43101</v>
       </c>
@@ -42646,17 +42750,18 @@
       <c r="F18" s="132" t="s">
         <v>383</v>
       </c>
-      <c r="G18" s="95"/>
+      <c r="G18" s="132"/>
       <c r="H18" s="95"/>
-      <c r="I18" s="95">
+      <c r="I18" s="95"/>
+      <c r="J18" s="95">
         <v>5</v>
       </c>
-      <c r="J18" s="132" t="s">
+      <c r="K18" s="132" t="s">
         <v>375</v>
       </c>
-      <c r="K18" s="78"/>
-    </row>
-    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L18" s="78"/>
+    </row>
+    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="250">
         <v>43101</v>
       </c>
@@ -42673,19 +42778,20 @@
       <c r="F19" s="132" t="s">
         <v>384</v>
       </c>
-      <c r="G19" s="95"/>
+      <c r="G19" s="132"/>
       <c r="H19" s="95"/>
-      <c r="I19" s="95">
+      <c r="I19" s="95"/>
+      <c r="J19" s="95">
         <v>8</v>
       </c>
-      <c r="J19" s="132" t="s">
+      <c r="K19" s="132" t="s">
         <v>375</v>
       </c>
-      <c r="K19" s="231" t="s">
+      <c r="L19" s="231" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="250">
         <v>43101</v>
       </c>
@@ -42702,17 +42808,18 @@
       <c r="F20" s="132" t="s">
         <v>386</v>
       </c>
-      <c r="G20" s="95"/>
+      <c r="G20" s="132"/>
       <c r="H20" s="95"/>
       <c r="I20" s="95"/>
-      <c r="J20" s="132" t="s">
+      <c r="J20" s="95"/>
+      <c r="K20" s="132" t="s">
         <v>375</v>
       </c>
-      <c r="K20" s="231" t="s">
+      <c r="L20" s="231" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="344">
         <v>43101</v>
       </c>
@@ -42729,19 +42836,20 @@
       <c r="F21" s="357" t="s">
         <v>919</v>
       </c>
-      <c r="G21" s="345" t="s">
+      <c r="G21" s="357"/>
+      <c r="H21" s="345" t="s">
         <v>920</v>
       </c>
-      <c r="H21" s="345"/>
-      <c r="I21" s="345">
+      <c r="I21" s="345"/>
+      <c r="J21" s="345">
         <v>1</v>
       </c>
-      <c r="J21" s="357" t="s">
+      <c r="K21" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K21" s="358"/>
-    </row>
-    <row r="22" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L21" s="358"/>
+    </row>
+    <row r="22" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="344">
         <v>43101</v>
       </c>
@@ -42758,19 +42866,20 @@
       <c r="F22" s="357" t="s">
         <v>921</v>
       </c>
-      <c r="G22" s="357" t="s">
+      <c r="G22" s="357"/>
+      <c r="H22" s="357" t="s">
         <v>922</v>
       </c>
-      <c r="H22" s="345"/>
-      <c r="I22" s="345">
+      <c r="I22" s="345"/>
+      <c r="J22" s="345">
         <v>2</v>
       </c>
-      <c r="J22" s="357" t="s">
+      <c r="K22" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K22" s="358"/>
-    </row>
-    <row r="23" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L22" s="358"/>
+    </row>
+    <row r="23" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="344">
         <v>43101</v>
       </c>
@@ -42787,17 +42896,18 @@
       <c r="F23" s="357" t="s">
         <v>917</v>
       </c>
-      <c r="G23" s="345"/>
+      <c r="G23" s="357"/>
       <c r="H23" s="345"/>
-      <c r="I23" s="345">
+      <c r="I23" s="345"/>
+      <c r="J23" s="345">
         <v>3</v>
       </c>
-      <c r="J23" s="357" t="s">
+      <c r="K23" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K23" s="358"/>
-    </row>
-    <row r="24" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L23" s="358"/>
+    </row>
+    <row r="24" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="344">
         <v>43101</v>
       </c>
@@ -42814,17 +42924,18 @@
       <c r="F24" s="357" t="s">
         <v>918</v>
       </c>
-      <c r="G24" s="345"/>
+      <c r="G24" s="357"/>
       <c r="H24" s="345"/>
-      <c r="I24" s="345">
+      <c r="I24" s="345"/>
+      <c r="J24" s="345">
         <v>4</v>
       </c>
-      <c r="J24" s="357" t="s">
+      <c r="K24" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K24" s="358"/>
-    </row>
-    <row r="25" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L24" s="358"/>
+    </row>
+    <row r="25" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="344">
         <v>43101</v>
       </c>
@@ -42841,17 +42952,20 @@
       <c r="F25" s="357" t="s">
         <v>915</v>
       </c>
-      <c r="G25" s="345"/>
+      <c r="G25" s="357" t="s">
+        <v>687</v>
+      </c>
       <c r="H25" s="345"/>
-      <c r="I25" s="345">
+      <c r="I25" s="345"/>
+      <c r="J25" s="345">
         <v>5</v>
       </c>
-      <c r="J25" s="357" t="s">
+      <c r="K25" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K25" s="358"/>
-    </row>
-    <row r="26" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L25" s="358"/>
+    </row>
+    <row r="26" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="344">
         <v>43101</v>
       </c>
@@ -42868,17 +42982,18 @@
       <c r="F26" s="357" t="s">
         <v>916</v>
       </c>
-      <c r="G26" s="345"/>
+      <c r="G26" s="357"/>
       <c r="H26" s="345"/>
-      <c r="I26" s="345">
+      <c r="I26" s="345"/>
+      <c r="J26" s="345">
         <v>6</v>
       </c>
-      <c r="J26" s="357" t="s">
+      <c r="K26" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K26" s="358"/>
-    </row>
-    <row r="27" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L26" s="358"/>
+    </row>
+    <row r="27" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="344">
         <v>43101</v>
       </c>
@@ -42895,17 +43010,18 @@
       <c r="F27" s="357" t="s">
         <v>919</v>
       </c>
-      <c r="G27" s="345"/>
+      <c r="G27" s="357"/>
       <c r="H27" s="345"/>
-      <c r="I27" s="345">
+      <c r="I27" s="345"/>
+      <c r="J27" s="345">
         <v>1</v>
       </c>
-      <c r="J27" s="357" t="s">
+      <c r="K27" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K27" s="358"/>
-    </row>
-    <row r="28" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L27" s="358"/>
+    </row>
+    <row r="28" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="344">
         <v>43101</v>
       </c>
@@ -42923,16 +43039,17 @@
         <v>921</v>
       </c>
       <c r="G28" s="357"/>
-      <c r="H28" s="345"/>
-      <c r="I28" s="345">
+      <c r="H28" s="357"/>
+      <c r="I28" s="345"/>
+      <c r="J28" s="345">
         <v>2</v>
       </c>
-      <c r="J28" s="357" t="s">
+      <c r="K28" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K28" s="358"/>
-    </row>
-    <row r="29" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L28" s="358"/>
+    </row>
+    <row r="29" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="344">
         <v>43101</v>
       </c>
@@ -42949,17 +43066,18 @@
       <c r="F29" s="357" t="s">
         <v>917</v>
       </c>
-      <c r="G29" s="345"/>
+      <c r="G29" s="357"/>
       <c r="H29" s="345"/>
-      <c r="I29" s="345">
+      <c r="I29" s="345"/>
+      <c r="J29" s="345">
         <v>3</v>
       </c>
-      <c r="J29" s="357" t="s">
+      <c r="K29" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K29" s="358"/>
-    </row>
-    <row r="30" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L29" s="358"/>
+    </row>
+    <row r="30" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="344">
         <v>43101</v>
       </c>
@@ -42976,17 +43094,18 @@
       <c r="F30" s="357" t="s">
         <v>918</v>
       </c>
-      <c r="G30" s="345"/>
+      <c r="G30" s="357"/>
       <c r="H30" s="345"/>
-      <c r="I30" s="345">
+      <c r="I30" s="345"/>
+      <c r="J30" s="345">
         <v>4</v>
       </c>
-      <c r="J30" s="357" t="s">
+      <c r="K30" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K30" s="358"/>
-    </row>
-    <row r="31" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L30" s="358"/>
+    </row>
+    <row r="31" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="344">
         <v>43101</v>
       </c>
@@ -43003,17 +43122,20 @@
       <c r="F31" s="357" t="s">
         <v>915</v>
       </c>
-      <c r="G31" s="345"/>
+      <c r="G31" s="357" t="s">
+        <v>695</v>
+      </c>
       <c r="H31" s="345"/>
-      <c r="I31" s="345">
+      <c r="I31" s="345"/>
+      <c r="J31" s="345">
         <v>5</v>
       </c>
-      <c r="J31" s="357" t="s">
+      <c r="K31" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K31" s="358"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L31" s="358"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A32" s="344">
         <v>43101</v>
       </c>
@@ -43030,291 +43152,611 @@
       <c r="F32" s="357" t="s">
         <v>916</v>
       </c>
-      <c r="G32" s="345"/>
+      <c r="G32" s="357"/>
       <c r="H32" s="345"/>
-      <c r="I32" s="345">
+      <c r="I32" s="345"/>
+      <c r="J32" s="345">
         <v>6</v>
       </c>
-      <c r="J32" s="357" t="s">
+      <c r="K32" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K32" s="358"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A33" s="251">
+      <c r="L32" s="358"/>
+    </row>
+    <row r="33" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="413">
+        <v>43983</v>
+      </c>
+      <c r="B33" s="414"/>
+      <c r="C33" s="415"/>
+      <c r="D33" s="415" t="s">
+        <v>940</v>
+      </c>
+      <c r="E33" s="416" t="s">
+        <v>941</v>
+      </c>
+      <c r="F33" s="417" t="s">
+        <v>919</v>
+      </c>
+      <c r="G33" s="417"/>
+      <c r="H33" s="417"/>
+      <c r="I33" s="414"/>
+      <c r="J33" s="414"/>
+      <c r="K33" s="417"/>
+      <c r="L33" s="418"/>
+    </row>
+    <row r="34" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="413">
+        <v>43983</v>
+      </c>
+      <c r="B34" s="414"/>
+      <c r="C34" s="415"/>
+      <c r="D34" s="415" t="s">
+        <v>940</v>
+      </c>
+      <c r="E34" s="416" t="s">
+        <v>941</v>
+      </c>
+      <c r="F34" s="417" t="s">
+        <v>921</v>
+      </c>
+      <c r="G34" s="417"/>
+      <c r="H34" s="417"/>
+      <c r="I34" s="414"/>
+      <c r="J34" s="414"/>
+      <c r="K34" s="417"/>
+      <c r="L34" s="418"/>
+    </row>
+    <row r="35" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="413">
+        <v>43983</v>
+      </c>
+      <c r="B35" s="414"/>
+      <c r="C35" s="415"/>
+      <c r="D35" s="415" t="s">
+        <v>940</v>
+      </c>
+      <c r="E35" s="416" t="s">
+        <v>937</v>
+      </c>
+      <c r="F35" s="417" t="s">
+        <v>917</v>
+      </c>
+      <c r="G35" s="417"/>
+      <c r="H35" s="417"/>
+      <c r="I35" s="414"/>
+      <c r="J35" s="414"/>
+      <c r="K35" s="417"/>
+      <c r="L35" s="418"/>
+    </row>
+    <row r="36" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="413">
+        <v>43983</v>
+      </c>
+      <c r="B36" s="414"/>
+      <c r="C36" s="415"/>
+      <c r="D36" s="415" t="s">
+        <v>940</v>
+      </c>
+      <c r="E36" s="416" t="s">
+        <v>937</v>
+      </c>
+      <c r="F36" s="417" t="s">
+        <v>918</v>
+      </c>
+      <c r="G36" s="417"/>
+      <c r="H36" s="417"/>
+      <c r="I36" s="414"/>
+      <c r="J36" s="414"/>
+      <c r="K36" s="417"/>
+      <c r="L36" s="418"/>
+    </row>
+    <row r="37" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="413">
+        <v>43983</v>
+      </c>
+      <c r="B37" s="414"/>
+      <c r="C37" s="415"/>
+      <c r="D37" s="415" t="s">
+        <v>940</v>
+      </c>
+      <c r="E37" s="416" t="s">
+        <v>937</v>
+      </c>
+      <c r="F37" s="417" t="s">
+        <v>915</v>
+      </c>
+      <c r="G37" s="417"/>
+      <c r="H37" s="417"/>
+      <c r="I37" s="414"/>
+      <c r="J37" s="414"/>
+      <c r="K37" s="417"/>
+      <c r="L37" s="418"/>
+    </row>
+    <row r="38" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="413">
+        <v>43983</v>
+      </c>
+      <c r="B38" s="414"/>
+      <c r="C38" s="415"/>
+      <c r="D38" s="415" t="s">
+        <v>940</v>
+      </c>
+      <c r="E38" s="416" t="s">
+        <v>937</v>
+      </c>
+      <c r="F38" s="417" t="s">
+        <v>916</v>
+      </c>
+      <c r="G38" s="417"/>
+      <c r="H38" s="417"/>
+      <c r="I38" s="414"/>
+      <c r="J38" s="414"/>
+      <c r="K38" s="417"/>
+      <c r="L38" s="418"/>
+    </row>
+    <row r="39" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="413">
+        <v>43983</v>
+      </c>
+      <c r="B39" s="414"/>
+      <c r="C39" s="415"/>
+      <c r="D39" s="415" t="s">
+        <v>940</v>
+      </c>
+      <c r="E39" s="416" t="s">
+        <v>938</v>
+      </c>
+      <c r="F39" s="417" t="s">
+        <v>917</v>
+      </c>
+      <c r="G39" s="417"/>
+      <c r="H39" s="417"/>
+      <c r="I39" s="414"/>
+      <c r="J39" s="414"/>
+      <c r="K39" s="417"/>
+      <c r="L39" s="418"/>
+    </row>
+    <row r="40" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="413">
+        <v>43983</v>
+      </c>
+      <c r="B40" s="414"/>
+      <c r="C40" s="415"/>
+      <c r="D40" s="415" t="s">
+        <v>940</v>
+      </c>
+      <c r="E40" s="416" t="s">
+        <v>938</v>
+      </c>
+      <c r="F40" s="417" t="s">
+        <v>918</v>
+      </c>
+      <c r="G40" s="417"/>
+      <c r="H40" s="417"/>
+      <c r="I40" s="414"/>
+      <c r="J40" s="414"/>
+      <c r="K40" s="417"/>
+      <c r="L40" s="418"/>
+    </row>
+    <row r="41" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="413">
+        <v>43983</v>
+      </c>
+      <c r="B41" s="414"/>
+      <c r="C41" s="415"/>
+      <c r="D41" s="415" t="s">
+        <v>940</v>
+      </c>
+      <c r="E41" s="416" t="s">
+        <v>938</v>
+      </c>
+      <c r="F41" s="417" t="s">
+        <v>915</v>
+      </c>
+      <c r="G41" s="417"/>
+      <c r="H41" s="417"/>
+      <c r="I41" s="414"/>
+      <c r="J41" s="414"/>
+      <c r="K41" s="417"/>
+      <c r="L41" s="418"/>
+    </row>
+    <row r="42" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="413">
+        <v>43983</v>
+      </c>
+      <c r="B42" s="414"/>
+      <c r="C42" s="415"/>
+      <c r="D42" s="415" t="s">
+        <v>940</v>
+      </c>
+      <c r="E42" s="416" t="s">
+        <v>938</v>
+      </c>
+      <c r="F42" s="417" t="s">
+        <v>916</v>
+      </c>
+      <c r="G42" s="417"/>
+      <c r="H42" s="417"/>
+      <c r="I42" s="414"/>
+      <c r="J42" s="414"/>
+      <c r="K42" s="417"/>
+      <c r="L42" s="418"/>
+    </row>
+    <row r="43" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="413">
+        <v>43983</v>
+      </c>
+      <c r="B43" s="414"/>
+      <c r="C43" s="415"/>
+      <c r="D43" s="415" t="s">
+        <v>940</v>
+      </c>
+      <c r="E43" s="416" t="s">
+        <v>939</v>
+      </c>
+      <c r="F43" s="417" t="s">
+        <v>917</v>
+      </c>
+      <c r="G43" s="417"/>
+      <c r="H43" s="417"/>
+      <c r="I43" s="414"/>
+      <c r="J43" s="414"/>
+      <c r="K43" s="417"/>
+      <c r="L43" s="418"/>
+    </row>
+    <row r="44" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="413">
+        <v>43983</v>
+      </c>
+      <c r="B44" s="414"/>
+      <c r="C44" s="415"/>
+      <c r="D44" s="415" t="s">
+        <v>940</v>
+      </c>
+      <c r="E44" s="416" t="s">
+        <v>939</v>
+      </c>
+      <c r="F44" s="417" t="s">
+        <v>918</v>
+      </c>
+      <c r="G44" s="417"/>
+      <c r="H44" s="417"/>
+      <c r="I44" s="414"/>
+      <c r="J44" s="414"/>
+      <c r="K44" s="417"/>
+      <c r="L44" s="418"/>
+    </row>
+    <row r="45" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="413">
+        <v>43983</v>
+      </c>
+      <c r="B45" s="414"/>
+      <c r="C45" s="415"/>
+      <c r="D45" s="415" t="s">
+        <v>940</v>
+      </c>
+      <c r="E45" s="416" t="s">
+        <v>939</v>
+      </c>
+      <c r="F45" s="417" t="s">
+        <v>915</v>
+      </c>
+      <c r="G45" s="417"/>
+      <c r="H45" s="417"/>
+      <c r="I45" s="414"/>
+      <c r="J45" s="414"/>
+      <c r="K45" s="417"/>
+      <c r="L45" s="418"/>
+    </row>
+    <row r="46" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="413">
+        <v>43983</v>
+      </c>
+      <c r="B46" s="414"/>
+      <c r="C46" s="415"/>
+      <c r="D46" s="415" t="s">
+        <v>940</v>
+      </c>
+      <c r="E46" s="416" t="s">
+        <v>939</v>
+      </c>
+      <c r="F46" s="417" t="s">
+        <v>916</v>
+      </c>
+      <c r="G46" s="417"/>
+      <c r="H46" s="417"/>
+      <c r="I46" s="414"/>
+      <c r="J46" s="414"/>
+      <c r="K46" s="417"/>
+      <c r="L46" s="418"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A47" s="251">
         <v>43101</v>
       </c>
-      <c r="B33" s="98"/>
-      <c r="C33" s="98" t="s">
+      <c r="B47" s="98"/>
+      <c r="C47" s="98" t="s">
         <v>297</v>
       </c>
-      <c r="D33" s="132" t="s">
+      <c r="D47" s="132" t="s">
         <v>388</v>
       </c>
-      <c r="E33" s="132" t="s">
+      <c r="E47" s="132" t="s">
         <v>124</v>
       </c>
-      <c r="F33" s="132" t="s">
+      <c r="F47" s="132" t="s">
         <v>344</v>
       </c>
-      <c r="G33" s="98"/>
-      <c r="H33" s="98"/>
-      <c r="I33" s="98">
+      <c r="G47" s="132"/>
+      <c r="H47" s="98"/>
+      <c r="I47" s="98"/>
+      <c r="J47" s="98">
         <v>1</v>
       </c>
-      <c r="J33" s="132" t="s">
+      <c r="K47" s="132" t="s">
         <v>389</v>
       </c>
-      <c r="K33" s="231" t="s">
+      <c r="L47" s="231" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A34" s="251">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A48" s="251">
         <v>43101</v>
       </c>
-      <c r="B34" s="98"/>
-      <c r="C34" s="98" t="s">
+      <c r="B48" s="98"/>
+      <c r="C48" s="98" t="s">
         <v>297</v>
       </c>
-      <c r="D34" s="132" t="s">
+      <c r="D48" s="132" t="s">
         <v>388</v>
       </c>
-      <c r="E34" s="132" t="s">
+      <c r="E48" s="132" t="s">
         <v>124</v>
       </c>
-      <c r="F34" s="132" t="s">
+      <c r="F48" s="132" t="s">
         <v>341</v>
       </c>
-      <c r="G34" s="98"/>
-      <c r="H34" s="98"/>
-      <c r="I34" s="98">
+      <c r="G48" s="132"/>
+      <c r="H48" s="98"/>
+      <c r="I48" s="98"/>
+      <c r="J48" s="98">
         <v>1</v>
       </c>
-      <c r="J34" s="132" t="s">
+      <c r="K48" s="132" t="s">
         <v>375</v>
       </c>
-      <c r="K34" s="231" t="s">
+      <c r="L48" s="231" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A35" s="251">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A49" s="251">
         <v>43101</v>
       </c>
-      <c r="B35" s="98"/>
-      <c r="C35" s="79" t="s">
+      <c r="B49" s="98"/>
+      <c r="C49" s="79" t="s">
         <v>214</v>
       </c>
-      <c r="D35" s="82" t="s">
+      <c r="D49" s="82" t="s">
         <v>392</v>
       </c>
-      <c r="E35" s="96" t="s">
+      <c r="E49" s="96" t="s">
         <v>212</v>
       </c>
-      <c r="F35" s="132" t="s">
+      <c r="F49" s="132" t="s">
         <v>326</v>
       </c>
-      <c r="G35" s="98"/>
-      <c r="H35" s="98"/>
-      <c r="I35" s="98">
+      <c r="G49" s="132"/>
+      <c r="H49" s="98"/>
+      <c r="I49" s="98"/>
+      <c r="J49" s="98">
         <v>1</v>
       </c>
-      <c r="J35" s="132" t="s">
+      <c r="K49" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K35" s="77"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A36" s="251">
+      <c r="L49" s="77"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A50" s="251">
         <v>43101</v>
       </c>
-      <c r="B36" s="98"/>
-      <c r="C36" s="79" t="s">
+      <c r="B50" s="98"/>
+      <c r="C50" s="79" t="s">
         <v>214</v>
       </c>
-      <c r="D36" s="82" t="s">
+      <c r="D50" s="82" t="s">
         <v>392</v>
       </c>
-      <c r="E36" s="96" t="s">
+      <c r="E50" s="96" t="s">
         <v>212</v>
       </c>
-      <c r="F36" s="132" t="s">
+      <c r="F50" s="132" t="s">
         <v>328</v>
       </c>
-      <c r="G36" s="98"/>
-      <c r="H36" s="98"/>
-      <c r="I36" s="98">
+      <c r="G50" s="132"/>
+      <c r="H50" s="98"/>
+      <c r="I50" s="98"/>
+      <c r="J50" s="98">
         <v>1</v>
       </c>
-      <c r="J36" s="132" t="s">
+      <c r="K50" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K36" s="77"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A37" s="251">
+      <c r="L50" s="77"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A51" s="251">
         <v>43101</v>
       </c>
-      <c r="B37" s="98"/>
-      <c r="C37" s="82" t="s">
+      <c r="B51" s="98"/>
+      <c r="C51" s="82" t="s">
         <v>218</v>
       </c>
-      <c r="D37" s="82" t="s">
+      <c r="D51" s="82" t="s">
         <v>392</v>
       </c>
-      <c r="E37" s="96" t="s">
+      <c r="E51" s="96" t="s">
         <v>216</v>
       </c>
-      <c r="F37" s="132" t="s">
+      <c r="F51" s="132" t="s">
         <v>330</v>
       </c>
-      <c r="G37" s="98"/>
-      <c r="H37" s="98"/>
-      <c r="I37" s="98">
+      <c r="G51" s="132"/>
+      <c r="H51" s="98"/>
+      <c r="I51" s="98"/>
+      <c r="J51" s="98">
         <v>2</v>
       </c>
-      <c r="J37" s="132" t="s">
+      <c r="K51" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K37" s="77"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A38" s="251">
+      <c r="L51" s="77"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A52" s="251">
         <v>43101</v>
       </c>
-      <c r="B38" s="98"/>
-      <c r="C38" s="79" t="s">
+      <c r="B52" s="98"/>
+      <c r="C52" s="79" t="s">
         <v>214</v>
       </c>
-      <c r="D38" s="82" t="s">
+      <c r="D52" s="82" t="s">
         <v>393</v>
       </c>
-      <c r="E38" s="96" t="s">
+      <c r="E52" s="96" t="s">
         <v>212</v>
       </c>
-      <c r="F38" s="132" t="s">
+      <c r="F52" s="132" t="s">
         <v>326</v>
       </c>
-      <c r="G38" s="98"/>
-      <c r="H38" s="98"/>
-      <c r="I38" s="98">
+      <c r="G52" s="132"/>
+      <c r="H52" s="98"/>
+      <c r="I52" s="98"/>
+      <c r="J52" s="98">
         <v>1</v>
       </c>
-      <c r="J38" s="132" t="s">
+      <c r="K52" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K38" s="77"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A39" s="251">
+      <c r="L52" s="77"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A53" s="251">
         <v>43101</v>
       </c>
-      <c r="B39" s="98"/>
-      <c r="C39" s="79" t="s">
+      <c r="B53" s="98"/>
+      <c r="C53" s="79" t="s">
         <v>214</v>
       </c>
-      <c r="D39" s="82" t="s">
+      <c r="D53" s="82" t="s">
         <v>393</v>
       </c>
-      <c r="E39" s="96" t="s">
+      <c r="E53" s="96" t="s">
         <v>212</v>
       </c>
-      <c r="F39" s="132" t="s">
+      <c r="F53" s="132" t="s">
         <v>328</v>
       </c>
-      <c r="G39" s="98"/>
-      <c r="H39" s="98"/>
-      <c r="I39" s="98">
+      <c r="G53" s="132"/>
+      <c r="H53" s="98"/>
+      <c r="I53" s="98"/>
+      <c r="J53" s="98">
         <v>1</v>
       </c>
-      <c r="J39" s="132" t="s">
+      <c r="K53" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K39" s="77"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A40" s="251">
+      <c r="L53" s="77"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A54" s="251">
         <v>43101</v>
       </c>
-      <c r="B40" s="98"/>
-      <c r="C40" s="82" t="s">
+      <c r="B54" s="98"/>
+      <c r="C54" s="82" t="s">
         <v>218</v>
       </c>
-      <c r="D40" s="82" t="s">
+      <c r="D54" s="82" t="s">
         <v>393</v>
       </c>
-      <c r="E40" s="96" t="s">
+      <c r="E54" s="96" t="s">
         <v>216</v>
       </c>
-      <c r="F40" s="132" t="s">
+      <c r="F54" s="132" t="s">
         <v>330</v>
       </c>
-      <c r="G40" s="98"/>
-      <c r="H40" s="98"/>
-      <c r="I40" s="98">
+      <c r="G54" s="132"/>
+      <c r="H54" s="98"/>
+      <c r="I54" s="98"/>
+      <c r="J54" s="98">
         <v>2</v>
       </c>
-      <c r="J40" s="132" t="s">
+      <c r="K54" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K40" s="77"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A41" s="251">
+      <c r="L54" s="77"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A55" s="251">
         <v>43101</v>
       </c>
-      <c r="B41" s="98"/>
-      <c r="C41" s="79" t="s">
+      <c r="B55" s="98"/>
+      <c r="C55" s="79" t="s">
         <v>214</v>
       </c>
-      <c r="D41" s="82" t="s">
+      <c r="D55" s="82" t="s">
         <v>394</v>
       </c>
-      <c r="E41" s="96" t="s">
+      <c r="E55" s="96" t="s">
         <v>212</v>
       </c>
-      <c r="F41" s="132" t="s">
+      <c r="F55" s="132" t="s">
         <v>326</v>
       </c>
-      <c r="G41" s="98"/>
-      <c r="H41" s="98"/>
-      <c r="I41" s="98">
+      <c r="G55" s="132"/>
+      <c r="H55" s="98"/>
+      <c r="I55" s="98"/>
+      <c r="J55" s="98">
         <v>1</v>
       </c>
-      <c r="J41" s="132" t="s">
+      <c r="K55" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K41" s="77"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A42" s="252">
+      <c r="L55" s="77"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A56" s="252">
         <v>43101</v>
       </c>
-      <c r="B42" s="104"/>
-      <c r="C42" s="87" t="s">
+      <c r="B56" s="104"/>
+      <c r="C56" s="87" t="s">
         <v>214</v>
       </c>
-      <c r="D42" s="100" t="s">
+      <c r="D56" s="100" t="s">
         <v>394</v>
       </c>
-      <c r="E42" s="102" t="s">
+      <c r="E56" s="102" t="s">
         <v>212</v>
       </c>
-      <c r="F42" s="253" t="s">
+      <c r="F56" s="253" t="s">
         <v>328</v>
       </c>
-      <c r="G42" s="104"/>
-      <c r="H42" s="104"/>
-      <c r="I42" s="104">
+      <c r="G56" s="253"/>
+      <c r="H56" s="104"/>
+      <c r="I56" s="104"/>
+      <c r="J56" s="104">
         <v>1</v>
       </c>
-      <c r="J42" s="253" t="s">
+      <c r="K56" s="253" t="s">
         <v>374</v>
       </c>
-      <c r="K42" s="105"/>
+      <c r="L56" s="105"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="58" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Removed duplicate entry in AuthorisationCaseState
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Defninition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Defninition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olawaleolanrewaju/Documents/Git_MOJ/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CF6EB6-227B-234C-AE8E-F8B4C1F86A55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE789FE7-4C8E-A744-B4CC-9E6AD5B57713}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5659" uniqueCount="951">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5647" uniqueCount="950">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -2950,9 +2950,6 @@
   </si>
   <si>
     <t>setOrganisationsForCaseRoles</t>
-  </si>
-  <si>
-    <t>DD/01/YYYY</t>
   </si>
   <si>
     <t>SomeOrganisation</t>
@@ -12111,7 +12108,7 @@
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F33" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F32" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="4"/>
@@ -13429,8 +13426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D6" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -14307,8 +14304,8 @@
       <c r="L28" s="365"/>
     </row>
     <row r="29" spans="1:12" s="343" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="436" t="s">
-        <v>938</v>
+      <c r="A29" s="436">
+        <v>42736</v>
       </c>
       <c r="B29" s="437"/>
       <c r="C29" s="440" t="s">
@@ -14327,7 +14324,7 @@
         <v>1</v>
       </c>
       <c r="H29" s="415" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="I29" s="439">
         <v>1</v>
@@ -14337,8 +14334,8 @@
       <c r="L29" s="418"/>
     </row>
     <row r="30" spans="1:12" s="343" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="436" t="s">
-        <v>938</v>
+      <c r="A30" s="436">
+        <v>42736</v>
       </c>
       <c r="B30" s="437"/>
       <c r="C30" s="440" t="s">
@@ -14357,7 +14354,7 @@
         <v>2</v>
       </c>
       <c r="H30" s="415" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="I30" s="439">
         <v>1</v>
@@ -14367,8 +14364,8 @@
       <c r="L30" s="418"/>
     </row>
     <row r="31" spans="1:12" s="343" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="436" t="s">
-        <v>938</v>
+      <c r="A31" s="436">
+        <v>42736</v>
       </c>
       <c r="B31" s="437"/>
       <c r="C31" s="440" t="s">
@@ -14387,7 +14384,7 @@
         <v>2</v>
       </c>
       <c r="H31" s="415" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="I31" s="439">
         <v>2</v>
@@ -14397,8 +14394,8 @@
       <c r="L31" s="418"/>
     </row>
     <row r="32" spans="1:12" s="343" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="436" t="s">
-        <v>938</v>
+      <c r="A32" s="436">
+        <v>42736</v>
       </c>
       <c r="B32" s="437"/>
       <c r="C32" s="440" t="s">
@@ -14417,7 +14414,7 @@
         <v>2</v>
       </c>
       <c r="H32" s="415" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="I32" s="439">
         <v>3</v>
@@ -18011,10 +18008,10 @@
         <v>937</v>
       </c>
       <c r="E41" s="429" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="F41" s="430" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="G41" s="431">
         <v>1</v>
@@ -18064,8 +18061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q166"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A12" zoomScale="88" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="88" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -19432,8 +19429,8 @@
       <c r="Q34" s="365"/>
     </row>
     <row r="35" spans="1:17" s="343" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="436" t="s">
-        <v>938</v>
+      <c r="A35" s="436">
+        <v>42736</v>
       </c>
       <c r="B35" s="437"/>
       <c r="C35" s="415" t="s">
@@ -19443,7 +19440,7 @@
         <v>937</v>
       </c>
       <c r="E35" s="415" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="F35" s="438">
         <v>1</v>
@@ -19455,7 +19452,7 @@
         <v>597</v>
       </c>
       <c r="I35" s="415" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="J35" s="439">
         <v>1</v>
@@ -19471,8 +19468,8 @@
       <c r="Q35" s="418"/>
     </row>
     <row r="36" spans="1:17" s="343" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="436" t="s">
-        <v>938</v>
+      <c r="A36" s="436">
+        <v>42736</v>
       </c>
       <c r="B36" s="437"/>
       <c r="C36" s="415" t="s">
@@ -19482,7 +19479,7 @@
         <v>937</v>
       </c>
       <c r="E36" s="415" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F36" s="438">
         <v>1</v>
@@ -19494,7 +19491,7 @@
         <v>597</v>
       </c>
       <c r="I36" s="415" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="J36" s="439">
         <v>1</v>
@@ -19510,8 +19507,8 @@
       <c r="Q36" s="418"/>
     </row>
     <row r="37" spans="1:17" s="343" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="436" t="s">
-        <v>938</v>
+      <c r="A37" s="436">
+        <v>42736</v>
       </c>
       <c r="B37" s="437"/>
       <c r="C37" s="415" t="s">
@@ -19521,7 +19518,7 @@
         <v>937</v>
       </c>
       <c r="E37" s="415" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="F37" s="438">
         <v>1</v>
@@ -19533,7 +19530,7 @@
         <v>597</v>
       </c>
       <c r="I37" s="415" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="J37" s="439">
         <v>1</v>
@@ -19549,8 +19546,8 @@
       <c r="Q37" s="418"/>
     </row>
     <row r="38" spans="1:17" s="343" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="436" t="s">
-        <v>938</v>
+      <c r="A38" s="436">
+        <v>42736</v>
       </c>
       <c r="B38" s="437"/>
       <c r="C38" s="415" t="s">
@@ -19560,7 +19557,7 @@
         <v>937</v>
       </c>
       <c r="E38" s="415" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="F38" s="438">
         <v>1</v>
@@ -19572,7 +19569,7 @@
         <v>597</v>
       </c>
       <c r="I38" s="415" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="J38" s="439">
         <v>1</v>
@@ -25361,7 +25358,7 @@
         <v>884</v>
       </c>
       <c r="D51" s="441" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="E51" s="446" t="s">
         <v>919</v>
@@ -26138,7 +26135,7 @@
         <v>884</v>
       </c>
       <c r="D36" s="451" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="E36" s="452" t="s">
         <v>909</v>
@@ -26159,10 +26156,10 @@
         <v>884</v>
       </c>
       <c r="D37" s="451" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="E37" s="452" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="F37" s="453"/>
       <c r="G37" s="454">
@@ -26180,10 +26177,10 @@
         <v>884</v>
       </c>
       <c r="D38" s="451" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="E38" s="452" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="F38" s="453"/>
       <c r="G38" s="454">
@@ -26201,10 +26198,10 @@
         <v>884</v>
       </c>
       <c r="D39" s="451" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="E39" s="452" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="F39" s="453"/>
       <c r="G39" s="454">
@@ -27344,7 +27341,7 @@
         <v>884</v>
       </c>
       <c r="D53" s="451" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="E53" s="457" t="s">
         <v>919</v>
@@ -28528,7 +28525,7 @@
         <v>884</v>
       </c>
       <c r="D53" s="462" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="E53" s="463"/>
       <c r="F53" s="462" t="s">
@@ -28550,11 +28547,11 @@
         <v>884</v>
       </c>
       <c r="D54" s="462" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="E54" s="463"/>
       <c r="F54" s="462" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="G54" s="464">
         <v>2</v>
@@ -28572,11 +28569,11 @@
         <v>884</v>
       </c>
       <c r="D55" s="462" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="E55" s="463"/>
       <c r="F55" s="462" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="G55" s="464">
         <v>3</v>
@@ -28594,11 +28591,11 @@
         <v>884</v>
       </c>
       <c r="D56" s="462" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="E56" s="463"/>
       <c r="F56" s="462" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="G56" s="464">
         <v>4</v>
@@ -29910,7 +29907,7 @@
         <v>884</v>
       </c>
       <c r="D39" s="415" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="E39" s="422" t="s">
         <v>778</v>
@@ -29928,7 +29925,7 @@
         <v>884</v>
       </c>
       <c r="D40" s="415" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="E40" s="422" t="s">
         <v>778</v>
@@ -29946,7 +29943,7 @@
         <v>884</v>
       </c>
       <c r="D41" s="415" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="E41" s="422" t="s">
         <v>778</v>
@@ -29964,7 +29961,7 @@
         <v>884</v>
       </c>
       <c r="D42" s="415" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="E42" s="422" t="s">
         <v>778</v>
@@ -31578,7 +31575,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -31685,31 +31682,31 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="220" t="s">
+      <c r="A8" s="470" t="s">
         <v>924</v>
       </c>
-      <c r="B8" s="469" t="s">
+      <c r="B8" s="470" t="s">
+        <v>687</v>
+      </c>
+      <c r="C8" s="470" t="s">
+        <v>693</v>
+      </c>
+      <c r="D8" s="470" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="220" t="s">
+        <v>924</v>
+      </c>
+      <c r="B9" s="469" t="s">
         <v>695</v>
       </c>
-      <c r="C8" s="469" t="s">
+      <c r="C9" s="469" t="s">
         <v>696</v>
       </c>
-      <c r="D8" s="469" t="s">
+      <c r="D9" s="469" t="s">
         <v>697</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="470" t="s">
-        <v>924</v>
-      </c>
-      <c r="B9" s="470" t="s">
-        <v>687</v>
-      </c>
-      <c r="C9" s="470" t="s">
-        <v>693</v>
-      </c>
-      <c r="D9" s="470" t="s">
-        <v>694</v>
       </c>
     </row>
   </sheetData>
@@ -32564,10 +32561,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -32744,57 +32741,57 @@
         <v>339</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="419">
-        <v>42736</v>
-      </c>
-      <c r="B10" s="422"/>
-      <c r="C10" s="415" t="s">
-        <v>884</v>
-      </c>
-      <c r="D10" s="415" t="s">
-        <v>489</v>
-      </c>
-      <c r="E10" s="468" t="s">
+    <row r="10" spans="1:6" s="306" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="359">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="352"/>
+      <c r="C10" s="307" t="s">
+        <v>924</v>
+      </c>
+      <c r="D10" s="307" t="s">
+        <v>493</v>
+      </c>
+      <c r="E10" s="385" t="s">
         <v>778</v>
       </c>
-      <c r="F10" s="466" t="s">
+      <c r="F10" s="381" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="306" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="359">
-        <v>42736</v>
-      </c>
-      <c r="B11" s="352"/>
+      <c r="A11" s="300">
+        <v>42736</v>
+      </c>
+      <c r="B11" s="303"/>
       <c r="C11" s="307" t="s">
         <v>924</v>
       </c>
       <c r="D11" s="307" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="E11" s="385" t="s">
         <v>778</v>
       </c>
-      <c r="F11" s="381" t="s">
+      <c r="F11" s="308" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="306" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="300">
-        <v>42736</v>
-      </c>
-      <c r="B12" s="303"/>
-      <c r="C12" s="307" t="s">
-        <v>924</v>
-      </c>
-      <c r="D12" s="307" t="s">
+    <row r="12" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B12" s="95"/>
+      <c r="C12" s="79" t="s">
+        <v>885</v>
+      </c>
+      <c r="D12" s="76" t="s">
         <v>489</v>
       </c>
-      <c r="E12" s="385" t="s">
+      <c r="E12" s="148" t="s">
         <v>778</v>
       </c>
-      <c r="F12" s="308" t="s">
+      <c r="F12" s="129" t="s">
         <v>339</v>
       </c>
     </row>
@@ -32804,9 +32801,9 @@
       </c>
       <c r="B13" s="95"/>
       <c r="C13" s="79" t="s">
-        <v>885</v>
-      </c>
-      <c r="D13" s="76" t="s">
+        <v>886</v>
+      </c>
+      <c r="D13" s="96" t="s">
         <v>489</v>
       </c>
       <c r="E13" s="148" t="s">
@@ -32825,7 +32822,7 @@
         <v>886</v>
       </c>
       <c r="D14" s="96" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="E14" s="148" t="s">
         <v>778</v>
@@ -32843,7 +32840,7 @@
         <v>886</v>
       </c>
       <c r="D15" s="96" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="E15" s="148" t="s">
         <v>778</v>
@@ -32852,16 +32849,16 @@
         <v>339</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="74">
         <v>42736</v>
       </c>
       <c r="B16" s="95"/>
-      <c r="C16" s="79" t="s">
-        <v>886</v>
-      </c>
-      <c r="D16" s="96" t="s">
-        <v>497</v>
+      <c r="C16" s="76" t="s">
+        <v>887</v>
+      </c>
+      <c r="D16" s="76" t="s">
+        <v>489</v>
       </c>
       <c r="E16" s="148" t="s">
         <v>778</v>
@@ -32870,13 +32867,13 @@
         <v>339</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="74">
         <v>42736</v>
       </c>
       <c r="B17" s="95"/>
       <c r="C17" s="76" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="D17" s="76" t="s">
         <v>489</v>
@@ -32888,57 +32885,57 @@
         <v>339</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B18" s="95"/>
-      <c r="C18" s="76" t="s">
+    <row r="18" spans="1:6" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="80">
+        <v>42736</v>
+      </c>
+      <c r="B18" s="98"/>
+      <c r="C18" s="82" t="s">
         <v>888</v>
       </c>
-      <c r="D18" s="76" t="s">
-        <v>489</v>
+      <c r="D18" s="82" t="s">
+        <v>498</v>
       </c>
       <c r="E18" s="148" t="s">
         <v>778</v>
       </c>
-      <c r="F18" s="129" t="s">
+      <c r="F18" s="133" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="80">
-        <v>42736</v>
-      </c>
-      <c r="B19" s="98"/>
-      <c r="C19" s="82" t="s">
-        <v>888</v>
-      </c>
-      <c r="D19" s="82" t="s">
-        <v>498</v>
+      <c r="A19" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B19" s="95"/>
+      <c r="C19" s="76" t="s">
+        <v>890</v>
+      </c>
+      <c r="D19" s="76" t="s">
+        <v>489</v>
       </c>
       <c r="E19" s="148" t="s">
         <v>778</v>
       </c>
-      <c r="F19" s="133" t="s">
+      <c r="F19" s="129" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B20" s="95"/>
-      <c r="C20" s="76" t="s">
-        <v>890</v>
-      </c>
-      <c r="D20" s="76" t="s">
+      <c r="A20" s="80">
+        <v>42736</v>
+      </c>
+      <c r="B20" s="98"/>
+      <c r="C20" s="98" t="s">
+        <v>889</v>
+      </c>
+      <c r="D20" s="82" t="s">
         <v>489</v>
       </c>
       <c r="E20" s="148" t="s">
         <v>778</v>
       </c>
-      <c r="F20" s="129" t="s">
+      <c r="F20" s="133" t="s">
         <v>339</v>
       </c>
     </row>
@@ -32951,7 +32948,7 @@
         <v>889</v>
       </c>
       <c r="D21" s="82" t="s">
-        <v>489</v>
+        <v>500</v>
       </c>
       <c r="E21" s="148" t="s">
         <v>778</v>
@@ -32969,7 +32966,7 @@
         <v>889</v>
       </c>
       <c r="D22" s="82" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="E22" s="148" t="s">
         <v>778</v>
@@ -32983,11 +32980,11 @@
         <v>42736</v>
       </c>
       <c r="B23" s="98"/>
-      <c r="C23" s="98" t="s">
-        <v>889</v>
+      <c r="C23" s="79" t="s">
+        <v>891</v>
       </c>
       <c r="D23" s="82" t="s">
-        <v>502</v>
+        <v>489</v>
       </c>
       <c r="E23" s="148" t="s">
         <v>778</v>
@@ -33001,14 +32998,14 @@
         <v>42736</v>
       </c>
       <c r="B24" s="98"/>
-      <c r="C24" s="79" t="s">
-        <v>891</v>
+      <c r="C24" s="82" t="s">
+        <v>894</v>
       </c>
       <c r="D24" s="82" t="s">
         <v>489</v>
       </c>
-      <c r="E24" s="148" t="s">
-        <v>778</v>
+      <c r="E24" s="98" t="s">
+        <v>779</v>
       </c>
       <c r="F24" s="133" t="s">
         <v>339</v>
@@ -33023,7 +33020,7 @@
         <v>894</v>
       </c>
       <c r="D25" s="82" t="s">
-        <v>489</v>
+        <v>505</v>
       </c>
       <c r="E25" s="98" t="s">
         <v>779</v>
@@ -33032,7 +33029,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="80">
         <v>42736</v>
       </c>
@@ -33041,10 +33038,10 @@
         <v>894</v>
       </c>
       <c r="D26" s="82" t="s">
-        <v>505</v>
+        <v>489</v>
       </c>
       <c r="E26" s="98" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="F26" s="133" t="s">
         <v>339</v>
@@ -33059,7 +33056,7 @@
         <v>894</v>
       </c>
       <c r="D27" s="82" t="s">
-        <v>489</v>
+        <v>505</v>
       </c>
       <c r="E27" s="98" t="s">
         <v>780</v>
@@ -33068,39 +33065,39 @@
         <v>339</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="80">
         <v>42736</v>
       </c>
       <c r="B28" s="98"/>
-      <c r="C28" s="82" t="s">
-        <v>894</v>
-      </c>
-      <c r="D28" s="82" t="s">
-        <v>505</v>
-      </c>
-      <c r="E28" s="98" t="s">
-        <v>780</v>
+      <c r="C28" s="79" t="s">
+        <v>892</v>
+      </c>
+      <c r="D28" s="96" t="s">
+        <v>489</v>
+      </c>
+      <c r="E28" s="148" t="s">
+        <v>778</v>
       </c>
       <c r="F28" s="133" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="80">
-        <v>42736</v>
-      </c>
-      <c r="B29" s="98"/>
-      <c r="C29" s="79" t="s">
+      <c r="A29" s="85">
+        <v>42736</v>
+      </c>
+      <c r="B29" s="104"/>
+      <c r="C29" s="87" t="s">
         <v>892</v>
       </c>
-      <c r="D29" s="96" t="s">
-        <v>489</v>
-      </c>
-      <c r="E29" s="148" t="s">
+      <c r="D29" s="102" t="s">
+        <v>729</v>
+      </c>
+      <c r="E29" s="209" t="s">
         <v>778</v>
       </c>
-      <c r="F29" s="133" t="s">
+      <c r="F29" s="139" t="s">
         <v>339</v>
       </c>
     </row>
@@ -33108,12 +33105,12 @@
       <c r="A30" s="85">
         <v>42736</v>
       </c>
-      <c r="B30" s="104"/>
-      <c r="C30" s="87" t="s">
-        <v>892</v>
-      </c>
-      <c r="D30" s="102" t="s">
-        <v>729</v>
+      <c r="B30" s="83"/>
+      <c r="C30" s="310" t="s">
+        <v>893</v>
+      </c>
+      <c r="D30" s="312" t="s">
+        <v>830</v>
       </c>
       <c r="E30" s="209" t="s">
         <v>778</v>
@@ -33131,7 +33128,7 @@
         <v>893</v>
       </c>
       <c r="D31" s="312" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="E31" s="209" t="s">
         <v>778</v>
@@ -33144,35 +33141,17 @@
       <c r="A32" s="85">
         <v>42736</v>
       </c>
-      <c r="B32" s="83"/>
+      <c r="B32" s="86"/>
       <c r="C32" s="310" t="s">
         <v>893</v>
       </c>
       <c r="D32" s="312" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="E32" s="209" t="s">
         <v>778</v>
       </c>
       <c r="F32" s="139" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="85">
-        <v>42736</v>
-      </c>
-      <c r="B33" s="86"/>
-      <c r="C33" s="310" t="s">
-        <v>893</v>
-      </c>
-      <c r="D33" s="312" t="s">
-        <v>834</v>
-      </c>
-      <c r="E33" s="209" t="s">
-        <v>778</v>
-      </c>
-      <c r="F33" s="139" t="s">
         <v>339</v>
       </c>
     </row>
@@ -35596,10 +35575,10 @@
         <v>884</v>
       </c>
       <c r="D40" s="415" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="E40" s="415" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F40" s="417"/>
       <c r="G40" s="421" t="s">
@@ -35861,10 +35840,10 @@
         <v>884</v>
       </c>
       <c r="D41" s="415" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="E41" s="415" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="F41" s="417"/>
       <c r="G41" s="421" t="s">
@@ -36126,10 +36105,10 @@
         <v>884</v>
       </c>
       <c r="D42" s="415" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="E42" s="415" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="F42" s="417"/>
       <c r="G42" s="421" t="s">
@@ -36391,10 +36370,10 @@
         <v>884</v>
       </c>
       <c r="D43" s="415" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="E43" s="415" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="F43" s="417"/>
       <c r="G43" s="421" t="s">
@@ -44127,7 +44106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
@@ -45082,13 +45061,13 @@
       </c>
       <c r="B33" s="414"/>
       <c r="C33" s="415" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D33" s="415" t="s">
         <v>937</v>
       </c>
       <c r="E33" s="416" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="F33" s="417" t="s">
         <v>919</v>
@@ -45110,13 +45089,13 @@
       </c>
       <c r="B34" s="414"/>
       <c r="C34" s="415" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D34" s="415" t="s">
         <v>937</v>
       </c>
       <c r="E34" s="416" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="F34" s="417" t="s">
         <v>921</v>
@@ -45138,13 +45117,13 @@
       </c>
       <c r="B35" s="414"/>
       <c r="C35" s="415" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D35" s="415" t="s">
         <v>937</v>
       </c>
       <c r="E35" s="416" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F35" s="417" t="s">
         <v>917</v>
@@ -45166,13 +45145,13 @@
       </c>
       <c r="B36" s="414"/>
       <c r="C36" s="415" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D36" s="415" t="s">
         <v>937</v>
       </c>
       <c r="E36" s="416" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F36" s="417" t="s">
         <v>918</v>
@@ -45194,13 +45173,13 @@
       </c>
       <c r="B37" s="414"/>
       <c r="C37" s="415" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D37" s="415" t="s">
         <v>937</v>
       </c>
       <c r="E37" s="416" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F37" s="417" t="s">
         <v>915</v>
@@ -45224,13 +45203,13 @@
       </c>
       <c r="B38" s="414"/>
       <c r="C38" s="415" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D38" s="415" t="s">
         <v>937</v>
       </c>
       <c r="E38" s="416" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F38" s="417" t="s">
         <v>916</v>
@@ -45252,13 +45231,13 @@
       </c>
       <c r="B39" s="414"/>
       <c r="C39" s="415" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D39" s="415" t="s">
         <v>937</v>
       </c>
       <c r="E39" s="416" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="F39" s="417" t="s">
         <v>917</v>
@@ -45280,13 +45259,13 @@
       </c>
       <c r="B40" s="414"/>
       <c r="C40" s="415" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D40" s="415" t="s">
         <v>937</v>
       </c>
       <c r="E40" s="416" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="F40" s="417" t="s">
         <v>918</v>
@@ -45308,13 +45287,13 @@
       </c>
       <c r="B41" s="414"/>
       <c r="C41" s="415" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D41" s="415" t="s">
         <v>937</v>
       </c>
       <c r="E41" s="416" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="F41" s="417" t="s">
         <v>915</v>
@@ -45338,13 +45317,13 @@
       </c>
       <c r="B42" s="414"/>
       <c r="C42" s="415" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D42" s="415" t="s">
         <v>937</v>
       </c>
       <c r="E42" s="416" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="F42" s="417" t="s">
         <v>916</v>
@@ -45366,13 +45345,13 @@
       </c>
       <c r="B43" s="414"/>
       <c r="C43" s="415" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D43" s="415" t="s">
         <v>937</v>
       </c>
       <c r="E43" s="416" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="F43" s="417" t="s">
         <v>917</v>
@@ -45394,13 +45373,13 @@
       </c>
       <c r="B44" s="414"/>
       <c r="C44" s="415" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D44" s="415" t="s">
         <v>937</v>
       </c>
       <c r="E44" s="416" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="F44" s="417" t="s">
         <v>918</v>
@@ -45422,13 +45401,13 @@
       </c>
       <c r="B45" s="414"/>
       <c r="C45" s="415" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D45" s="415" t="s">
         <v>937</v>
       </c>
       <c r="E45" s="416" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="F45" s="417" t="s">
         <v>915</v>
@@ -45452,13 +45431,13 @@
       </c>
       <c r="B46" s="414"/>
       <c r="C46" s="415" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="D46" s="415" t="s">
         <v>937</v>
       </c>
       <c r="E46" s="416" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="F46" s="417" t="s">
         <v>916</v>

</xml_diff>

<commit_message>
Added COLLABORATOR case role
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Defninition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Defninition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olawaleolanrewaju/Documents/Git_MOJ/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE789FE7-4C8E-A744-B4CC-9E6AD5B57713}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7F0CFD-7AAC-2F40-8FBC-D315F467161B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5647" uniqueCount="950">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5647" uniqueCount="951">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -2986,6 +2986,9 @@
   </si>
   <si>
     <t>OrganisationCaseRoles</t>
+  </si>
+  <si>
+    <t>[COLLABORATOR]</t>
   </si>
 </sst>
 </file>
@@ -18061,7 +18064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q166"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="88" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A12" zoomScale="88" workbookViewId="0">
       <selection activeCell="A35" sqref="A35:A38"/>
     </sheetView>
   </sheetViews>
@@ -31575,7 +31578,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -44106,8 +44109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -45413,7 +45416,7 @@
         <v>915</v>
       </c>
       <c r="G45" s="417" t="s">
-        <v>701</v>
+        <v>950</v>
       </c>
       <c r="H45" s="417"/>
       <c r="I45" s="414"/>

</xml_diff>

<commit_message>
Converted excel spreadsheet to json
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Defninition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Defninition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafalkalita/dev/moj/ccd-api-test-automation-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olawaleolanrewaju/Documents/Git_MOJ/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67ED300F-7ABE-5744-A736-A6DFCA7FAC34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B45837E-13CA-AE47-9341-B0CD1C4AEF56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37300" yWindow="100" windowWidth="35220" windowHeight="18280" firstSheet="5" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" firstSheet="13" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5432" uniqueCount="936">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5443" uniqueCount="937">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -2944,6 +2944,9 @@
   </si>
   <si>
     <t>Policy Case Assigned Role</t>
+  </si>
+  <si>
+    <t>DefaultValue</t>
   </si>
 </sst>
 </file>
@@ -4674,7 +4677,48 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
     <cellStyle name="Normal 2 3" xfId="13" xr:uid="{983C50BB-8B6C-1941-95CA-614B186AEA1E}"/>
   </cellStyles>
-  <dxfs count="302">
+  <dxfs count="303">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
@@ -11618,372 +11662,373 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1F077F35-774C-E743-83C7-6E310AAD8337}" name="Table5" displayName="Table5" ref="A3:E4" totalsRowShown="0" headerRowDxfId="301" dataDxfId="299" headerRowBorderDxfId="300" tableBorderDxfId="298" totalsRowBorderDxfId="297">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1F077F35-774C-E743-83C7-6E310AAD8337}" name="Table5" displayName="Table5" ref="A3:E4" totalsRowShown="0" headerRowDxfId="302" dataDxfId="300" headerRowBorderDxfId="301" tableBorderDxfId="299" totalsRowBorderDxfId="298">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{46ECD1A9-127E-3F45-96EF-07D1A76637A0}" name="LiveFrom" dataDxfId="296"/>
-    <tableColumn id="2" xr3:uid="{13DE718E-2141-6449-B408-2893D5F825EE}" name="LiveTo" dataDxfId="295"/>
-    <tableColumn id="3" xr3:uid="{2B218C4E-E8AE-9640-AF62-1EB51790A676}" name="ID" dataDxfId="294"/>
-    <tableColumn id="4" xr3:uid="{3EF730D3-305C-8E4D-ADBC-A778C1C17A83}" name="Name" dataDxfId="293"/>
-    <tableColumn id="5" xr3:uid="{EB212619-E76B-834D-9639-6E70EF2B808C}" name="Description" dataDxfId="292"/>
+    <tableColumn id="1" xr3:uid="{46ECD1A9-127E-3F45-96EF-07D1A76637A0}" name="LiveFrom" dataDxfId="297"/>
+    <tableColumn id="2" xr3:uid="{13DE718E-2141-6449-B408-2893D5F825EE}" name="LiveTo" dataDxfId="296"/>
+    <tableColumn id="3" xr3:uid="{2B218C4E-E8AE-9640-AF62-1EB51790A676}" name="ID" dataDxfId="295"/>
+    <tableColumn id="4" xr3:uid="{3EF730D3-305C-8E4D-ADBC-A778C1C17A83}" name="Name" dataDxfId="294"/>
+    <tableColumn id="5" xr3:uid="{EB212619-E76B-834D-9639-6E70EF2B808C}" name="Description" dataDxfId="293"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4CFBCA8A-9EC2-9242-9BDE-961374475E58}" name="Table9" displayName="Table9" ref="A3:H27" totalsRowShown="0" headerRowDxfId="170" dataDxfId="168" headerRowBorderDxfId="169" tableBorderDxfId="167" totalsRowBorderDxfId="166">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4CFBCA8A-9EC2-9242-9BDE-961374475E58}" name="Table9" displayName="Table9" ref="A3:H27" totalsRowShown="0" headerRowDxfId="171" dataDxfId="169" headerRowBorderDxfId="170" tableBorderDxfId="168" totalsRowBorderDxfId="167">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{3A9C2213-3C87-B242-A50F-DAA873031CFD}" name="LiveFrom" dataDxfId="165"/>
-    <tableColumn id="2" xr3:uid="{4438559D-2DCB-194A-BFAA-A68A1596F0EA}" name="LiveTo" dataDxfId="164"/>
-    <tableColumn id="3" xr3:uid="{20BC5FF0-EE97-BA41-80E0-333D8430A55D}" name="CaseTypeID" dataDxfId="163"/>
-    <tableColumn id="4" xr3:uid="{660AAD23-D344-7148-A6CD-579BFC3B0553}" name="ID" dataDxfId="162"/>
-    <tableColumn id="5" xr3:uid="{0D9AC729-9189-6841-A6A5-90D572AE955C}" name="Name" dataDxfId="161"/>
-    <tableColumn id="6" xr3:uid="{FFD16467-336A-A547-B4D7-4F82B645BDFB}" name="Description" dataDxfId="160"/>
-    <tableColumn id="7" xr3:uid="{00DD245F-92BF-574F-AF05-7500BA8A31B1}" name="DisplayOrder" dataDxfId="159"/>
-    <tableColumn id="8" xr3:uid="{51D53217-2A1C-DA4C-BB84-EF7FA0AEE74E}" name="TitleDisplay" dataDxfId="158"/>
+    <tableColumn id="1" xr3:uid="{3A9C2213-3C87-B242-A50F-DAA873031CFD}" name="LiveFrom" dataDxfId="166"/>
+    <tableColumn id="2" xr3:uid="{4438559D-2DCB-194A-BFAA-A68A1596F0EA}" name="LiveTo" dataDxfId="165"/>
+    <tableColumn id="3" xr3:uid="{20BC5FF0-EE97-BA41-80E0-333D8430A55D}" name="CaseTypeID" dataDxfId="164"/>
+    <tableColumn id="4" xr3:uid="{660AAD23-D344-7148-A6CD-579BFC3B0553}" name="ID" dataDxfId="163"/>
+    <tableColumn id="5" xr3:uid="{0D9AC729-9189-6841-A6A5-90D572AE955C}" name="Name" dataDxfId="162"/>
+    <tableColumn id="6" xr3:uid="{FFD16467-336A-A547-B4D7-4F82B645BDFB}" name="Description" dataDxfId="161"/>
+    <tableColumn id="7" xr3:uid="{00DD245F-92BF-574F-AF05-7500BA8A31B1}" name="DisplayOrder" dataDxfId="160"/>
+    <tableColumn id="8" xr3:uid="{51D53217-2A1C-DA4C-BB84-EF7FA0AEE74E}" name="TitleDisplay" dataDxfId="159"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E477A732-1DEE-F046-8ECD-8D2F086ABA9E}" name="Table10" displayName="Table10" ref="A3:T38" totalsRowShown="0" headerRowDxfId="157" dataDxfId="155" headerRowBorderDxfId="156" tableBorderDxfId="154" totalsRowBorderDxfId="153">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E477A732-1DEE-F046-8ECD-8D2F086ABA9E}" name="Table10" displayName="Table10" ref="A3:T38" totalsRowShown="0" headerRowDxfId="158" dataDxfId="156" headerRowBorderDxfId="157" tableBorderDxfId="155" totalsRowBorderDxfId="154">
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{A9949271-C952-5B4E-BDD4-4AFFF2D8614D}" name="LiveFrom" dataDxfId="152"/>
-    <tableColumn id="2" xr3:uid="{D137D6E5-6C3F-A546-91A2-6E5E88E5BD8A}" name="LiveTo" dataDxfId="151"/>
-    <tableColumn id="3" xr3:uid="{3485553F-1201-FF40-807A-E908084BDCE3}" name="CaseTypeID" dataDxfId="150"/>
-    <tableColumn id="4" xr3:uid="{C3A27859-CA49-9344-834B-BF2BE2280BB4}" name="ID" dataDxfId="149"/>
-    <tableColumn id="5" xr3:uid="{72817C12-B46E-604D-AABA-E2DA5A7F4255}" name="Name" dataDxfId="148"/>
-    <tableColumn id="6" xr3:uid="{06145D1D-7832-CA4E-980E-F24369297133}" name="Description" dataDxfId="147"/>
-    <tableColumn id="7" xr3:uid="{C1DFBC7C-115D-3149-9402-7DEBAC2F59B0}" name="DisplayOrder" dataDxfId="146"/>
-    <tableColumn id="8" xr3:uid="{05E21023-6279-404D-8752-82C93B7DD0FC}" name="PreConditionState(s)" dataDxfId="145"/>
-    <tableColumn id="9" xr3:uid="{57F8432A-B070-BC4C-9AF1-0A4A5ECB36E6}" name="PostConditionState" dataDxfId="144"/>
-    <tableColumn id="10" xr3:uid="{21E5C290-DF7D-984C-AD84-C1D3B8F4424F}" name="CallBackURLAboutToStartEvent" dataDxfId="143" dataCellStyle="Hyperlink"/>
-    <tableColumn id="11" xr3:uid="{2C9FCA41-AF28-F544-8544-3684A2AD897E}" name="RetriesTimeoutAboutToStartEvent" dataDxfId="142"/>
-    <tableColumn id="12" xr3:uid="{D0331CD4-2EE6-504E-8F08-4697D43974EE}" name="CallBackURLAboutToSubmitEvent" dataDxfId="141"/>
-    <tableColumn id="13" xr3:uid="{B34611C8-3477-894C-92ED-CDE1252E012A}" name="RetriesTimeoutURLAboutToSubmitEvent" dataDxfId="140"/>
-    <tableColumn id="14" xr3:uid="{A562B2B1-BF10-184B-B111-9D18B99B33C6}" name="CallBackURLSubmittedEvent" dataDxfId="139"/>
-    <tableColumn id="15" xr3:uid="{D5665814-36D0-5248-A5BE-E38060DE9D83}" name="RetriesTimeoutURLSubmittedEvent" dataDxfId="138"/>
-    <tableColumn id="16" xr3:uid="{9616BB75-22E6-F24C-B873-522862AC1B37}" name="SecurityClassification" dataDxfId="137"/>
-    <tableColumn id="17" xr3:uid="{382FE088-0BCD-084F-9D03-25A08E5400C5}" name="ShowSummary" dataDxfId="136"/>
-    <tableColumn id="18" xr3:uid="{D488E70D-0F94-1F4D-96D4-756627B23921}" name="ShowEventNotes" dataDxfId="135"/>
-    <tableColumn id="19" xr3:uid="{E634F39B-A849-4841-8801-2AF4F6A4CB4E}" name="CanSaveDraft" dataDxfId="134"/>
-    <tableColumn id="20" xr3:uid="{AC1595BB-697C-6344-8AF3-1672794828BA}" name="EndButtonLabel" dataDxfId="133"/>
+    <tableColumn id="1" xr3:uid="{A9949271-C952-5B4E-BDD4-4AFFF2D8614D}" name="LiveFrom" dataDxfId="153"/>
+    <tableColumn id="2" xr3:uid="{D137D6E5-6C3F-A546-91A2-6E5E88E5BD8A}" name="LiveTo" dataDxfId="152"/>
+    <tableColumn id="3" xr3:uid="{3485553F-1201-FF40-807A-E908084BDCE3}" name="CaseTypeID" dataDxfId="151"/>
+    <tableColumn id="4" xr3:uid="{C3A27859-CA49-9344-834B-BF2BE2280BB4}" name="ID" dataDxfId="150"/>
+    <tableColumn id="5" xr3:uid="{72817C12-B46E-604D-AABA-E2DA5A7F4255}" name="Name" dataDxfId="149"/>
+    <tableColumn id="6" xr3:uid="{06145D1D-7832-CA4E-980E-F24369297133}" name="Description" dataDxfId="148"/>
+    <tableColumn id="7" xr3:uid="{C1DFBC7C-115D-3149-9402-7DEBAC2F59B0}" name="DisplayOrder" dataDxfId="147"/>
+    <tableColumn id="8" xr3:uid="{05E21023-6279-404D-8752-82C93B7DD0FC}" name="PreConditionState(s)" dataDxfId="146"/>
+    <tableColumn id="9" xr3:uid="{57F8432A-B070-BC4C-9AF1-0A4A5ECB36E6}" name="PostConditionState" dataDxfId="145"/>
+    <tableColumn id="10" xr3:uid="{21E5C290-DF7D-984C-AD84-C1D3B8F4424F}" name="CallBackURLAboutToStartEvent" dataDxfId="144" dataCellStyle="Hyperlink"/>
+    <tableColumn id="11" xr3:uid="{2C9FCA41-AF28-F544-8544-3684A2AD897E}" name="RetriesTimeoutAboutToStartEvent" dataDxfId="143"/>
+    <tableColumn id="12" xr3:uid="{D0331CD4-2EE6-504E-8F08-4697D43974EE}" name="CallBackURLAboutToSubmitEvent" dataDxfId="142"/>
+    <tableColumn id="13" xr3:uid="{B34611C8-3477-894C-92ED-CDE1252E012A}" name="RetriesTimeoutURLAboutToSubmitEvent" dataDxfId="141"/>
+    <tableColumn id="14" xr3:uid="{A562B2B1-BF10-184B-B111-9D18B99B33C6}" name="CallBackURLSubmittedEvent" dataDxfId="140"/>
+    <tableColumn id="15" xr3:uid="{D5665814-36D0-5248-A5BE-E38060DE9D83}" name="RetriesTimeoutURLSubmittedEvent" dataDxfId="139"/>
+    <tableColumn id="16" xr3:uid="{9616BB75-22E6-F24C-B873-522862AC1B37}" name="SecurityClassification" dataDxfId="138"/>
+    <tableColumn id="17" xr3:uid="{382FE088-0BCD-084F-9D03-25A08E5400C5}" name="ShowSummary" dataDxfId="137"/>
+    <tableColumn id="18" xr3:uid="{D488E70D-0F94-1F4D-96D4-756627B23921}" name="ShowEventNotes" dataDxfId="136"/>
+    <tableColumn id="19" xr3:uid="{E634F39B-A849-4841-8801-2AF4F6A4CB4E}" name="CanSaveDraft" dataDxfId="135"/>
+    <tableColumn id="20" xr3:uid="{AC1595BB-697C-6344-8AF3-1672794828BA}" name="EndButtonLabel" dataDxfId="134"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{3FE29A4D-B6F7-B846-B37F-DE13E60B0795}" name="Table11" displayName="Table11" ref="A3:Q152" totalsRowShown="0" headerRowDxfId="132" dataDxfId="130" headerRowBorderDxfId="131" tableBorderDxfId="129" totalsRowBorderDxfId="128">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{3FE29A4D-B6F7-B846-B37F-DE13E60B0795}" name="Table11" displayName="Table11" ref="A3:Q152" totalsRowShown="0" headerRowDxfId="133" dataDxfId="131" headerRowBorderDxfId="132" tableBorderDxfId="130" totalsRowBorderDxfId="129">
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{09247200-910B-D14F-B26E-C50BECE0CCDE}" name="LiveFrom" dataDxfId="127"/>
-    <tableColumn id="2" xr3:uid="{D786058E-A950-5447-A9D7-81AFC8311866}" name="LiveTo" dataDxfId="126"/>
-    <tableColumn id="3" xr3:uid="{AED0E002-7D37-FB41-AD15-A0C135BF7DB3}" name="CaseTypeID" dataDxfId="125"/>
-    <tableColumn id="4" xr3:uid="{C474B0B2-C3DD-C64D-9F85-849C309F4E8F}" name="CaseEventID" dataDxfId="124"/>
-    <tableColumn id="5" xr3:uid="{E022EAF9-1C59-A049-B2D0-18417D29991E}" name="CaseFieldID" dataDxfId="123"/>
-    <tableColumn id="6" xr3:uid="{BA15E598-8D72-9D46-AB77-B605C7E29638}" name="PageFieldDisplayOrder" dataDxfId="122"/>
-    <tableColumn id="7" xr3:uid="{29A321E2-396E-8048-9500-1781CBB8AF23}" name="DisplayContext" dataDxfId="121"/>
-    <tableColumn id="8" xr3:uid="{500AE31D-F96A-9B4B-A577-919C9F7EB527}" name="PageID" dataDxfId="120"/>
-    <tableColumn id="9" xr3:uid="{77251A7B-4C0C-C44D-98D1-9673C5AAF038}" name="PageLabel" dataDxfId="119"/>
-    <tableColumn id="10" xr3:uid="{C3731FA3-2CB9-F448-B34D-5174A743CFC8}" name="PageDisplayOrder" dataDxfId="118"/>
-    <tableColumn id="11" xr3:uid="{087C997E-1430-BA4E-BE31-C1E6F8A09FC4}" name="PageColumnNumber" dataDxfId="117"/>
-    <tableColumn id="12" xr3:uid="{5F8D1DCD-BFA6-5D41-9085-4E8392AFBA5C}" name="FieldShowCondition" dataDxfId="116"/>
-    <tableColumn id="13" xr3:uid="{60ABBC14-F21E-7149-B13C-78981EAAC5AD}" name="PageShowCondition" dataDxfId="115"/>
-    <tableColumn id="14" xr3:uid="{92F3BFA3-CAC9-2C47-B4B5-E5193838BFBF}" name="DisplayContextParameter" dataDxfId="114"/>
-    <tableColumn id="15" xr3:uid="{6E7E82A2-72B3-1E4A-BB83-8C87B685E5AC}" name="ShowSummaryChangeOption" dataDxfId="113"/>
-    <tableColumn id="16" xr3:uid="{11418AC4-C205-D945-A936-1A37779FB35F}" name="ShowSummaryContentOption" dataDxfId="112"/>
-    <tableColumn id="17" xr3:uid="{CB58B471-584C-5B49-865D-C3B523596273}" name="CallBackURLMidEvent" dataDxfId="111"/>
+    <tableColumn id="1" xr3:uid="{09247200-910B-D14F-B26E-C50BECE0CCDE}" name="LiveFrom" dataDxfId="128"/>
+    <tableColumn id="2" xr3:uid="{D786058E-A950-5447-A9D7-81AFC8311866}" name="LiveTo" dataDxfId="127"/>
+    <tableColumn id="3" xr3:uid="{AED0E002-7D37-FB41-AD15-A0C135BF7DB3}" name="CaseTypeID" dataDxfId="126"/>
+    <tableColumn id="4" xr3:uid="{C474B0B2-C3DD-C64D-9F85-849C309F4E8F}" name="CaseEventID" dataDxfId="125"/>
+    <tableColumn id="5" xr3:uid="{E022EAF9-1C59-A049-B2D0-18417D29991E}" name="CaseFieldID" dataDxfId="124"/>
+    <tableColumn id="6" xr3:uid="{BA15E598-8D72-9D46-AB77-B605C7E29638}" name="PageFieldDisplayOrder" dataDxfId="123"/>
+    <tableColumn id="7" xr3:uid="{29A321E2-396E-8048-9500-1781CBB8AF23}" name="DisplayContext" dataDxfId="122"/>
+    <tableColumn id="8" xr3:uid="{500AE31D-F96A-9B4B-A577-919C9F7EB527}" name="PageID" dataDxfId="121"/>
+    <tableColumn id="9" xr3:uid="{77251A7B-4C0C-C44D-98D1-9673C5AAF038}" name="PageLabel" dataDxfId="120"/>
+    <tableColumn id="10" xr3:uid="{C3731FA3-2CB9-F448-B34D-5174A743CFC8}" name="PageDisplayOrder" dataDxfId="119"/>
+    <tableColumn id="11" xr3:uid="{087C997E-1430-BA4E-BE31-C1E6F8A09FC4}" name="PageColumnNumber" dataDxfId="118"/>
+    <tableColumn id="12" xr3:uid="{5F8D1DCD-BFA6-5D41-9085-4E8392AFBA5C}" name="FieldShowCondition" dataDxfId="117"/>
+    <tableColumn id="13" xr3:uid="{60ABBC14-F21E-7149-B13C-78981EAAC5AD}" name="PageShowCondition" dataDxfId="116"/>
+    <tableColumn id="14" xr3:uid="{92F3BFA3-CAC9-2C47-B4B5-E5193838BFBF}" name="DisplayContextParameter" dataDxfId="115"/>
+    <tableColumn id="15" xr3:uid="{6E7E82A2-72B3-1E4A-BB83-8C87B685E5AC}" name="ShowSummaryChangeOption" dataDxfId="114"/>
+    <tableColumn id="16" xr3:uid="{11418AC4-C205-D945-A936-1A37779FB35F}" name="ShowSummaryContentOption" dataDxfId="113"/>
+    <tableColumn id="17" xr3:uid="{CB58B471-584C-5B49-865D-C3B523596273}" name="CallBackURLMidEvent" dataDxfId="112"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C0942DB8-64D6-184E-8B7E-425FFE75053F}" name="Table12" displayName="Table12" ref="A3:H46" totalsRowShown="0" headerRowDxfId="110" dataDxfId="108" headerRowBorderDxfId="109" tableBorderDxfId="107" totalsRowBorderDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C0942DB8-64D6-184E-8B7E-425FFE75053F}" name="Table12" displayName="Table12" ref="A3:H46" totalsRowShown="0" headerRowDxfId="111" dataDxfId="109" headerRowBorderDxfId="110" tableBorderDxfId="108" totalsRowBorderDxfId="107">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{D94535AC-AF6B-A346-9394-2AEC1726FFC2}" name="LiveFrom" dataDxfId="105"/>
-    <tableColumn id="2" xr3:uid="{C1E40171-ED97-924B-9092-45E6DCB4FBD8}" name="LiveTo" dataDxfId="104"/>
-    <tableColumn id="3" xr3:uid="{22DC41E1-CD9E-1242-8CBA-BC0A19E00355}" name="CaseTypeID" dataDxfId="103"/>
-    <tableColumn id="4" xr3:uid="{84C83114-BBD1-C244-AF58-8DD790788A0E}" name="CaseFieldID" dataDxfId="102"/>
-    <tableColumn id="5" xr3:uid="{0346AC0F-F0E3-154A-9634-D0AA66CA21FD}" name="ListElementCode" dataDxfId="101"/>
-    <tableColumn id="6" xr3:uid="{E6AADCBC-8243-9F41-B0DB-0BE53FC0C362}" name="Label" dataDxfId="100"/>
-    <tableColumn id="7" xr3:uid="{FCF69EEE-2E56-444B-86FC-7F66B3D6AC95}" name="DisplayOrder" dataDxfId="99"/>
-    <tableColumn id="8" xr3:uid="{35DCFF60-D0A8-B54E-82C5-A30ED8395060}" name="DisplayContextParameter" dataDxfId="98"/>
+    <tableColumn id="1" xr3:uid="{D94535AC-AF6B-A346-9394-2AEC1726FFC2}" name="LiveFrom" dataDxfId="106"/>
+    <tableColumn id="2" xr3:uid="{C1E40171-ED97-924B-9092-45E6DCB4FBD8}" name="LiveTo" dataDxfId="105"/>
+    <tableColumn id="3" xr3:uid="{22DC41E1-CD9E-1242-8CBA-BC0A19E00355}" name="CaseTypeID" dataDxfId="104"/>
+    <tableColumn id="4" xr3:uid="{84C83114-BBD1-C244-AF58-8DD790788A0E}" name="CaseFieldID" dataDxfId="103"/>
+    <tableColumn id="5" xr3:uid="{0346AC0F-F0E3-154A-9634-D0AA66CA21FD}" name="ListElementCode" dataDxfId="102"/>
+    <tableColumn id="6" xr3:uid="{E6AADCBC-8243-9F41-B0DB-0BE53FC0C362}" name="Label" dataDxfId="101"/>
+    <tableColumn id="7" xr3:uid="{FCF69EEE-2E56-444B-86FC-7F66B3D6AC95}" name="DisplayOrder" dataDxfId="100"/>
+    <tableColumn id="8" xr3:uid="{35DCFF60-D0A8-B54E-82C5-A30ED8395060}" name="DisplayContextParameter" dataDxfId="99"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E7EE5CF4-F848-A444-80DE-82691AE949C0}" name="Table14" displayName="Table14" ref="A3:G35" totalsRowShown="0" headerRowDxfId="97" dataDxfId="95" headerRowBorderDxfId="96" tableBorderDxfId="94" totalsRowBorderDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E7EE5CF4-F848-A444-80DE-82691AE949C0}" name="Table14" displayName="Table14" ref="A3:G35" totalsRowShown="0" headerRowDxfId="98" dataDxfId="96" headerRowBorderDxfId="97" tableBorderDxfId="95" totalsRowBorderDxfId="94">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3A97DD00-8341-8A41-A062-99688A018570}" name="LiveFrom" dataDxfId="92"/>
-    <tableColumn id="2" xr3:uid="{7F24098A-B78A-4D49-BA3A-C64496932992}" name="LiveTo" dataDxfId="91"/>
-    <tableColumn id="3" xr3:uid="{4CECB00E-A59E-564E-9219-37AD7AAD6CA5}" name="CaseTypeID" dataDxfId="90"/>
-    <tableColumn id="4" xr3:uid="{32CEDFFA-35E9-B14E-89B8-F141DF840E42}" name="CaseFieldID" dataDxfId="89"/>
-    <tableColumn id="5" xr3:uid="{8A24F22E-1F45-F74A-B5FB-62E38937CC1B}" name="Label" dataDxfId="88"/>
-    <tableColumn id="6" xr3:uid="{73036E3A-A2DE-6345-B66E-F08F294B3920}" name="ListElementCode" dataDxfId="87"/>
-    <tableColumn id="7" xr3:uid="{0835D7A8-697B-CC41-AD8F-1A04E56A255E}" name="DisplayOrder" dataDxfId="86"/>
+    <tableColumn id="1" xr3:uid="{3A97DD00-8341-8A41-A062-99688A018570}" name="LiveFrom" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{7F24098A-B78A-4D49-BA3A-C64496932992}" name="LiveTo" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{4CECB00E-A59E-564E-9219-37AD7AAD6CA5}" name="CaseTypeID" dataDxfId="91"/>
+    <tableColumn id="4" xr3:uid="{32CEDFFA-35E9-B14E-89B8-F141DF840E42}" name="CaseFieldID" dataDxfId="90"/>
+    <tableColumn id="5" xr3:uid="{8A24F22E-1F45-F74A-B5FB-62E38937CC1B}" name="Label" dataDxfId="89"/>
+    <tableColumn id="6" xr3:uid="{73036E3A-A2DE-6345-B66E-F08F294B3920}" name="ListElementCode" dataDxfId="88"/>
+    <tableColumn id="7" xr3:uid="{0835D7A8-697B-CC41-AD8F-1A04E56A255E}" name="DisplayOrder" dataDxfId="87"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{23DB5BED-2DD5-DE42-8EA2-592AC1696272}" name="Table15" displayName="Table15" ref="A3:H52" totalsRowShown="0" headerRowDxfId="85" dataDxfId="83" headerRowBorderDxfId="84" tableBorderDxfId="82" totalsRowBorderDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{23DB5BED-2DD5-DE42-8EA2-592AC1696272}" name="Table15" displayName="Table15" ref="A3:H52" totalsRowShown="0" headerRowDxfId="86" dataDxfId="84" headerRowBorderDxfId="85" tableBorderDxfId="83" totalsRowBorderDxfId="82">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{4FCEDBE0-A9B0-0441-86AD-C7E7E6374F81}" name="LiveFrom" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{56793764-D9BF-1745-BA2A-131F10197717}" name="LiveTo" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{7B736E9A-236E-E84D-AB00-D5119AE8FDF4}" name="CaseTypeID" dataDxfId="78"/>
-    <tableColumn id="4" xr3:uid="{B2C20176-DB0A-0249-981A-083B6720F21B}" name="CaseFieldID" dataDxfId="77"/>
-    <tableColumn id="5" xr3:uid="{CA39F3C7-9B7B-1540-8FA6-8FE5E75DB625}" name="ListElementCode" dataDxfId="76"/>
-    <tableColumn id="6" xr3:uid="{B86E7729-2A08-3346-89EB-D64286E6CEED}" name="Label" dataDxfId="75"/>
-    <tableColumn id="7" xr3:uid="{E92211C5-8284-6246-B2E2-BC654D7297A5}" name="DisplayOrder" dataDxfId="74"/>
-    <tableColumn id="8" xr3:uid="{23A34836-8CA8-D941-A339-02B719A12676}" name="DisplayContextParameter" dataDxfId="73"/>
+    <tableColumn id="1" xr3:uid="{4FCEDBE0-A9B0-0441-86AD-C7E7E6374F81}" name="LiveFrom" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{56793764-D9BF-1745-BA2A-131F10197717}" name="LiveTo" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{7B736E9A-236E-E84D-AB00-D5119AE8FDF4}" name="CaseTypeID" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{B2C20176-DB0A-0249-981A-083B6720F21B}" name="CaseFieldID" dataDxfId="78"/>
+    <tableColumn id="5" xr3:uid="{CA39F3C7-9B7B-1540-8FA6-8FE5E75DB625}" name="ListElementCode" dataDxfId="77"/>
+    <tableColumn id="6" xr3:uid="{B86E7729-2A08-3346-89EB-D64286E6CEED}" name="Label" dataDxfId="76"/>
+    <tableColumn id="7" xr3:uid="{E92211C5-8284-6246-B2E2-BC654D7297A5}" name="DisplayOrder" dataDxfId="75"/>
+    <tableColumn id="8" xr3:uid="{23A34836-8CA8-D941-A339-02B719A12676}" name="DisplayContextParameter" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{0CA40DD8-8152-3D46-8168-0AE0B6974BE8}" name="Table16" displayName="Table16" ref="A3:I52" totalsRowShown="0" headerRowDxfId="72" dataDxfId="70" headerRowBorderDxfId="71" tableBorderDxfId="69" totalsRowBorderDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{0CA40DD8-8152-3D46-8168-0AE0B6974BE8}" name="Table16" displayName="Table16" ref="A3:I52" totalsRowShown="0" headerRowDxfId="73" dataDxfId="71" headerRowBorderDxfId="72" tableBorderDxfId="70" totalsRowBorderDxfId="69">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{89FB5309-B489-D04A-A245-5D0966E24720}" name="LiveFrom" dataDxfId="67"/>
-    <tableColumn id="2" xr3:uid="{0FF183E8-34AA-1E40-9440-3AF75B9978C6}" name="LiveTo" dataDxfId="66"/>
-    <tableColumn id="3" xr3:uid="{3390D839-8BB1-154A-AE30-84D075D9116D}" name="CaseTypeID" dataDxfId="65"/>
-    <tableColumn id="4" xr3:uid="{35990B77-262E-AE45-8172-61C1076B15BA}" name="CaseFieldID" dataDxfId="64"/>
-    <tableColumn id="7" xr3:uid="{70CF7FE5-8C40-2744-A7FE-26E60C76A62F}" name="ListElementCode" dataDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{BB41D60A-EC82-9941-A7B0-EF6AA438629F}" name="Label" dataDxfId="62"/>
-    <tableColumn id="6" xr3:uid="{031B36DA-C870-5745-A2EF-349414540475}" name="DisplayOrder" dataDxfId="61"/>
-    <tableColumn id="8" xr3:uid="{D282B24B-D0FD-DA44-9FC3-F20196FBA42D}" name="ResultsOrdering" dataDxfId="60"/>
-    <tableColumn id="9" xr3:uid="{7023267C-7AEA-EA4A-B007-2A8D3955A354}" name="DisplayContextParameter" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{89FB5309-B489-D04A-A245-5D0966E24720}" name="LiveFrom" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{0FF183E8-34AA-1E40-9440-3AF75B9978C6}" name="LiveTo" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{3390D839-8BB1-154A-AE30-84D075D9116D}" name="CaseTypeID" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{35990B77-262E-AE45-8172-61C1076B15BA}" name="CaseFieldID" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{70CF7FE5-8C40-2744-A7FE-26E60C76A62F}" name="ListElementCode" dataDxfId="64"/>
+    <tableColumn id="5" xr3:uid="{BB41D60A-EC82-9941-A7B0-EF6AA438629F}" name="Label" dataDxfId="63"/>
+    <tableColumn id="6" xr3:uid="{031B36DA-C870-5745-A2EF-349414540475}" name="DisplayOrder" dataDxfId="62"/>
+    <tableColumn id="8" xr3:uid="{D282B24B-D0FD-DA44-9FC3-F20196FBA42D}" name="ResultsOrdering" dataDxfId="61"/>
+    <tableColumn id="9" xr3:uid="{7023267C-7AEA-EA4A-B007-2A8D3955A354}" name="DisplayContextParameter" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{68D1BADF-97D2-B54C-B71F-46D015D9E181}" name="Table17" displayName="Table17" ref="A3:F5" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55" totalsRowBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{68D1BADF-97D2-B54C-B71F-46D015D9E181}" name="Table17" displayName="Table17" ref="A3:F5" totalsRowShown="0" headerRowDxfId="59" dataDxfId="57" headerRowBorderDxfId="58" tableBorderDxfId="56" totalsRowBorderDxfId="55">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7E998E97-505C-684E-9311-941AC17D5757}" name="LiveFrom" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{374279D4-23E7-9049-A9CB-C1788CC30194}" name="LiveTo" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{ADDEDA3F-CF2C-6D47-BC79-E1E4F6B6FF9B}" name="UserIDAMId" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{5D5CFFD9-D505-374F-8608-56EFBB6781C4}" name="WorkBasketDefaultJurisdiction" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{B2DEADF8-CB97-CD4B-9539-A848AD58DF04}" name="WorkBasketDefaultCaseType" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{CCAA7475-CF17-FD4A-B27C-B26DE0267EB6}" name="WorkBasketDefaultState" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{7E998E97-505C-684E-9311-941AC17D5757}" name="LiveFrom" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{374279D4-23E7-9049-A9CB-C1788CC30194}" name="LiveTo" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{ADDEDA3F-CF2C-6D47-BC79-E1E4F6B6FF9B}" name="UserIDAMId" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{5D5CFFD9-D505-374F-8608-56EFBB6781C4}" name="WorkBasketDefaultJurisdiction" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{B2DEADF8-CB97-CD4B-9539-A848AD58DF04}" name="WorkBasketDefaultCaseType" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{CCAA7475-CF17-FD4A-B27C-B26DE0267EB6}" name="WorkBasketDefaultState" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E19" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{AA7F7860-6544-2644-BE2C-52011A59B49F}" name="Table18" displayName="Table18" ref="A3:E19" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D7EDF212-81C7-1F49-98C0-8F28E87DCE6C}" name="LiveFrom" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{36550BF7-0E65-0D45-9932-4D227DD7D5DE}" name="LiveTo" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{D8A5019D-CCD7-0844-A9A5-378A259F60E5}" name="CaseTypeID" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{592355E2-FBF9-0947-A50E-1100535FD79E}" name="UserRole" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{B020D27C-2BA7-4145-B517-CECBAD029F6A}" name="CRUD" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{D7EDF212-81C7-1F49-98C0-8F28E87DCE6C}" name="LiveFrom" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{36550BF7-0E65-0D45-9932-4D227DD7D5DE}" name="LiveTo" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{D8A5019D-CCD7-0844-A9A5-378A259F60E5}" name="CaseTypeID" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{592355E2-FBF9-0947-A50E-1100535FD79E}" name="UserRole" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{B020D27C-2BA7-4145-B517-CECBAD029F6A}" name="CRUD" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F126" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{BF60EFC9-06B0-AF4B-BF05-86C7AFDAB66D}" name="Table19" displayName="Table19" ref="A3:F126" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{72C60802-2E7D-F542-8A1C-F0E147FA4DCE}" name="LiveFrom" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{FC67D30A-2836-1743-B4FA-D61DEE5FAF0A}" name="LiveTo" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{DE9841E4-2385-6944-AC9E-2418EBE9C323}" name="CaseTypeID" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{129D8AD7-2252-2343-A6AC-C828E01663E8}" name="CaseFieldID" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{313DEE97-0F1D-EB44-AAA1-862E98AA51C6}" name="UserRole" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{ED6F0D67-5349-4C4E-8FFC-F133A2D34661}" name="CRUD" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{72C60802-2E7D-F542-8A1C-F0E147FA4DCE}" name="LiveFrom" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{FC67D30A-2836-1743-B4FA-D61DEE5FAF0A}" name="LiveTo" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{DE9841E4-2385-6944-AC9E-2418EBE9C323}" name="CaseTypeID" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{129D8AD7-2252-2343-A6AC-C828E01663E8}" name="CaseFieldID" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{313DEE97-0F1D-EB44-AAA1-862E98AA51C6}" name="UserRole" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{ED6F0D67-5349-4C4E-8FFC-F133A2D34661}" name="CRUD" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C2696846-A994-B14A-A929-B58A056832F8}" name="Table4" displayName="Table4" ref="A3:D4" totalsRowShown="0" headerRowDxfId="291" dataDxfId="289" headerRowBorderDxfId="290" tableBorderDxfId="288" totalsRowBorderDxfId="287">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C2696846-A994-B14A-A929-B58A056832F8}" name="Table4" displayName="Table4" ref="A3:D4" totalsRowShown="0" headerRowDxfId="292" dataDxfId="290" headerRowBorderDxfId="291" tableBorderDxfId="289" totalsRowBorderDxfId="288">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DAC385B5-3CA7-F54F-ABF5-8A0FB9739A81}" name="BannerEnabled" dataDxfId="286"/>
-    <tableColumn id="2" xr3:uid="{5063DD1E-29B3-9240-B104-B878A78A961D}" name="BannerDescription" dataDxfId="285"/>
-    <tableColumn id="3" xr3:uid="{1802650A-8968-8C49-94DD-3A508725B56E}" name="BannerUrlText" dataDxfId="284"/>
-    <tableColumn id="4" xr3:uid="{C2492B8E-6768-C945-9E6B-68B481B89F36}" name="BannerUrl" dataDxfId="283" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" xr3:uid="{DAC385B5-3CA7-F54F-ABF5-8A0FB9739A81}" name="BannerEnabled" dataDxfId="287"/>
+    <tableColumn id="2" xr3:uid="{5063DD1E-29B3-9240-B104-B878A78A961D}" name="BannerDescription" dataDxfId="286"/>
+    <tableColumn id="3" xr3:uid="{1802650A-8968-8C49-94DD-3A508725B56E}" name="BannerUrlText" dataDxfId="285"/>
+    <tableColumn id="4" xr3:uid="{C2492B8E-6768-C945-9E6B-68B481B89F36}" name="BannerUrl" dataDxfId="284" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{F689229C-DA57-CE47-9FAB-39CC9062D12E}" name="Table20" displayName="Table20" ref="A3:D7" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{F689229C-DA57-CE47-9FAB-39CC9062D12E}" name="Table20" displayName="Table20" ref="A3:D9" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="27" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{108C9CDA-76BA-EE4D-8549-5BED5EA603A6}" name="CaseTypeID" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{4C2ED72C-37EE-A14B-9BFE-577416753198}" name="ID" dataDxfId="22" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{A13E9F3C-9866-6844-97A2-CECF13410611}" name="Name" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{5010B2BB-616D-A946-8844-A944EB690018}" name="Description" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{108C9CDA-76BA-EE4D-8549-5BED5EA603A6}" name="CaseTypeID" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{4C2ED72C-37EE-A14B-9BFE-577416753198}" name="ID" dataDxfId="23" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{A13E9F3C-9866-6844-97A2-CECF13410611}" name="Name" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{5010B2BB-616D-A946-8844-A944EB690018}" name="Description" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F44" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F44" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{EE9F57B3-787C-C642-A2B0-1CB2CD584A64}" name="CaseTypeID" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{A6633300-114A-5846-B7B7-C57244A39F58}" name="CaseEventID" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{229CDFFE-02D8-6042-9F1C-B67EA1F30C09}" name="UserRole" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{872585F6-B038-2149-8440-E4F3A404C8A9}" name="CRUD" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{EE9F57B3-787C-C642-A2B0-1CB2CD584A64}" name="CaseTypeID" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{A6633300-114A-5846-B7B7-C57244A39F58}" name="CaseEventID" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{229CDFFE-02D8-6042-9F1C-B67EA1F30C09}" name="UserRole" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{872585F6-B038-2149-8440-E4F3A404C8A9}" name="CRUD" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F32" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F32" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{F6F18BFB-2335-8D4F-9DC5-89FC7FD3B64B}" name="CaseTypeID" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{EB11A8E2-8EA8-0B46-B3B3-103461A3AF54}" name="CaseStateID" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{1C1D63D9-6997-9E47-9725-BB01CA7FD1F3}" name="UserRole" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{82473FFF-1C61-B242-A091-BA139462FACF}" name="CRUD" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{F6F18BFB-2335-8D4F-9DC5-89FC7FD3B64B}" name="CaseTypeID" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{EB11A8E2-8EA8-0B46-B3B3-103461A3AF54}" name="CaseStateID" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{1C1D63D9-6997-9E47-9725-BB01CA7FD1F3}" name="UserRole" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{82473FFF-1C61-B242-A091-BA139462FACF}" name="CRUD" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40D0FC50-9439-5741-A23D-29ACBB37469B}" name="Table3" displayName="Table3" ref="A3:I17" totalsRowShown="0" headerRowDxfId="282" dataDxfId="280" headerRowBorderDxfId="281" tableBorderDxfId="279" totalsRowBorderDxfId="278">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40D0FC50-9439-5741-A23D-29ACBB37469B}" name="Table3" displayName="Table3" ref="A3:I17" totalsRowShown="0" headerRowDxfId="283" dataDxfId="281" headerRowBorderDxfId="282" tableBorderDxfId="280" totalsRowBorderDxfId="279">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D407453C-8672-E84F-A1D8-F563E678DC8E}" name="LiveFrom" dataDxfId="277"/>
-    <tableColumn id="2" xr3:uid="{14122774-0C33-6C4D-A9AB-91FA15DB8A2C}" name="LiveTo" dataDxfId="276"/>
-    <tableColumn id="3" xr3:uid="{CB71BBA2-34F1-C545-B80D-4FB0AC6ACAFF}" name="ID" dataDxfId="275"/>
-    <tableColumn id="4" xr3:uid="{2CFC219C-166E-B343-97B5-1158954E0D8F}" name="Name" dataDxfId="274"/>
-    <tableColumn id="5" xr3:uid="{5592454F-E93D-5A44-B0EC-7DBD0663FC3A}" name="Description" dataDxfId="273"/>
-    <tableColumn id="6" xr3:uid="{0DB64C3F-680C-9C46-96C5-C0C984291BE2}" name="JurisdictionID" dataDxfId="272"/>
-    <tableColumn id="7" xr3:uid="{3EF72FC4-7B2C-7D46-8B03-99FBCADE4E25}" name="PrintableDocumentsUrl" dataDxfId="271"/>
-    <tableColumn id="8" xr3:uid="{35352FF6-3E6C-7440-9592-B69B66487A2F}" name="RetriesTimeoutURLPrintEvent" dataDxfId="270"/>
-    <tableColumn id="9" xr3:uid="{1ACB6DB4-FECA-7B47-9847-0243E309AD6A}" name="SecurityClassification" dataDxfId="269"/>
+    <tableColumn id="1" xr3:uid="{D407453C-8672-E84F-A1D8-F563E678DC8E}" name="LiveFrom" dataDxfId="278"/>
+    <tableColumn id="2" xr3:uid="{14122774-0C33-6C4D-A9AB-91FA15DB8A2C}" name="LiveTo" dataDxfId="277"/>
+    <tableColumn id="3" xr3:uid="{CB71BBA2-34F1-C545-B80D-4FB0AC6ACAFF}" name="ID" dataDxfId="276"/>
+    <tableColumn id="4" xr3:uid="{2CFC219C-166E-B343-97B5-1158954E0D8F}" name="Name" dataDxfId="275"/>
+    <tableColumn id="5" xr3:uid="{5592454F-E93D-5A44-B0EC-7DBD0663FC3A}" name="Description" dataDxfId="274"/>
+    <tableColumn id="6" xr3:uid="{0DB64C3F-680C-9C46-96C5-C0C984291BE2}" name="JurisdictionID" dataDxfId="273"/>
+    <tableColumn id="7" xr3:uid="{3EF72FC4-7B2C-7D46-8B03-99FBCADE4E25}" name="PrintableDocumentsUrl" dataDxfId="272"/>
+    <tableColumn id="8" xr3:uid="{35352FF6-3E6C-7440-9592-B69B66487A2F}" name="RetriesTimeoutURLPrintEvent" dataDxfId="271"/>
+    <tableColumn id="9" xr3:uid="{1ACB6DB4-FECA-7B47-9847-0243E309AD6A}" name="SecurityClassification" dataDxfId="270"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7853914-D748-214F-AB78-CCB4D9972099}" name="Table1" displayName="Table1" ref="A3:M126" totalsRowShown="0" headerRowDxfId="268" dataDxfId="266" headerRowBorderDxfId="267" tableBorderDxfId="265" totalsRowBorderDxfId="264">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7853914-D748-214F-AB78-CCB4D9972099}" name="Table1" displayName="Table1" ref="A3:M126" totalsRowShown="0" headerRowDxfId="269" dataDxfId="267" headerRowBorderDxfId="268" tableBorderDxfId="266" totalsRowBorderDxfId="265">
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{E6FCE3E8-E7C3-7C45-8832-C5E6EBCF5AD5}" name="LiveFrom" dataDxfId="263"/>
-    <tableColumn id="2" xr3:uid="{CCAF30FC-5E10-F84C-B526-0674ECA9972F}" name="LiveTo" dataDxfId="262"/>
-    <tableColumn id="3" xr3:uid="{9C767F7C-E4A3-E840-9D9C-30A8E9D03DE5}" name="CaseTypeID" dataDxfId="261"/>
-    <tableColumn id="4" xr3:uid="{0094B065-3327-9942-8F35-B92CB893A599}" name="ID" dataDxfId="260"/>
-    <tableColumn id="5" xr3:uid="{4CDE5603-12E3-DC45-91B4-D3F9BD04951B}" name="Label" dataDxfId="259"/>
-    <tableColumn id="6" xr3:uid="{5191E0DF-A515-CB40-9BD8-A0244E4F8C57}" name="HintText" dataDxfId="258"/>
-    <tableColumn id="7" xr3:uid="{00561C5B-D5D1-DC47-8E78-49D3C85569ED}" name="FieldType" dataDxfId="257"/>
-    <tableColumn id="13" xr3:uid="{41692C06-7AD8-F04A-B809-308DF1149252}" name="CategoryID" dataDxfId="256"/>
-    <tableColumn id="8" xr3:uid="{10BF8A09-644E-FB4A-8572-93D527306174}" name="FieldTypeParameter" dataDxfId="255"/>
-    <tableColumn id="9" xr3:uid="{DBABBB37-2DCF-2241-AEE6-1F2042FDD321}" name="RegularExpression" dataDxfId="254"/>
-    <tableColumn id="10" xr3:uid="{04F14DFC-0A0D-ED4E-B6FF-D294F3DF9079}" name="SecurityClassification" dataDxfId="253"/>
-    <tableColumn id="11" xr3:uid="{715917FF-FEBF-B843-A600-2D124CAB48A3}" name="Min" dataDxfId="252"/>
-    <tableColumn id="12" xr3:uid="{5FE67360-F088-F14B-A346-DE81B164ECE4}" name="Max" dataDxfId="251"/>
+    <tableColumn id="1" xr3:uid="{E6FCE3E8-E7C3-7C45-8832-C5E6EBCF5AD5}" name="LiveFrom" dataDxfId="264"/>
+    <tableColumn id="2" xr3:uid="{CCAF30FC-5E10-F84C-B526-0674ECA9972F}" name="LiveTo" dataDxfId="263"/>
+    <tableColumn id="3" xr3:uid="{9C767F7C-E4A3-E840-9D9C-30A8E9D03DE5}" name="CaseTypeID" dataDxfId="262"/>
+    <tableColumn id="4" xr3:uid="{0094B065-3327-9942-8F35-B92CB893A599}" name="ID" dataDxfId="261"/>
+    <tableColumn id="5" xr3:uid="{4CDE5603-12E3-DC45-91B4-D3F9BD04951B}" name="Label" dataDxfId="260"/>
+    <tableColumn id="6" xr3:uid="{5191E0DF-A515-CB40-9BD8-A0244E4F8C57}" name="HintText" dataDxfId="259"/>
+    <tableColumn id="7" xr3:uid="{00561C5B-D5D1-DC47-8E78-49D3C85569ED}" name="FieldType" dataDxfId="258"/>
+    <tableColumn id="13" xr3:uid="{41692C06-7AD8-F04A-B809-308DF1149252}" name="CategoryID" dataDxfId="257"/>
+    <tableColumn id="8" xr3:uid="{10BF8A09-644E-FB4A-8572-93D527306174}" name="FieldTypeParameter" dataDxfId="256"/>
+    <tableColumn id="9" xr3:uid="{DBABBB37-2DCF-2241-AEE6-1F2042FDD321}" name="RegularExpression" dataDxfId="255"/>
+    <tableColumn id="10" xr3:uid="{04F14DFC-0A0D-ED4E-B6FF-D294F3DF9079}" name="SecurityClassification" dataDxfId="254"/>
+    <tableColumn id="11" xr3:uid="{715917FF-FEBF-B843-A600-2D124CAB48A3}" name="Min" dataDxfId="253"/>
+    <tableColumn id="12" xr3:uid="{5FE67360-F088-F14B-A346-DE81B164ECE4}" name="Max" dataDxfId="252"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74540BC8-D704-5047-98FB-694A477BC83D}" name="Table2" displayName="Table2" ref="A3:R76" totalsRowShown="0" headerRowDxfId="250" dataDxfId="248" headerRowBorderDxfId="249" tableBorderDxfId="247" totalsRowBorderDxfId="246">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74540BC8-D704-5047-98FB-694A477BC83D}" name="Table2" displayName="Table2" ref="A3:R76" totalsRowShown="0" headerRowDxfId="251" dataDxfId="249" headerRowBorderDxfId="250" tableBorderDxfId="248" totalsRowBorderDxfId="247">
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{069BCF45-09C7-1D4D-9D96-EA818F065192}" name="LiveFrom" dataDxfId="245"/>
-    <tableColumn id="2" xr3:uid="{3201B607-7572-A641-B166-02ABBDA29C68}" name="LiveTo" dataDxfId="244"/>
-    <tableColumn id="3" xr3:uid="{BF418433-54F7-784B-88CA-F18E9603844B}" name="ID" dataDxfId="243"/>
-    <tableColumn id="4" xr3:uid="{9C8DE998-5550-0640-B6C2-CB5427FC3A63}" name="ListElementCode" dataDxfId="242"/>
-    <tableColumn id="5" xr3:uid="{D21D6A37-98CD-4E4A-BCE8-9A25879A6E2D}" name="FieldType" dataDxfId="241"/>
-    <tableColumn id="14" xr3:uid="{0CA72D38-CCA8-E348-8398-3563015AFFB0}" name="CategoryID" dataDxfId="240"/>
-    <tableColumn id="6" xr3:uid="{4BAE99B3-6B76-CF47-810C-6E284FAC7C45}" name="FieldTypeParameter" dataDxfId="239"/>
-    <tableColumn id="7" xr3:uid="{4E74D643-6B67-0D46-9AB2-7DF2E1703511}" name="ElementLabel" dataDxfId="238"/>
-    <tableColumn id="8" xr3:uid="{C675650F-2935-D647-A61E-517A892F4378}" name="FieldShowCondition" dataDxfId="237"/>
-    <tableColumn id="9" xr3:uid="{EA69CEA6-E76B-D949-9578-347B7A74E10D}" name="RegularExpression" dataDxfId="236"/>
-    <tableColumn id="10" xr3:uid="{D3A49B2C-58F9-B842-9608-581A999364E4}" name="HintText" dataDxfId="235"/>
-    <tableColumn id="11" xr3:uid="{CC47353C-D501-AA41-8CF6-3B49859BA97A}" name="SecurityClassification" dataDxfId="234"/>
-    <tableColumn id="12" xr3:uid="{6EBA010E-76A9-2946-B1FA-052FBF58B238}" name="Min" dataDxfId="233"/>
-    <tableColumn id="13" xr3:uid="{60640AE7-10CC-AB4C-B4E8-13C947D3CC74}" name="Max" dataDxfId="232"/>
-    <tableColumn id="15" xr3:uid="{C2DEBC92-657F-8B48-AEF6-35F078A0DDF4}" name="DisplayContextParameter" dataDxfId="231"/>
-    <tableColumn id="16" xr3:uid="{1D93B227-456B-3E42-85B4-0F278B7523D8}" name="Column2" dataDxfId="230"/>
-    <tableColumn id="17" xr3:uid="{F79DC235-9922-6D4E-9889-C653A521E8AE}" name="Column3" dataDxfId="229"/>
-    <tableColumn id="18" xr3:uid="{F1215911-B6F6-C345-9EC6-179495CC62C1}" name="Column4" dataDxfId="228"/>
+    <tableColumn id="1" xr3:uid="{069BCF45-09C7-1D4D-9D96-EA818F065192}" name="LiveFrom" dataDxfId="246"/>
+    <tableColumn id="2" xr3:uid="{3201B607-7572-A641-B166-02ABBDA29C68}" name="LiveTo" dataDxfId="245"/>
+    <tableColumn id="3" xr3:uid="{BF418433-54F7-784B-88CA-F18E9603844B}" name="ID" dataDxfId="244"/>
+    <tableColumn id="4" xr3:uid="{9C8DE998-5550-0640-B6C2-CB5427FC3A63}" name="ListElementCode" dataDxfId="243"/>
+    <tableColumn id="5" xr3:uid="{D21D6A37-98CD-4E4A-BCE8-9A25879A6E2D}" name="FieldType" dataDxfId="242"/>
+    <tableColumn id="14" xr3:uid="{0CA72D38-CCA8-E348-8398-3563015AFFB0}" name="CategoryID" dataDxfId="241"/>
+    <tableColumn id="6" xr3:uid="{4BAE99B3-6B76-CF47-810C-6E284FAC7C45}" name="FieldTypeParameter" dataDxfId="240"/>
+    <tableColumn id="7" xr3:uid="{4E74D643-6B67-0D46-9AB2-7DF2E1703511}" name="ElementLabel" dataDxfId="239"/>
+    <tableColumn id="8" xr3:uid="{C675650F-2935-D647-A61E-517A892F4378}" name="FieldShowCondition" dataDxfId="238"/>
+    <tableColumn id="9" xr3:uid="{EA69CEA6-E76B-D949-9578-347B7A74E10D}" name="RegularExpression" dataDxfId="237"/>
+    <tableColumn id="10" xr3:uid="{D3A49B2C-58F9-B842-9608-581A999364E4}" name="HintText" dataDxfId="236"/>
+    <tableColumn id="11" xr3:uid="{CC47353C-D501-AA41-8CF6-3B49859BA97A}" name="SecurityClassification" dataDxfId="235"/>
+    <tableColumn id="12" xr3:uid="{6EBA010E-76A9-2946-B1FA-052FBF58B238}" name="Min" dataDxfId="234"/>
+    <tableColumn id="13" xr3:uid="{60640AE7-10CC-AB4C-B4E8-13C947D3CC74}" name="Max" dataDxfId="233"/>
+    <tableColumn id="15" xr3:uid="{C2DEBC92-657F-8B48-AEF6-35F078A0DDF4}" name="DisplayContextParameter" dataDxfId="232"/>
+    <tableColumn id="16" xr3:uid="{1D93B227-456B-3E42-85B4-0F278B7523D8}" name="Column2" dataDxfId="231"/>
+    <tableColumn id="17" xr3:uid="{F79DC235-9922-6D4E-9889-C653A521E8AE}" name="Column3" dataDxfId="230"/>
+    <tableColumn id="18" xr3:uid="{F1215911-B6F6-C345-9EC6-179495CC62C1}" name="Column4" dataDxfId="229"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7776E297-B7F9-FE43-8EE1-4BFB68FF9F3F}" name="Table6" displayName="Table6" ref="A3:G41" totalsRowShown="0" headerRowDxfId="227" dataDxfId="225" headerRowBorderDxfId="226" tableBorderDxfId="224" totalsRowBorderDxfId="223" headerRowCellStyle="Normal 2 3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7776E297-B7F9-FE43-8EE1-4BFB68FF9F3F}" name="Table6" displayName="Table6" ref="A3:G41" totalsRowShown="0" headerRowDxfId="228" dataDxfId="226" headerRowBorderDxfId="227" tableBorderDxfId="225" totalsRowBorderDxfId="224" headerRowCellStyle="Normal 2 3">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{10086A25-442C-7449-826A-B35FDEA13C5A}" name="LiveFrom" dataDxfId="222"/>
-    <tableColumn id="2" xr3:uid="{FB00A34E-44D3-2D4F-B5A8-96DA629491A0}" name="LiveTo" dataDxfId="221"/>
-    <tableColumn id="3" xr3:uid="{57331FEC-6C64-FF4E-AA60-883707FE9499}" name="CaseTypeID" dataDxfId="220"/>
-    <tableColumn id="4" xr3:uid="{88000BEA-50CE-2F4B-AD0C-7BEACAD282A9}" name="CaseFieldID" dataDxfId="219"/>
-    <tableColumn id="5" xr3:uid="{221E5BAD-472B-5347-A0E1-E4EB0C802640}" name="ListElementCode" dataDxfId="218"/>
-    <tableColumn id="6" xr3:uid="{B9EB3CC1-0BFB-F14D-AC9C-52AE589CD01A}" name="UserRole" dataDxfId="217"/>
-    <tableColumn id="7" xr3:uid="{777EED2E-8C44-2049-B5F3-F79010FCB8B9}" name="CRUD" dataDxfId="216"/>
+    <tableColumn id="1" xr3:uid="{10086A25-442C-7449-826A-B35FDEA13C5A}" name="LiveFrom" dataDxfId="223"/>
+    <tableColumn id="2" xr3:uid="{FB00A34E-44D3-2D4F-B5A8-96DA629491A0}" name="LiveTo" dataDxfId="222"/>
+    <tableColumn id="3" xr3:uid="{57331FEC-6C64-FF4E-AA60-883707FE9499}" name="CaseTypeID" dataDxfId="221"/>
+    <tableColumn id="4" xr3:uid="{88000BEA-50CE-2F4B-AD0C-7BEACAD282A9}" name="CaseFieldID" dataDxfId="220"/>
+    <tableColumn id="5" xr3:uid="{221E5BAD-472B-5347-A0E1-E4EB0C802640}" name="ListElementCode" dataDxfId="219"/>
+    <tableColumn id="6" xr3:uid="{B9EB3CC1-0BFB-F14D-AC9C-52AE589CD01A}" name="UserRole" dataDxfId="218"/>
+    <tableColumn id="7" xr3:uid="{777EED2E-8C44-2049-B5F3-F79010FCB8B9}" name="CRUD" dataDxfId="217"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{3217A593-E48A-BB42-A2D0-9D3131CA3F9C}" name="Table23" displayName="Table23" ref="A3:K42" totalsRowShown="0" headerRowDxfId="215" dataDxfId="213" headerRowBorderDxfId="214" tableBorderDxfId="212" totalsRowBorderDxfId="211">
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{CDA5C744-4A48-0C44-9DDE-72388C860C99}" name="LiveFrom" dataDxfId="210"/>
-    <tableColumn id="2" xr3:uid="{8A3CAE25-78FA-AC45-B741-FC9B0207A6D2}" name="LiveTo" dataDxfId="209"/>
-    <tableColumn id="3" xr3:uid="{E48B42B4-FF8F-E247-B69B-452FB019B56A}" name="ID" dataDxfId="208"/>
-    <tableColumn id="4" xr3:uid="{10CD4350-B2F2-C548-B931-D6CE2C4B3E79}" name="CaseEventID" dataDxfId="207"/>
-    <tableColumn id="5" xr3:uid="{E3E6155A-EA92-DF46-8888-ED7D749B974B}" name="CaseFieldId" dataDxfId="206"/>
-    <tableColumn id="6" xr3:uid="{09371456-1EA3-1E4E-A5BB-2B5AA70A6515}" name="ListElementCode" dataDxfId="205"/>
-    <tableColumn id="7" xr3:uid="{4BB7C15A-9707-A84E-B400-8458D3F72D15}" name="EventElementLabel" dataDxfId="204"/>
-    <tableColumn id="8" xr3:uid="{CFDCFEAC-052F-4E4F-97AB-3DD41D189409}" name="EventHintText" dataDxfId="203"/>
-    <tableColumn id="9" xr3:uid="{27B7471F-FF90-7A47-8A9D-E9D960A6E136}" name="FieldDisplayOrder" dataDxfId="202"/>
-    <tableColumn id="10" xr3:uid="{E2F9B116-7625-3446-AC24-38AEC7DDE066}" name="DisplayContext" dataDxfId="201"/>
-    <tableColumn id="11" xr3:uid="{33B43FDA-A050-7949-85A2-D71C872415D1}" name="FieldShowCondition" dataDxfId="200"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{3217A593-E48A-BB42-A2D0-9D3131CA3F9C}" name="Table23" displayName="Table23" ref="A3:L42" totalsRowShown="0" headerRowDxfId="216" dataDxfId="214" headerRowBorderDxfId="215" tableBorderDxfId="213" totalsRowBorderDxfId="212">
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{CDA5C744-4A48-0C44-9DDE-72388C860C99}" name="LiveFrom" dataDxfId="211"/>
+    <tableColumn id="2" xr3:uid="{8A3CAE25-78FA-AC45-B741-FC9B0207A6D2}" name="LiveTo" dataDxfId="210"/>
+    <tableColumn id="3" xr3:uid="{E48B42B4-FF8F-E247-B69B-452FB019B56A}" name="ID" dataDxfId="209"/>
+    <tableColumn id="4" xr3:uid="{10CD4350-B2F2-C548-B931-D6CE2C4B3E79}" name="CaseEventID" dataDxfId="208"/>
+    <tableColumn id="5" xr3:uid="{E3E6155A-EA92-DF46-8888-ED7D749B974B}" name="CaseFieldId" dataDxfId="207"/>
+    <tableColumn id="6" xr3:uid="{09371456-1EA3-1E4E-A5BB-2B5AA70A6515}" name="ListElementCode" dataDxfId="206"/>
+    <tableColumn id="12" xr3:uid="{14BDAF75-550C-3348-BAC9-ECF479753E61}" name="DefaultValue" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{4BB7C15A-9707-A84E-B400-8458D3F72D15}" name="EventElementLabel" dataDxfId="205"/>
+    <tableColumn id="8" xr3:uid="{CFDCFEAC-052F-4E4F-97AB-3DD41D189409}" name="EventHintText" dataDxfId="204"/>
+    <tableColumn id="9" xr3:uid="{27B7471F-FF90-7A47-8A9D-E9D960A6E136}" name="FieldDisplayOrder" dataDxfId="203"/>
+    <tableColumn id="10" xr3:uid="{E2F9B116-7625-3446-AC24-38AEC7DDE066}" name="DisplayContext" dataDxfId="202"/>
+    <tableColumn id="11" xr3:uid="{33B43FDA-A050-7949-85A2-D71C872415D1}" name="FieldShowCondition" dataDxfId="201"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{261F291B-49E9-7A47-AB56-BF364E30DB6B}" name="Table7" displayName="Table7" ref="A3:G24" totalsRowShown="0" headerRowDxfId="199" dataDxfId="197" headerRowBorderDxfId="198" tableBorderDxfId="196" totalsRowBorderDxfId="195">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{261F291B-49E9-7A47-AB56-BF364E30DB6B}" name="Table7" displayName="Table7" ref="A3:G24" totalsRowShown="0" headerRowDxfId="200" dataDxfId="198" headerRowBorderDxfId="199" tableBorderDxfId="197" totalsRowBorderDxfId="196">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{0FE98DA5-8D77-8146-ABB3-BB35B0A6C8A0}" name="LiveFrom" dataDxfId="194"/>
-    <tableColumn id="2" xr3:uid="{40479094-15A4-7F47-89AA-CC3E78D030E7}" name="LiveTo" dataDxfId="193"/>
-    <tableColumn id="3" xr3:uid="{FC1F3A20-DA92-A542-8712-9F23DC888392}" name="ID" dataDxfId="192"/>
-    <tableColumn id="4" xr3:uid="{88A6995E-37E7-2D43-A83A-FB28F631182B}" name="ListElementCode" dataDxfId="191"/>
-    <tableColumn id="5" xr3:uid="{70D3C9B9-96C2-F543-AAC5-6A771FC842FB}" name="ListElement" dataDxfId="190"/>
-    <tableColumn id="8" xr3:uid="{59643B70-8EC4-EA40-A49D-8B57B783888C}" name="CategoryID" dataDxfId="189"/>
-    <tableColumn id="6" xr3:uid="{60021BAA-94DF-114C-B62A-D5D7CFD8AC66}" name="DisplayOrder" dataDxfId="188"/>
+    <tableColumn id="1" xr3:uid="{0FE98DA5-8D77-8146-ABB3-BB35B0A6C8A0}" name="LiveFrom" dataDxfId="195"/>
+    <tableColumn id="2" xr3:uid="{40479094-15A4-7F47-89AA-CC3E78D030E7}" name="LiveTo" dataDxfId="194"/>
+    <tableColumn id="3" xr3:uid="{FC1F3A20-DA92-A542-8712-9F23DC888392}" name="ID" dataDxfId="193"/>
+    <tableColumn id="4" xr3:uid="{88A6995E-37E7-2D43-A83A-FB28F631182B}" name="ListElementCode" dataDxfId="192"/>
+    <tableColumn id="5" xr3:uid="{70D3C9B9-96C2-F543-AAC5-6A771FC842FB}" name="ListElement" dataDxfId="191"/>
+    <tableColumn id="8" xr3:uid="{59643B70-8EC4-EA40-A49D-8B57B783888C}" name="CategoryID" dataDxfId="190"/>
+    <tableColumn id="6" xr3:uid="{60021BAA-94DF-114C-B62A-D5D7CFD8AC66}" name="DisplayOrder" dataDxfId="189"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B2671E45-89F4-0848-8638-A186A962D516}" name="Table8" displayName="Table8" ref="A3:L65" totalsRowShown="0" headerRowDxfId="187" dataDxfId="185" headerRowBorderDxfId="186" tableBorderDxfId="184" totalsRowBorderDxfId="183">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B2671E45-89F4-0848-8638-A186A962D516}" name="Table8" displayName="Table8" ref="A3:L65" totalsRowShown="0" headerRowDxfId="188" dataDxfId="186" headerRowBorderDxfId="187" tableBorderDxfId="185" totalsRowBorderDxfId="184">
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{0A3DAEEE-2CC5-0044-A886-149AE812BFAA}" name="LiveFrom" dataDxfId="182"/>
-    <tableColumn id="2" xr3:uid="{0034116A-2F06-744E-96DE-13C53D21D193}" name="LiveTo" dataDxfId="181"/>
-    <tableColumn id="3" xr3:uid="{4E6FF688-3BC6-B34A-92F8-7285F5956CC6}" name="CaseTypeID" dataDxfId="180"/>
-    <tableColumn id="4" xr3:uid="{09102647-DA84-5E49-88D5-212E4C82F684}" name="Channel" dataDxfId="179"/>
-    <tableColumn id="5" xr3:uid="{5162BADF-56AB-0642-B0E0-D4BFAB4F3A56}" name="TabID" dataDxfId="178"/>
-    <tableColumn id="6" xr3:uid="{0BF66D3F-8E5E-FD48-ADD9-C749E508C46F}" name="TabLabel" dataDxfId="177"/>
-    <tableColumn id="7" xr3:uid="{69F4B009-8625-BC4D-9C35-6ADA6C44F63C}" name="TabDisplayOrder" dataDxfId="176"/>
-    <tableColumn id="8" xr3:uid="{F3B4D28F-14B6-0B4F-B9D7-E418EC66FF7D}" name="CaseFieldID" dataDxfId="175"/>
-    <tableColumn id="9" xr3:uid="{D7540CEE-0139-244D-B0F6-61FB3BAFAB2E}" name="TabFieldDisplayOrder" dataDxfId="174"/>
-    <tableColumn id="10" xr3:uid="{F03848C6-8BF9-C045-BE97-D5A5B7B6AF7E}" name="FieldShowCondition" dataDxfId="173"/>
-    <tableColumn id="11" xr3:uid="{351643CD-F5C2-594D-B984-2BD6A557A2A6}" name="TabShowCondition" dataDxfId="172"/>
-    <tableColumn id="12" xr3:uid="{E5813993-7410-BE44-87B6-E432B935A456}" name="DisplayContextParameter" dataDxfId="171"/>
+    <tableColumn id="1" xr3:uid="{0A3DAEEE-2CC5-0044-A886-149AE812BFAA}" name="LiveFrom" dataDxfId="183"/>
+    <tableColumn id="2" xr3:uid="{0034116A-2F06-744E-96DE-13C53D21D193}" name="LiveTo" dataDxfId="182"/>
+    <tableColumn id="3" xr3:uid="{4E6FF688-3BC6-B34A-92F8-7285F5956CC6}" name="CaseTypeID" dataDxfId="181"/>
+    <tableColumn id="4" xr3:uid="{09102647-DA84-5E49-88D5-212E4C82F684}" name="Channel" dataDxfId="180"/>
+    <tableColumn id="5" xr3:uid="{5162BADF-56AB-0642-B0E0-D4BFAB4F3A56}" name="TabID" dataDxfId="179"/>
+    <tableColumn id="6" xr3:uid="{0BF66D3F-8E5E-FD48-ADD9-C749E508C46F}" name="TabLabel" dataDxfId="178"/>
+    <tableColumn id="7" xr3:uid="{69F4B009-8625-BC4D-9C35-6ADA6C44F63C}" name="TabDisplayOrder" dataDxfId="177"/>
+    <tableColumn id="8" xr3:uid="{F3B4D28F-14B6-0B4F-B9D7-E418EC66FF7D}" name="CaseFieldID" dataDxfId="176"/>
+    <tableColumn id="9" xr3:uid="{D7540CEE-0139-244D-B0F6-61FB3BAFAB2E}" name="TabFieldDisplayOrder" dataDxfId="175"/>
+    <tableColumn id="10" xr3:uid="{F03848C6-8BF9-C045-BE97-D5A5B7B6AF7E}" name="FieldShowCondition" dataDxfId="174"/>
+    <tableColumn id="11" xr3:uid="{351643CD-F5C2-594D-B984-2BD6A557A2A6}" name="TabShowCondition" dataDxfId="173"/>
+    <tableColumn id="12" xr3:uid="{E5813993-7410-BE44-87B6-E432B935A456}" name="DisplayContextParameter" dataDxfId="172"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -17636,7 +17681,7 @@
   <dimension ref="A1:Q162"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A17" zoomScale="88" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33:D33"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -24788,7 +24833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
@@ -26666,7 +26711,7 @@
   <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -30702,10 +30747,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -30809,6 +30854,34 @@
       </c>
       <c r="D7" s="224" t="s">
         <v>703</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8" s="220" t="s">
+        <v>924</v>
+      </c>
+      <c r="B8" s="219" t="s">
+        <v>687</v>
+      </c>
+      <c r="C8" s="156" t="s">
+        <v>693</v>
+      </c>
+      <c r="D8" s="187" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" s="221" t="s">
+        <v>924</v>
+      </c>
+      <c r="B9" s="222" t="s">
+        <v>695</v>
+      </c>
+      <c r="C9" s="223" t="s">
+        <v>696</v>
+      </c>
+      <c r="D9" s="224" t="s">
+        <v>697</v>
       </c>
     </row>
   </sheetData>
@@ -42128,10 +42201,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="C3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -42142,15 +42215,16 @@
     <col min="4" max="4" width="23.5" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" customWidth="1"/>
     <col min="6" max="6" width="57.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" customWidth="1"/>
-    <col min="11" max="11" width="88.5" customWidth="1"/>
-    <col min="12" max="16384" width="11.5" style="19"/>
+    <col min="7" max="7" width="57.6640625" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="88.5" customWidth="1"/>
+    <col min="13" max="16384" width="11.5" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.15">
       <c r="A1" s="242" t="s">
         <v>355</v>
       </c>
@@ -42167,19 +42241,20 @@
       <c r="F1" s="245" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="243" t="s">
+      <c r="G1" s="245"/>
+      <c r="H1" s="243" t="s">
         <v>356</v>
       </c>
-      <c r="H1" s="243" t="s">
+      <c r="I1" s="243" t="s">
         <v>357</v>
       </c>
-      <c r="I1" s="243" t="s">
+      <c r="J1" s="243" t="s">
         <v>358</v>
       </c>
-      <c r="J1" s="95"/>
-      <c r="K1" s="243"/>
-    </row>
-    <row r="2" spans="1:11" ht="122" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K1" s="95"/>
+      <c r="L1" s="243"/>
+    </row>
+    <row r="2" spans="1:12" ht="122" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="246"/>
       <c r="B2" s="246"/>
       <c r="C2" s="247" t="s">
@@ -42194,23 +42269,24 @@
       <c r="F2" s="246" t="s">
         <v>359</v>
       </c>
-      <c r="G2" s="246" t="s">
+      <c r="G2" s="246"/>
+      <c r="H2" s="246" t="s">
         <v>362</v>
       </c>
-      <c r="H2" s="246" t="s">
+      <c r="I2" s="246" t="s">
         <v>363</v>
       </c>
-      <c r="I2" s="248" t="s">
+      <c r="J2" s="248" t="s">
         <v>364</v>
       </c>
-      <c r="J2" s="248" t="s">
+      <c r="K2" s="248" t="s">
         <v>365</v>
       </c>
-      <c r="K2" s="249" t="s">
+      <c r="L2" s="249" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="254" t="s">
         <v>9</v>
       </c>
@@ -42230,22 +42306,25 @@
         <v>225</v>
       </c>
       <c r="G3" s="255" t="s">
+        <v>936</v>
+      </c>
+      <c r="H3" s="255" t="s">
         <v>369</v>
       </c>
-      <c r="H3" s="255" t="s">
+      <c r="I3" s="255" t="s">
         <v>370</v>
       </c>
-      <c r="I3" s="255" t="s">
+      <c r="J3" s="255" t="s">
         <v>371</v>
       </c>
-      <c r="J3" s="255" t="s">
+      <c r="K3" s="255" t="s">
         <v>372</v>
       </c>
-      <c r="K3" s="256" t="s">
+      <c r="L3" s="256" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="250">
         <v>43101</v>
       </c>
@@ -42262,17 +42341,18 @@
       <c r="F4" s="132" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="95"/>
+      <c r="G4" s="132"/>
       <c r="H4" s="95"/>
-      <c r="I4" s="95">
+      <c r="I4" s="95"/>
+      <c r="J4" s="95">
         <v>1</v>
       </c>
-      <c r="J4" s="132" t="s">
+      <c r="K4" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K4" s="78"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L4" s="78"/>
+    </row>
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="250">
         <v>43101</v>
       </c>
@@ -42289,17 +42369,18 @@
       <c r="F5" s="132" t="s">
         <v>311</v>
       </c>
-      <c r="G5" s="95"/>
+      <c r="G5" s="132"/>
       <c r="H5" s="95"/>
-      <c r="I5" s="95">
+      <c r="I5" s="95"/>
+      <c r="J5" s="95">
         <v>2</v>
       </c>
-      <c r="J5" s="132" t="s">
+      <c r="K5" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K5" s="78"/>
-    </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L5" s="78"/>
+    </row>
+    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="250">
         <v>43101</v>
       </c>
@@ -42316,17 +42397,18 @@
       <c r="F6" s="81" t="s">
         <v>315</v>
       </c>
-      <c r="G6" s="95"/>
+      <c r="G6" s="81"/>
       <c r="H6" s="95"/>
-      <c r="I6" s="95">
+      <c r="I6" s="95"/>
+      <c r="J6" s="95">
         <v>3</v>
       </c>
-      <c r="J6" s="132" t="s">
+      <c r="K6" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K6" s="78"/>
-    </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L6" s="78"/>
+    </row>
+    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="250">
         <v>43101</v>
       </c>
@@ -42343,17 +42425,18 @@
       <c r="F7" s="132" t="s">
         <v>341</v>
       </c>
-      <c r="G7" s="95"/>
+      <c r="G7" s="132"/>
       <c r="H7" s="95"/>
-      <c r="I7" s="95">
+      <c r="I7" s="95"/>
+      <c r="J7" s="95">
         <v>1</v>
       </c>
-      <c r="J7" s="132" t="s">
+      <c r="K7" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K7" s="78"/>
-    </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L7" s="78"/>
+    </row>
+    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="250">
         <v>43101</v>
       </c>
@@ -42370,17 +42453,18 @@
       <c r="F8" s="132" t="s">
         <v>344</v>
       </c>
-      <c r="G8" s="95"/>
+      <c r="G8" s="132"/>
       <c r="H8" s="95"/>
-      <c r="I8" s="95">
+      <c r="I8" s="95"/>
+      <c r="J8" s="95">
         <v>2</v>
       </c>
-      <c r="J8" s="132" t="s">
+      <c r="K8" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K8" s="78"/>
-    </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L8" s="78"/>
+    </row>
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="250">
         <v>43101</v>
       </c>
@@ -42399,15 +42483,16 @@
       </c>
       <c r="G9" s="95"/>
       <c r="H9" s="95"/>
-      <c r="I9" s="95">
+      <c r="I9" s="95"/>
+      <c r="J9" s="95">
         <v>2</v>
       </c>
-      <c r="J9" s="132" t="s">
+      <c r="K9" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K9" s="78"/>
-    </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L9" s="78"/>
+    </row>
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="250">
         <v>43101</v>
       </c>
@@ -42426,15 +42511,16 @@
       </c>
       <c r="G10" s="95"/>
       <c r="H10" s="95"/>
-      <c r="I10" s="95">
+      <c r="I10" s="95"/>
+      <c r="J10" s="95">
         <v>3</v>
       </c>
-      <c r="J10" s="132" t="s">
+      <c r="K10" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K10" s="78"/>
-    </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L10" s="78"/>
+    </row>
+    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="251">
         <v>43101</v>
       </c>
@@ -42453,15 +42539,16 @@
       </c>
       <c r="G11" s="98"/>
       <c r="H11" s="98"/>
-      <c r="I11" s="98">
+      <c r="I11" s="98"/>
+      <c r="J11" s="98">
         <v>5</v>
       </c>
-      <c r="J11" s="98" t="s">
+      <c r="K11" s="98" t="s">
         <v>375</v>
       </c>
-      <c r="K11" s="77"/>
-    </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L11" s="77"/>
+    </row>
+    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="251">
         <v>43101</v>
       </c>
@@ -42480,15 +42567,16 @@
       </c>
       <c r="G12" s="98"/>
       <c r="H12" s="98"/>
-      <c r="I12" s="98">
+      <c r="I12" s="98"/>
+      <c r="J12" s="98">
         <v>6</v>
       </c>
-      <c r="J12" s="132" t="s">
+      <c r="K12" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K12" s="77"/>
-    </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L12" s="77"/>
+    </row>
+    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="250">
         <v>43101</v>
       </c>
@@ -42505,17 +42593,18 @@
       <c r="F13" s="132" t="s">
         <v>342</v>
       </c>
-      <c r="G13" s="95"/>
+      <c r="G13" s="132"/>
       <c r="H13" s="95"/>
       <c r="I13" s="95"/>
-      <c r="J13" s="132" t="s">
+      <c r="J13" s="95"/>
+      <c r="K13" s="132" t="s">
         <v>375</v>
       </c>
-      <c r="K13" s="231" t="s">
+      <c r="L13" s="231" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="250">
         <v>43101</v>
       </c>
@@ -42532,19 +42621,20 @@
       <c r="F14" s="132" t="s">
         <v>377</v>
       </c>
-      <c r="G14" s="95"/>
+      <c r="G14" s="132"/>
       <c r="H14" s="95"/>
-      <c r="I14" s="95">
+      <c r="I14" s="95"/>
+      <c r="J14" s="95">
         <v>7</v>
       </c>
-      <c r="J14" s="132" t="s">
+      <c r="K14" s="132" t="s">
         <v>375</v>
       </c>
-      <c r="K14" s="231" t="s">
+      <c r="L14" s="231" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="250">
         <v>43101</v>
       </c>
@@ -42561,21 +42651,22 @@
       <c r="F15" s="132" t="s">
         <v>379</v>
       </c>
-      <c r="G15" s="132" t="s">
+      <c r="G15" s="132"/>
+      <c r="H15" s="132" t="s">
         <v>380</v>
       </c>
-      <c r="H15" s="132" t="s">
+      <c r="I15" s="132" t="s">
         <v>381</v>
       </c>
-      <c r="I15" s="95">
+      <c r="J15" s="95">
         <v>4</v>
       </c>
-      <c r="J15" s="132" t="s">
+      <c r="K15" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K15" s="231"/>
-    </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L15" s="231"/>
+    </row>
+    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="250">
         <v>43101</v>
       </c>
@@ -42592,17 +42683,18 @@
       <c r="F16" s="132" t="s">
         <v>382</v>
       </c>
-      <c r="G16" s="95"/>
+      <c r="G16" s="132"/>
       <c r="H16" s="95"/>
-      <c r="I16" s="95">
+      <c r="I16" s="95"/>
+      <c r="J16" s="95">
         <v>6</v>
       </c>
-      <c r="J16" s="132" t="s">
+      <c r="K16" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K16" s="78"/>
-    </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L16" s="78"/>
+    </row>
+    <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="250">
         <v>43101</v>
       </c>
@@ -42619,17 +42711,18 @@
       <c r="F17" s="132" t="s">
         <v>772</v>
       </c>
-      <c r="G17" s="95"/>
+      <c r="G17" s="132"/>
       <c r="H17" s="95"/>
-      <c r="I17" s="95">
+      <c r="I17" s="95"/>
+      <c r="J17" s="95">
         <v>6</v>
       </c>
-      <c r="J17" s="132" t="s">
+      <c r="K17" s="132" t="s">
         <v>375</v>
       </c>
-      <c r="K17" s="78"/>
-    </row>
-    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L17" s="78"/>
+    </row>
+    <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="250">
         <v>43101</v>
       </c>
@@ -42646,17 +42739,18 @@
       <c r="F18" s="132" t="s">
         <v>383</v>
       </c>
-      <c r="G18" s="95"/>
+      <c r="G18" s="132"/>
       <c r="H18" s="95"/>
-      <c r="I18" s="95">
+      <c r="I18" s="95"/>
+      <c r="J18" s="95">
         <v>5</v>
       </c>
-      <c r="J18" s="132" t="s">
+      <c r="K18" s="132" t="s">
         <v>375</v>
       </c>
-      <c r="K18" s="78"/>
-    </row>
-    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L18" s="78"/>
+    </row>
+    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="250">
         <v>43101</v>
       </c>
@@ -42673,19 +42767,20 @@
       <c r="F19" s="132" t="s">
         <v>384</v>
       </c>
-      <c r="G19" s="95"/>
+      <c r="G19" s="132"/>
       <c r="H19" s="95"/>
-      <c r="I19" s="95">
+      <c r="I19" s="95"/>
+      <c r="J19" s="95">
         <v>8</v>
       </c>
-      <c r="J19" s="132" t="s">
+      <c r="K19" s="132" t="s">
         <v>375</v>
       </c>
-      <c r="K19" s="231" t="s">
+      <c r="L19" s="231" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="250">
         <v>43101</v>
       </c>
@@ -42702,17 +42797,18 @@
       <c r="F20" s="132" t="s">
         <v>386</v>
       </c>
-      <c r="G20" s="95"/>
+      <c r="G20" s="132"/>
       <c r="H20" s="95"/>
       <c r="I20" s="95"/>
-      <c r="J20" s="132" t="s">
+      <c r="J20" s="95"/>
+      <c r="K20" s="132" t="s">
         <v>375</v>
       </c>
-      <c r="K20" s="231" t="s">
+      <c r="L20" s="231" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="344">
         <v>43101</v>
       </c>
@@ -42729,19 +42825,20 @@
       <c r="F21" s="357" t="s">
         <v>919</v>
       </c>
-      <c r="G21" s="345" t="s">
+      <c r="G21" s="357"/>
+      <c r="H21" s="345" t="s">
         <v>920</v>
       </c>
-      <c r="H21" s="345"/>
-      <c r="I21" s="345">
+      <c r="I21" s="345"/>
+      <c r="J21" s="345">
         <v>1</v>
       </c>
-      <c r="J21" s="357" t="s">
+      <c r="K21" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K21" s="358"/>
-    </row>
-    <row r="22" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L21" s="358"/>
+    </row>
+    <row r="22" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="344">
         <v>43101</v>
       </c>
@@ -42758,19 +42855,20 @@
       <c r="F22" s="357" t="s">
         <v>921</v>
       </c>
-      <c r="G22" s="357" t="s">
+      <c r="G22" s="357"/>
+      <c r="H22" s="357" t="s">
         <v>922</v>
       </c>
-      <c r="H22" s="345"/>
-      <c r="I22" s="345">
+      <c r="I22" s="345"/>
+      <c r="J22" s="345">
         <v>2</v>
       </c>
-      <c r="J22" s="357" t="s">
+      <c r="K22" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K22" s="358"/>
-    </row>
-    <row r="23" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L22" s="358"/>
+    </row>
+    <row r="23" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="344">
         <v>43101</v>
       </c>
@@ -42787,17 +42885,18 @@
       <c r="F23" s="357" t="s">
         <v>917</v>
       </c>
-      <c r="G23" s="345"/>
+      <c r="G23" s="357"/>
       <c r="H23" s="345"/>
-      <c r="I23" s="345">
+      <c r="I23" s="345"/>
+      <c r="J23" s="345">
         <v>3</v>
       </c>
-      <c r="J23" s="357" t="s">
+      <c r="K23" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K23" s="358"/>
-    </row>
-    <row r="24" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L23" s="358"/>
+    </row>
+    <row r="24" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="344">
         <v>43101</v>
       </c>
@@ -42814,17 +42913,18 @@
       <c r="F24" s="357" t="s">
         <v>918</v>
       </c>
-      <c r="G24" s="345"/>
+      <c r="G24" s="357"/>
       <c r="H24" s="345"/>
-      <c r="I24" s="345">
+      <c r="I24" s="345"/>
+      <c r="J24" s="345">
         <v>4</v>
       </c>
-      <c r="J24" s="357" t="s">
+      <c r="K24" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K24" s="358"/>
-    </row>
-    <row r="25" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L24" s="358"/>
+    </row>
+    <row r="25" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="344">
         <v>43101</v>
       </c>
@@ -42841,17 +42941,20 @@
       <c r="F25" s="357" t="s">
         <v>915</v>
       </c>
-      <c r="G25" s="345"/>
+      <c r="G25" s="357" t="s">
+        <v>687</v>
+      </c>
       <c r="H25" s="345"/>
-      <c r="I25" s="345">
+      <c r="I25" s="345"/>
+      <c r="J25" s="345">
         <v>5</v>
       </c>
-      <c r="J25" s="357" t="s">
+      <c r="K25" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K25" s="358"/>
-    </row>
-    <row r="26" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L25" s="358"/>
+    </row>
+    <row r="26" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="344">
         <v>43101</v>
       </c>
@@ -42868,17 +42971,18 @@
       <c r="F26" s="357" t="s">
         <v>916</v>
       </c>
-      <c r="G26" s="345"/>
+      <c r="G26" s="357"/>
       <c r="H26" s="345"/>
-      <c r="I26" s="345">
+      <c r="I26" s="345"/>
+      <c r="J26" s="345">
         <v>6</v>
       </c>
-      <c r="J26" s="357" t="s">
+      <c r="K26" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K26" s="358"/>
-    </row>
-    <row r="27" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L26" s="358"/>
+    </row>
+    <row r="27" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="344">
         <v>43101</v>
       </c>
@@ -42895,17 +42999,18 @@
       <c r="F27" s="357" t="s">
         <v>919</v>
       </c>
-      <c r="G27" s="345"/>
+      <c r="G27" s="357"/>
       <c r="H27" s="345"/>
-      <c r="I27" s="345">
+      <c r="I27" s="345"/>
+      <c r="J27" s="345">
         <v>1</v>
       </c>
-      <c r="J27" s="357" t="s">
+      <c r="K27" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K27" s="358"/>
-    </row>
-    <row r="28" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L27" s="358"/>
+    </row>
+    <row r="28" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="344">
         <v>43101</v>
       </c>
@@ -42923,16 +43028,17 @@
         <v>921</v>
       </c>
       <c r="G28" s="357"/>
-      <c r="H28" s="345"/>
-      <c r="I28" s="345">
+      <c r="H28" s="357"/>
+      <c r="I28" s="345"/>
+      <c r="J28" s="345">
         <v>2</v>
       </c>
-      <c r="J28" s="357" t="s">
+      <c r="K28" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K28" s="358"/>
-    </row>
-    <row r="29" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L28" s="358"/>
+    </row>
+    <row r="29" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="344">
         <v>43101</v>
       </c>
@@ -42949,17 +43055,18 @@
       <c r="F29" s="357" t="s">
         <v>917</v>
       </c>
-      <c r="G29" s="345"/>
+      <c r="G29" s="357"/>
       <c r="H29" s="345"/>
-      <c r="I29" s="345">
+      <c r="I29" s="345"/>
+      <c r="J29" s="345">
         <v>3</v>
       </c>
-      <c r="J29" s="357" t="s">
+      <c r="K29" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K29" s="358"/>
-    </row>
-    <row r="30" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L29" s="358"/>
+    </row>
+    <row r="30" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="344">
         <v>43101</v>
       </c>
@@ -42976,17 +43083,18 @@
       <c r="F30" s="357" t="s">
         <v>918</v>
       </c>
-      <c r="G30" s="345"/>
+      <c r="G30" s="357"/>
       <c r="H30" s="345"/>
-      <c r="I30" s="345">
+      <c r="I30" s="345"/>
+      <c r="J30" s="345">
         <v>4</v>
       </c>
-      <c r="J30" s="357" t="s">
+      <c r="K30" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K30" s="358"/>
-    </row>
-    <row r="31" spans="1:11" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L30" s="358"/>
+    </row>
+    <row r="31" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="344">
         <v>43101</v>
       </c>
@@ -43003,17 +43111,20 @@
       <c r="F31" s="357" t="s">
         <v>915</v>
       </c>
-      <c r="G31" s="345"/>
+      <c r="G31" s="357" t="s">
+        <v>695</v>
+      </c>
       <c r="H31" s="345"/>
-      <c r="I31" s="345">
+      <c r="I31" s="345"/>
+      <c r="J31" s="345">
         <v>5</v>
       </c>
-      <c r="J31" s="357" t="s">
+      <c r="K31" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K31" s="358"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L31" s="358"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A32" s="344">
         <v>43101</v>
       </c>
@@ -43030,17 +43141,18 @@
       <c r="F32" s="357" t="s">
         <v>916</v>
       </c>
-      <c r="G32" s="345"/>
+      <c r="G32" s="357"/>
       <c r="H32" s="345"/>
-      <c r="I32" s="345">
+      <c r="I32" s="345"/>
+      <c r="J32" s="345">
         <v>6</v>
       </c>
-      <c r="J32" s="357" t="s">
+      <c r="K32" s="357" t="s">
         <v>375</v>
       </c>
-      <c r="K32" s="358"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L32" s="358"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A33" s="251">
         <v>43101</v>
       </c>
@@ -43057,19 +43169,20 @@
       <c r="F33" s="132" t="s">
         <v>344</v>
       </c>
-      <c r="G33" s="98"/>
+      <c r="G33" s="132"/>
       <c r="H33" s="98"/>
-      <c r="I33" s="98">
+      <c r="I33" s="98"/>
+      <c r="J33" s="98">
         <v>1</v>
       </c>
-      <c r="J33" s="132" t="s">
+      <c r="K33" s="132" t="s">
         <v>389</v>
       </c>
-      <c r="K33" s="231" t="s">
+      <c r="L33" s="231" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A34" s="251">
         <v>43101</v>
       </c>
@@ -43086,19 +43199,20 @@
       <c r="F34" s="132" t="s">
         <v>341</v>
       </c>
-      <c r="G34" s="98"/>
+      <c r="G34" s="132"/>
       <c r="H34" s="98"/>
-      <c r="I34" s="98">
+      <c r="I34" s="98"/>
+      <c r="J34" s="98">
         <v>1</v>
       </c>
-      <c r="J34" s="132" t="s">
+      <c r="K34" s="132" t="s">
         <v>375</v>
       </c>
-      <c r="K34" s="231" t="s">
+      <c r="L34" s="231" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A35" s="251">
         <v>43101</v>
       </c>
@@ -43115,17 +43229,18 @@
       <c r="F35" s="132" t="s">
         <v>326</v>
       </c>
-      <c r="G35" s="98"/>
+      <c r="G35" s="132"/>
       <c r="H35" s="98"/>
-      <c r="I35" s="98">
+      <c r="I35" s="98"/>
+      <c r="J35" s="98">
         <v>1</v>
       </c>
-      <c r="J35" s="132" t="s">
+      <c r="K35" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K35" s="77"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L35" s="77"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A36" s="251">
         <v>43101</v>
       </c>
@@ -43142,17 +43257,18 @@
       <c r="F36" s="132" t="s">
         <v>328</v>
       </c>
-      <c r="G36" s="98"/>
+      <c r="G36" s="132"/>
       <c r="H36" s="98"/>
-      <c r="I36" s="98">
+      <c r="I36" s="98"/>
+      <c r="J36" s="98">
         <v>1</v>
       </c>
-      <c r="J36" s="132" t="s">
+      <c r="K36" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K36" s="77"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L36" s="77"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A37" s="251">
         <v>43101</v>
       </c>
@@ -43169,17 +43285,18 @@
       <c r="F37" s="132" t="s">
         <v>330</v>
       </c>
-      <c r="G37" s="98"/>
+      <c r="G37" s="132"/>
       <c r="H37" s="98"/>
-      <c r="I37" s="98">
+      <c r="I37" s="98"/>
+      <c r="J37" s="98">
         <v>2</v>
       </c>
-      <c r="J37" s="132" t="s">
+      <c r="K37" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K37" s="77"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L37" s="77"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A38" s="251">
         <v>43101</v>
       </c>
@@ -43196,17 +43313,18 @@
       <c r="F38" s="132" t="s">
         <v>326</v>
       </c>
-      <c r="G38" s="98"/>
+      <c r="G38" s="132"/>
       <c r="H38" s="98"/>
-      <c r="I38" s="98">
+      <c r="I38" s="98"/>
+      <c r="J38" s="98">
         <v>1</v>
       </c>
-      <c r="J38" s="132" t="s">
+      <c r="K38" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K38" s="77"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L38" s="77"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A39" s="251">
         <v>43101</v>
       </c>
@@ -43223,17 +43341,18 @@
       <c r="F39" s="132" t="s">
         <v>328</v>
       </c>
-      <c r="G39" s="98"/>
+      <c r="G39" s="132"/>
       <c r="H39" s="98"/>
-      <c r="I39" s="98">
+      <c r="I39" s="98"/>
+      <c r="J39" s="98">
         <v>1</v>
       </c>
-      <c r="J39" s="132" t="s">
+      <c r="K39" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K39" s="77"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L39" s="77"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A40" s="251">
         <v>43101</v>
       </c>
@@ -43250,17 +43369,18 @@
       <c r="F40" s="132" t="s">
         <v>330</v>
       </c>
-      <c r="G40" s="98"/>
+      <c r="G40" s="132"/>
       <c r="H40" s="98"/>
-      <c r="I40" s="98">
+      <c r="I40" s="98"/>
+      <c r="J40" s="98">
         <v>2</v>
       </c>
-      <c r="J40" s="132" t="s">
+      <c r="K40" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K40" s="77"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L40" s="77"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A41" s="251">
         <v>43101</v>
       </c>
@@ -43277,17 +43397,18 @@
       <c r="F41" s="132" t="s">
         <v>326</v>
       </c>
-      <c r="G41" s="98"/>
+      <c r="G41" s="132"/>
       <c r="H41" s="98"/>
-      <c r="I41" s="98">
+      <c r="I41" s="98"/>
+      <c r="J41" s="98">
         <v>1</v>
       </c>
-      <c r="J41" s="132" t="s">
+      <c r="K41" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="K41" s="77"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L41" s="77"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A42" s="252">
         <v>43101</v>
       </c>
@@ -43304,15 +43425,16 @@
       <c r="F42" s="253" t="s">
         <v>328</v>
       </c>
-      <c r="G42" s="104"/>
+      <c r="G42" s="253"/>
       <c r="H42" s="104"/>
-      <c r="I42" s="104">
+      <c r="I42" s="104"/>
+      <c r="J42" s="104">
         <v>1</v>
       </c>
-      <c r="J42" s="253" t="s">
+      <c r="K42" s="253" t="s">
         <v>374</v>
       </c>
-      <c r="K42" s="105"/>
+      <c r="L42" s="105"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Convert excel to json
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Defninition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Defninition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olawaleolanrewaju/Documents/Git_MOJ/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73DCECD-0CE0-C445-A1DC-806FD66723FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F34AEC6-5920-CA46-8860-A97E10CB69EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" firstSheet="2" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -4929,22 +4929,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -4996,22 +4980,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
@@ -5095,6 +5063,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -5102,15 +5079,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -5176,6 +5144,22 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -5227,6 +5211,22 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
@@ -12099,28 +12099,28 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F48" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D6A08A61-2CBC-2440-A55B-973E9A2BBBB2}" name="Table21" displayName="Table21" ref="A3:F48" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{EE9F57B3-787C-C642-A2B0-1CB2CD584A64}" name="CaseTypeID" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{A6633300-114A-5846-B7B7-C57244A39F58}" name="CaseEventID" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{229CDFFE-02D8-6042-9F1C-B67EA1F30C09}" name="UserRole" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{872585F6-B038-2149-8440-E4F3A404C8A9}" name="CRUD" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{47319793-AA7E-7241-AE2D-C13844517EB1}" name="LiveFrom" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{4BC3F1CC-B8A0-DD42-BBD4-5BD8DB4634CE}" name="LiveTo" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{EE9F57B3-787C-C642-A2B0-1CB2CD584A64}" name="CaseTypeID" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{A6633300-114A-5846-B7B7-C57244A39F58}" name="CaseEventID" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{229CDFFE-02D8-6042-9F1C-B67EA1F30C09}" name="UserRole" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{872585F6-B038-2149-8440-E4F3A404C8A9}" name="CRUD" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F37" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F37" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{F6F18BFB-2335-8D4F-9DC5-89FC7FD3B64B}" name="CaseTypeID" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{EB11A8E2-8EA8-0B46-B3B3-103461A3AF54}" name="CaseStateID" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{1C1D63D9-6997-9E47-9725-BB01CA7FD1F3}" name="UserRole" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{82473FFF-1C61-B242-A091-BA139462FACF}" name="CRUD" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{F6F18BFB-2335-8D4F-9DC5-89FC7FD3B64B}" name="CaseTypeID" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{EB11A8E2-8EA8-0B46-B3B3-103461A3AF54}" name="CaseStateID" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{1C1D63D9-6997-9E47-9725-BB01CA7FD1F3}" name="UserRole" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{82473FFF-1C61-B242-A091-BA139462FACF}" name="CRUD" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -26629,7 +26629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:DS39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B6" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B6" workbookViewId="0">
       <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
@@ -47379,8 +47379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Removed redundant state authorisation
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Defninition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/BEFTA_Master_Defninition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olawaleolanrewaju/Documents/Git_MOJ/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F34AEC6-5920-CA46-8860-A97E10CB69EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4962600F-71C3-BC4A-A2E9-4AE2CC81DA4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" firstSheet="14" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5827" uniqueCount="951">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5823" uniqueCount="951">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -12113,7 +12113,7 @@
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F37" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{315AA6A0-C96B-A042-AD60-5F6D63D17CA6}" name="Table22" displayName="Table22" ref="A3:F36" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{509EB312-569C-A943-92C0-18A849F5F9AF}" name="LiveFrom" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{806AAD02-2C59-5441-80DF-1037D88236E9}" name="LiveTo" dataDxfId="4"/>
@@ -34690,10 +34690,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:CF37"/>
+  <dimension ref="A1:CF36"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -34789,13 +34789,13 @@
         <v>884</v>
       </c>
       <c r="D5" s="76" t="s">
-        <v>493</v>
-      </c>
-      <c r="E5" s="148" t="s">
-        <v>778</v>
+        <v>489</v>
+      </c>
+      <c r="E5" s="76" t="s">
+        <v>698</v>
       </c>
       <c r="F5" s="129" t="s">
-        <v>339</v>
+        <v>709</v>
       </c>
     </row>
     <row r="6" spans="1:84" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -34804,16 +34804,16 @@
       </c>
       <c r="B6" s="95"/>
       <c r="C6" s="76" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="D6" s="76" t="s">
         <v>489</v>
       </c>
-      <c r="E6" s="76" t="s">
-        <v>698</v>
+      <c r="E6" s="148" t="s">
+        <v>778</v>
       </c>
       <c r="F6" s="129" t="s">
-        <v>709</v>
+        <v>339</v>
       </c>
     </row>
     <row r="7" spans="1:84" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -34824,8 +34824,8 @@
       <c r="C7" s="76" t="s">
         <v>882</v>
       </c>
-      <c r="D7" s="76" t="s">
-        <v>489</v>
+      <c r="D7" s="79" t="s">
+        <v>491</v>
       </c>
       <c r="E7" s="148" t="s">
         <v>778</v>
@@ -34834,75 +34834,153 @@
         <v>339</v>
       </c>
     </row>
-    <row r="8" spans="1:84" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B8" s="95"/>
-      <c r="C8" s="76" t="s">
-        <v>882</v>
+    <row r="8" spans="1:84" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="80">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="98"/>
+      <c r="C8" s="79" t="s">
+        <v>883</v>
       </c>
       <c r="D8" s="79" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="E8" s="148" t="s">
         <v>778</v>
       </c>
-      <c r="F8" s="129" t="s">
+      <c r="F8" s="133" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="9" spans="1:84" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="80">
-        <v>42736</v>
-      </c>
-      <c r="B9" s="98"/>
+    <row r="9" spans="1:84" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B9" s="95"/>
       <c r="C9" s="79" t="s">
         <v>883</v>
       </c>
       <c r="D9" s="79" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="E9" s="148" t="s">
         <v>778</v>
       </c>
-      <c r="F9" s="133" t="s">
+      <c r="F9" s="129" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="10" spans="1:84" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B10" s="95"/>
-      <c r="C10" s="79" t="s">
-        <v>883</v>
-      </c>
-      <c r="D10" s="79" t="s">
-        <v>489</v>
-      </c>
-      <c r="E10" s="148" t="s">
+    <row r="10" spans="1:84" s="306" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="359">
+        <v>42736</v>
+      </c>
+      <c r="B10" s="352"/>
+      <c r="C10" s="307" t="s">
+        <v>924</v>
+      </c>
+      <c r="D10" s="307" t="s">
+        <v>493</v>
+      </c>
+      <c r="E10" s="385" t="s">
         <v>778</v>
       </c>
-      <c r="F10" s="129" t="s">
+      <c r="F10" s="381" t="s">
         <v>339</v>
       </c>
+      <c r="G10" s="425"/>
+      <c r="H10" s="425"/>
+      <c r="I10" s="425"/>
+      <c r="J10" s="425"/>
+      <c r="K10" s="425"/>
+      <c r="L10" s="425"/>
+      <c r="M10" s="425"/>
+      <c r="N10" s="425"/>
+      <c r="O10" s="425"/>
+      <c r="P10" s="425"/>
+      <c r="Q10" s="425"/>
+      <c r="R10" s="425"/>
+      <c r="S10" s="425"/>
+      <c r="T10" s="425"/>
+      <c r="U10" s="425"/>
+      <c r="V10" s="425"/>
+      <c r="W10" s="425"/>
+      <c r="X10" s="425"/>
+      <c r="Y10" s="425"/>
+      <c r="Z10" s="425"/>
+      <c r="AA10" s="425"/>
+      <c r="AB10" s="425"/>
+      <c r="AC10" s="425"/>
+      <c r="AD10" s="425"/>
+      <c r="AE10" s="425"/>
+      <c r="AF10" s="425"/>
+      <c r="AG10" s="425"/>
+      <c r="AH10" s="425"/>
+      <c r="AI10" s="425"/>
+      <c r="AJ10" s="425"/>
+      <c r="AK10" s="425"/>
+      <c r="AL10" s="425"/>
+      <c r="AM10" s="425"/>
+      <c r="AN10" s="425"/>
+      <c r="AO10" s="425"/>
+      <c r="AP10" s="425"/>
+      <c r="AQ10" s="425"/>
+      <c r="AR10" s="425"/>
+      <c r="AS10" s="425"/>
+      <c r="AT10" s="425"/>
+      <c r="AU10" s="425"/>
+      <c r="AV10" s="425"/>
+      <c r="AW10" s="425"/>
+      <c r="AX10" s="425"/>
+      <c r="AY10" s="425"/>
+      <c r="AZ10" s="425"/>
+      <c r="BA10" s="425"/>
+      <c r="BB10" s="425"/>
+      <c r="BC10" s="425"/>
+      <c r="BD10" s="425"/>
+      <c r="BE10" s="425"/>
+      <c r="BF10" s="425"/>
+      <c r="BG10" s="425"/>
+      <c r="BH10" s="425"/>
+      <c r="BI10" s="425"/>
+      <c r="BJ10" s="425"/>
+      <c r="BK10" s="425"/>
+      <c r="BL10" s="425"/>
+      <c r="BM10" s="425"/>
+      <c r="BN10" s="425"/>
+      <c r="BO10" s="425"/>
+      <c r="BP10" s="425"/>
+      <c r="BQ10" s="425"/>
+      <c r="BR10" s="425"/>
+      <c r="BS10" s="425"/>
+      <c r="BT10" s="425"/>
+      <c r="BU10" s="425"/>
+      <c r="BV10" s="425"/>
+      <c r="BW10" s="425"/>
+      <c r="BX10" s="425"/>
+      <c r="BY10" s="425"/>
+      <c r="BZ10" s="425"/>
+      <c r="CA10" s="425"/>
+      <c r="CB10" s="425"/>
+      <c r="CC10" s="425"/>
+      <c r="CD10" s="425"/>
+      <c r="CE10" s="425"/>
+      <c r="CF10" s="425"/>
     </row>
     <row r="11" spans="1:84" s="306" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="359">
-        <v>42736</v>
-      </c>
-      <c r="B11" s="352"/>
+      <c r="A11" s="300">
+        <v>42736</v>
+      </c>
+      <c r="B11" s="303"/>
       <c r="C11" s="307" t="s">
         <v>924</v>
       </c>
       <c r="D11" s="307" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="E11" s="385" t="s">
         <v>778</v>
       </c>
-      <c r="F11" s="381" t="s">
+      <c r="F11" s="308" t="s">
         <v>339</v>
       </c>
       <c r="G11" s="425"/>
@@ -34985,20 +35063,20 @@
       <c r="CF11" s="425"/>
     </row>
     <row r="12" spans="1:84" s="306" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="300">
-        <v>42736</v>
-      </c>
-      <c r="B12" s="303"/>
-      <c r="C12" s="307" t="s">
-        <v>924</v>
-      </c>
-      <c r="D12" s="307" t="s">
+      <c r="A12" s="419">
+        <v>42736</v>
+      </c>
+      <c r="B12" s="422"/>
+      <c r="C12" s="421" t="s">
+        <v>939</v>
+      </c>
+      <c r="D12" s="421" t="s">
         <v>489</v>
       </c>
-      <c r="E12" s="385" t="s">
-        <v>778</v>
-      </c>
-      <c r="F12" s="308" t="s">
+      <c r="E12" s="468" t="s">
+        <v>942</v>
+      </c>
+      <c r="F12" s="466" t="s">
         <v>339</v>
       </c>
       <c r="G12" s="425"/>
@@ -35089,7 +35167,7 @@
         <v>939</v>
       </c>
       <c r="D13" s="421" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="E13" s="468" t="s">
         <v>942</v>
@@ -35185,10 +35263,10 @@
         <v>939</v>
       </c>
       <c r="D14" s="421" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="E14" s="468" t="s">
-        <v>942</v>
+        <v>778</v>
       </c>
       <c r="F14" s="466" t="s">
         <v>339</v>
@@ -35281,7 +35359,7 @@
         <v>939</v>
       </c>
       <c r="D15" s="421" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="E15" s="468" t="s">
         <v>778</v>
@@ -35368,101 +35446,23 @@
       <c r="CE15" s="425"/>
       <c r="CF15" s="425"/>
     </row>
-    <row r="16" spans="1:84" s="306" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="419">
-        <v>42736</v>
-      </c>
-      <c r="B16" s="422"/>
-      <c r="C16" s="421" t="s">
-        <v>939</v>
-      </c>
-      <c r="D16" s="421" t="s">
-        <v>493</v>
-      </c>
-      <c r="E16" s="468" t="s">
+    <row r="16" spans="1:84" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B16" s="95"/>
+      <c r="C16" s="79" t="s">
+        <v>885</v>
+      </c>
+      <c r="D16" s="76" t="s">
+        <v>489</v>
+      </c>
+      <c r="E16" s="148" t="s">
         <v>778</v>
       </c>
-      <c r="F16" s="466" t="s">
+      <c r="F16" s="129" t="s">
         <v>339</v>
       </c>
-      <c r="G16" s="425"/>
-      <c r="H16" s="425"/>
-      <c r="I16" s="425"/>
-      <c r="J16" s="425"/>
-      <c r="K16" s="425"/>
-      <c r="L16" s="425"/>
-      <c r="M16" s="425"/>
-      <c r="N16" s="425"/>
-      <c r="O16" s="425"/>
-      <c r="P16" s="425"/>
-      <c r="Q16" s="425"/>
-      <c r="R16" s="425"/>
-      <c r="S16" s="425"/>
-      <c r="T16" s="425"/>
-      <c r="U16" s="425"/>
-      <c r="V16" s="425"/>
-      <c r="W16" s="425"/>
-      <c r="X16" s="425"/>
-      <c r="Y16" s="425"/>
-      <c r="Z16" s="425"/>
-      <c r="AA16" s="425"/>
-      <c r="AB16" s="425"/>
-      <c r="AC16" s="425"/>
-      <c r="AD16" s="425"/>
-      <c r="AE16" s="425"/>
-      <c r="AF16" s="425"/>
-      <c r="AG16" s="425"/>
-      <c r="AH16" s="425"/>
-      <c r="AI16" s="425"/>
-      <c r="AJ16" s="425"/>
-      <c r="AK16" s="425"/>
-      <c r="AL16" s="425"/>
-      <c r="AM16" s="425"/>
-      <c r="AN16" s="425"/>
-      <c r="AO16" s="425"/>
-      <c r="AP16" s="425"/>
-      <c r="AQ16" s="425"/>
-      <c r="AR16" s="425"/>
-      <c r="AS16" s="425"/>
-      <c r="AT16" s="425"/>
-      <c r="AU16" s="425"/>
-      <c r="AV16" s="425"/>
-      <c r="AW16" s="425"/>
-      <c r="AX16" s="425"/>
-      <c r="AY16" s="425"/>
-      <c r="AZ16" s="425"/>
-      <c r="BA16" s="425"/>
-      <c r="BB16" s="425"/>
-      <c r="BC16" s="425"/>
-      <c r="BD16" s="425"/>
-      <c r="BE16" s="425"/>
-      <c r="BF16" s="425"/>
-      <c r="BG16" s="425"/>
-      <c r="BH16" s="425"/>
-      <c r="BI16" s="425"/>
-      <c r="BJ16" s="425"/>
-      <c r="BK16" s="425"/>
-      <c r="BL16" s="425"/>
-      <c r="BM16" s="425"/>
-      <c r="BN16" s="425"/>
-      <c r="BO16" s="425"/>
-      <c r="BP16" s="425"/>
-      <c r="BQ16" s="425"/>
-      <c r="BR16" s="425"/>
-      <c r="BS16" s="425"/>
-      <c r="BT16" s="425"/>
-      <c r="BU16" s="425"/>
-      <c r="BV16" s="425"/>
-      <c r="BW16" s="425"/>
-      <c r="BX16" s="425"/>
-      <c r="BY16" s="425"/>
-      <c r="BZ16" s="425"/>
-      <c r="CA16" s="425"/>
-      <c r="CB16" s="425"/>
-      <c r="CC16" s="425"/>
-      <c r="CD16" s="425"/>
-      <c r="CE16" s="425"/>
-      <c r="CF16" s="425"/>
     </row>
     <row r="17" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="74">
@@ -35470,9 +35470,9 @@
       </c>
       <c r="B17" s="95"/>
       <c r="C17" s="79" t="s">
-        <v>885</v>
-      </c>
-      <c r="D17" s="76" t="s">
+        <v>886</v>
+      </c>
+      <c r="D17" s="96" t="s">
         <v>489</v>
       </c>
       <c r="E17" s="148" t="s">
@@ -35491,7 +35491,7 @@
         <v>886</v>
       </c>
       <c r="D18" s="96" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="E18" s="148" t="s">
         <v>778</v>
@@ -35509,7 +35509,7 @@
         <v>886</v>
       </c>
       <c r="D19" s="96" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="E19" s="148" t="s">
         <v>778</v>
@@ -35518,16 +35518,16 @@
         <v>339</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="74">
         <v>42736</v>
       </c>
       <c r="B20" s="95"/>
-      <c r="C20" s="79" t="s">
-        <v>886</v>
-      </c>
-      <c r="D20" s="96" t="s">
-        <v>497</v>
+      <c r="C20" s="76" t="s">
+        <v>887</v>
+      </c>
+      <c r="D20" s="76" t="s">
+        <v>489</v>
       </c>
       <c r="E20" s="148" t="s">
         <v>778</v>
@@ -35536,13 +35536,13 @@
         <v>339</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="74">
         <v>42736</v>
       </c>
       <c r="B21" s="95"/>
       <c r="C21" s="76" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="D21" s="76" t="s">
         <v>489</v>
@@ -35554,57 +35554,57 @@
         <v>339</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B22" s="95"/>
-      <c r="C22" s="76" t="s">
+    <row r="22" spans="1:6" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="80">
+        <v>42736</v>
+      </c>
+      <c r="B22" s="98"/>
+      <c r="C22" s="82" t="s">
         <v>888</v>
       </c>
-      <c r="D22" s="76" t="s">
-        <v>489</v>
+      <c r="D22" s="82" t="s">
+        <v>498</v>
       </c>
       <c r="E22" s="148" t="s">
         <v>778</v>
       </c>
-      <c r="F22" s="129" t="s">
+      <c r="F22" s="133" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="80">
-        <v>42736</v>
-      </c>
-      <c r="B23" s="98"/>
-      <c r="C23" s="82" t="s">
-        <v>888</v>
-      </c>
-      <c r="D23" s="82" t="s">
-        <v>498</v>
+      <c r="A23" s="74">
+        <v>42736</v>
+      </c>
+      <c r="B23" s="95"/>
+      <c r="C23" s="76" t="s">
+        <v>890</v>
+      </c>
+      <c r="D23" s="76" t="s">
+        <v>489</v>
       </c>
       <c r="E23" s="148" t="s">
         <v>778</v>
       </c>
-      <c r="F23" s="133" t="s">
+      <c r="F23" s="129" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="74">
-        <v>42736</v>
-      </c>
-      <c r="B24" s="95"/>
-      <c r="C24" s="76" t="s">
-        <v>890</v>
-      </c>
-      <c r="D24" s="76" t="s">
+      <c r="A24" s="80">
+        <v>42736</v>
+      </c>
+      <c r="B24" s="98"/>
+      <c r="C24" s="98" t="s">
+        <v>889</v>
+      </c>
+      <c r="D24" s="82" t="s">
         <v>489</v>
       </c>
       <c r="E24" s="148" t="s">
         <v>778</v>
       </c>
-      <c r="F24" s="129" t="s">
+      <c r="F24" s="133" t="s">
         <v>339</v>
       </c>
     </row>
@@ -35617,7 +35617,7 @@
         <v>889</v>
       </c>
       <c r="D25" s="82" t="s">
-        <v>489</v>
+        <v>500</v>
       </c>
       <c r="E25" s="148" t="s">
         <v>778</v>
@@ -35635,7 +35635,7 @@
         <v>889</v>
       </c>
       <c r="D26" s="82" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="E26" s="148" t="s">
         <v>778</v>
@@ -35649,11 +35649,11 @@
         <v>42736</v>
       </c>
       <c r="B27" s="98"/>
-      <c r="C27" s="98" t="s">
-        <v>889</v>
+      <c r="C27" s="79" t="s">
+        <v>891</v>
       </c>
       <c r="D27" s="82" t="s">
-        <v>502</v>
+        <v>489</v>
       </c>
       <c r="E27" s="148" t="s">
         <v>778</v>
@@ -35667,14 +35667,14 @@
         <v>42736</v>
       </c>
       <c r="B28" s="98"/>
-      <c r="C28" s="79" t="s">
-        <v>891</v>
+      <c r="C28" s="82" t="s">
+        <v>894</v>
       </c>
       <c r="D28" s="82" t="s">
         <v>489</v>
       </c>
-      <c r="E28" s="148" t="s">
-        <v>778</v>
+      <c r="E28" s="98" t="s">
+        <v>779</v>
       </c>
       <c r="F28" s="133" t="s">
         <v>339</v>
@@ -35689,7 +35689,7 @@
         <v>894</v>
       </c>
       <c r="D29" s="82" t="s">
-        <v>489</v>
+        <v>505</v>
       </c>
       <c r="E29" s="98" t="s">
         <v>779</v>
@@ -35698,7 +35698,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="80">
         <v>42736</v>
       </c>
@@ -35707,10 +35707,10 @@
         <v>894</v>
       </c>
       <c r="D30" s="82" t="s">
-        <v>505</v>
+        <v>489</v>
       </c>
       <c r="E30" s="98" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="F30" s="133" t="s">
         <v>339</v>
@@ -35725,7 +35725,7 @@
         <v>894</v>
       </c>
       <c r="D31" s="82" t="s">
-        <v>489</v>
+        <v>505</v>
       </c>
       <c r="E31" s="98" t="s">
         <v>780</v>
@@ -35734,39 +35734,39 @@
         <v>339</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="80">
         <v>42736</v>
       </c>
       <c r="B32" s="98"/>
-      <c r="C32" s="82" t="s">
-        <v>894</v>
-      </c>
-      <c r="D32" s="82" t="s">
-        <v>505</v>
-      </c>
-      <c r="E32" s="98" t="s">
-        <v>780</v>
+      <c r="C32" s="79" t="s">
+        <v>892</v>
+      </c>
+      <c r="D32" s="96" t="s">
+        <v>489</v>
+      </c>
+      <c r="E32" s="148" t="s">
+        <v>778</v>
       </c>
       <c r="F32" s="133" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="80">
-        <v>42736</v>
-      </c>
-      <c r="B33" s="98"/>
-      <c r="C33" s="79" t="s">
+      <c r="A33" s="85">
+        <v>42736</v>
+      </c>
+      <c r="B33" s="104"/>
+      <c r="C33" s="87" t="s">
         <v>892</v>
       </c>
-      <c r="D33" s="96" t="s">
-        <v>489</v>
-      </c>
-      <c r="E33" s="148" t="s">
+      <c r="D33" s="102" t="s">
+        <v>729</v>
+      </c>
+      <c r="E33" s="209" t="s">
         <v>778</v>
       </c>
-      <c r="F33" s="133" t="s">
+      <c r="F33" s="139" t="s">
         <v>339</v>
       </c>
     </row>
@@ -35774,12 +35774,12 @@
       <c r="A34" s="85">
         <v>42736</v>
       </c>
-      <c r="B34" s="104"/>
-      <c r="C34" s="87" t="s">
-        <v>892</v>
-      </c>
-      <c r="D34" s="102" t="s">
-        <v>729</v>
+      <c r="B34" s="83"/>
+      <c r="C34" s="310" t="s">
+        <v>893</v>
+      </c>
+      <c r="D34" s="312" t="s">
+        <v>830</v>
       </c>
       <c r="E34" s="209" t="s">
         <v>778</v>
@@ -35797,7 +35797,7 @@
         <v>893</v>
       </c>
       <c r="D35" s="312" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="E35" s="209" t="s">
         <v>778</v>
@@ -35810,35 +35810,17 @@
       <c r="A36" s="85">
         <v>42736</v>
       </c>
-      <c r="B36" s="83"/>
+      <c r="B36" s="86"/>
       <c r="C36" s="310" t="s">
         <v>893</v>
       </c>
       <c r="D36" s="312" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="E36" s="209" t="s">
         <v>778</v>
       </c>
       <c r="F36" s="139" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="85">
-        <v>42736</v>
-      </c>
-      <c r="B37" s="86"/>
-      <c r="C37" s="310" t="s">
-        <v>893</v>
-      </c>
-      <c r="D37" s="312" t="s">
-        <v>834</v>
-      </c>
-      <c r="E37" s="209" t="s">
-        <v>778</v>
-      </c>
-      <c r="F37" s="139" t="s">
         <v>339</v>
       </c>
     </row>
@@ -47379,7 +47361,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>

</xml_diff>